<commit_message>
Filtering by number of category
</commit_message>
<xml_diff>
--- a/xlsx/BMW_Sales_Standards_2016_ME.xlsx
+++ b/xlsx/BMW_Sales_Standards_2016_ME.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KAPTA Camilo\AuditoriasMedioOriente\Retail Standards 2016\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Camilo\Desktop\python\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -7988,189 +7988,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="64" fillId="18" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="64" fillId="18" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="64" fillId="18" borderId="0" xfId="4" applyAlignment="1">
       <alignment vertical="top"/>
@@ -8189,6 +8006,189 @@
     </xf>
     <xf numFmtId="0" fontId="64" fillId="18" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="18" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -9149,19 +9149,19 @@
       <c r="L20" s="539"/>
     </row>
     <row r="21" spans="1:12" ht="186.75" customHeight="1">
-      <c r="A21" s="939" t="s">
+      <c r="A21" s="946" t="s">
         <v>783</v>
       </c>
-      <c r="B21" s="939"/>
-      <c r="C21" s="939"/>
-      <c r="D21" s="939"/>
-      <c r="E21" s="939"/>
-      <c r="F21" s="939"/>
-      <c r="G21" s="939"/>
-      <c r="H21" s="939"/>
-      <c r="I21" s="939"/>
-      <c r="J21" s="939"/>
-      <c r="K21" s="939"/>
+      <c r="B21" s="946"/>
+      <c r="C21" s="946"/>
+      <c r="D21" s="946"/>
+      <c r="E21" s="946"/>
+      <c r="F21" s="946"/>
+      <c r="G21" s="946"/>
+      <c r="H21" s="946"/>
+      <c r="I21" s="946"/>
+      <c r="J21" s="946"/>
+      <c r="K21" s="946"/>
       <c r="L21" s="540"/>
     </row>
     <row r="22" spans="1:12" ht="14.4">
@@ -9259,44 +9259,44 @@
         <v>191</v>
       </c>
       <c r="F1" s="271"/>
-      <c r="G1" s="944" t="s">
+      <c r="G1" s="951" t="s">
         <v>744</v>
       </c>
-      <c r="H1" s="944"/>
-      <c r="I1" s="944"/>
-      <c r="J1" s="944"/>
-      <c r="K1" s="944"/>
-      <c r="L1" s="944"/>
+      <c r="H1" s="951"/>
+      <c r="I1" s="951"/>
+      <c r="J1" s="951"/>
+      <c r="K1" s="951"/>
+      <c r="L1" s="951"/>
       <c r="M1" s="128"/>
-      <c r="N1" s="943" t="s">
+      <c r="N1" s="950" t="s">
         <v>190</v>
       </c>
-      <c r="P1" s="943" t="s">
+      <c r="P1" s="950" t="s">
         <v>193</v>
       </c>
-      <c r="R1" s="943" t="s">
+      <c r="R1" s="950" t="s">
         <v>219</v>
       </c>
-      <c r="T1" s="943" t="s">
+      <c r="T1" s="950" t="s">
         <v>242</v>
       </c>
-      <c r="V1" s="943" t="s">
+      <c r="V1" s="950" t="s">
         <v>243</v>
       </c>
-      <c r="X1" s="943" t="s">
+      <c r="X1" s="950" t="s">
         <v>220</v>
       </c>
-      <c r="Z1" s="943" t="s">
+      <c r="Z1" s="950" t="s">
         <v>244</v>
       </c>
-      <c r="AB1" s="945" t="s">
+      <c r="AB1" s="952" t="s">
         <v>740</v>
       </c>
       <c r="AC1" s="123"/>
-      <c r="AD1" s="940" t="s">
+      <c r="AD1" s="947" t="s">
         <v>989</v>
       </c>
-      <c r="AF1" s="941" t="s">
+      <c r="AF1" s="948" t="s">
         <v>990</v>
       </c>
     </row>
@@ -9326,24 +9326,24 @@
         <v>7</v>
       </c>
       <c r="M2" s="129"/>
-      <c r="N2" s="943"/>
-      <c r="P2" s="943"/>
-      <c r="R2" s="943"/>
-      <c r="T2" s="943"/>
-      <c r="V2" s="943"/>
-      <c r="X2" s="943"/>
-      <c r="Z2" s="943"/>
-      <c r="AB2" s="945"/>
+      <c r="N2" s="950"/>
+      <c r="P2" s="950"/>
+      <c r="R2" s="950"/>
+      <c r="T2" s="950"/>
+      <c r="V2" s="950"/>
+      <c r="X2" s="950"/>
+      <c r="Z2" s="950"/>
+      <c r="AB2" s="952"/>
       <c r="AC2" s="123"/>
-      <c r="AD2" s="940"/>
-      <c r="AF2" s="941"/>
+      <c r="AD2" s="947"/>
+      <c r="AF2" s="948"/>
     </row>
     <row r="4" spans="1:32" ht="15">
-      <c r="A4" s="984" t="s">
+      <c r="A4" s="993" t="s">
         <v>96</v>
       </c>
-      <c r="B4" s="984"/>
-      <c r="C4" s="984"/>
+      <c r="B4" s="993"/>
+      <c r="C4" s="993"/>
       <c r="AD4" s="3"/>
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
@@ -10844,44 +10844,44 @@
         <v>191</v>
       </c>
       <c r="F1" s="271"/>
-      <c r="G1" s="944" t="s">
+      <c r="G1" s="951" t="s">
         <v>744</v>
       </c>
-      <c r="H1" s="944"/>
-      <c r="I1" s="944"/>
-      <c r="J1" s="944"/>
-      <c r="K1" s="944"/>
-      <c r="L1" s="944"/>
+      <c r="H1" s="951"/>
+      <c r="I1" s="951"/>
+      <c r="J1" s="951"/>
+      <c r="K1" s="951"/>
+      <c r="L1" s="951"/>
       <c r="M1" s="128"/>
-      <c r="N1" s="943" t="s">
+      <c r="N1" s="950" t="s">
         <v>190</v>
       </c>
-      <c r="P1" s="943" t="s">
+      <c r="P1" s="950" t="s">
         <v>193</v>
       </c>
-      <c r="R1" s="943" t="s">
+      <c r="R1" s="950" t="s">
         <v>219</v>
       </c>
-      <c r="T1" s="943" t="s">
+      <c r="T1" s="950" t="s">
         <v>242</v>
       </c>
-      <c r="V1" s="943" t="s">
+      <c r="V1" s="950" t="s">
         <v>243</v>
       </c>
-      <c r="X1" s="943" t="s">
+      <c r="X1" s="950" t="s">
         <v>220</v>
       </c>
-      <c r="Z1" s="943" t="s">
+      <c r="Z1" s="950" t="s">
         <v>244</v>
       </c>
-      <c r="AB1" s="945" t="s">
+      <c r="AB1" s="952" t="s">
         <v>740</v>
       </c>
       <c r="AC1" s="123"/>
-      <c r="AD1" s="940" t="s">
+      <c r="AD1" s="947" t="s">
         <v>989</v>
       </c>
-      <c r="AF1" s="941" t="s">
+      <c r="AF1" s="948" t="s">
         <v>990</v>
       </c>
     </row>
@@ -10911,24 +10911,24 @@
         <v>7</v>
       </c>
       <c r="M2" s="129"/>
-      <c r="N2" s="943"/>
-      <c r="P2" s="943"/>
-      <c r="R2" s="943"/>
-      <c r="T2" s="943"/>
-      <c r="V2" s="943"/>
-      <c r="X2" s="943"/>
-      <c r="Z2" s="943"/>
-      <c r="AB2" s="945"/>
+      <c r="N2" s="950"/>
+      <c r="P2" s="950"/>
+      <c r="R2" s="950"/>
+      <c r="T2" s="950"/>
+      <c r="V2" s="950"/>
+      <c r="X2" s="950"/>
+      <c r="Z2" s="950"/>
+      <c r="AB2" s="952"/>
       <c r="AC2" s="123"/>
-      <c r="AD2" s="940"/>
-      <c r="AF2" s="941"/>
+      <c r="AD2" s="947"/>
+      <c r="AF2" s="948"/>
     </row>
     <row r="4" spans="1:32" ht="15.6">
-      <c r="A4" s="987" t="s">
+      <c r="A4" s="998" t="s">
         <v>155</v>
       </c>
-      <c r="B4" s="987"/>
-      <c r="C4" s="987"/>
+      <c r="B4" s="998"/>
+      <c r="C4" s="998"/>
       <c r="AD4" s="3"/>
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
@@ -11248,34 +11248,34 @@
       <c r="AF10" s="936"/>
     </row>
     <row r="11" spans="1:32" s="1" customFormat="1" ht="191.25" customHeight="1">
-      <c r="A11" s="988" t="s">
+      <c r="A11" s="999" t="s">
         <v>107</v>
       </c>
-      <c r="B11" s="991" t="s">
+      <c r="B11" s="1002" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="993" t="s">
+      <c r="C11" s="994" t="s">
         <v>997</v>
       </c>
       <c r="D11" s="193"/>
-      <c r="E11" s="993"/>
+      <c r="E11" s="994"/>
       <c r="F11" s="193"/>
-      <c r="G11" s="957" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="957" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="957" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" s="957" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" s="957" t="s">
-        <v>10</v>
-      </c>
-      <c r="L11" s="957" t="s">
+      <c r="G11" s="988" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="988" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="988" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="988" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="988" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" s="988" t="s">
         <v>10</v>
       </c>
       <c r="M11" s="186"/>
@@ -11311,18 +11311,18 @@
       <c r="AF11" s="936"/>
     </row>
     <row r="12" spans="1:32" s="1" customFormat="1" ht="13.8">
-      <c r="A12" s="989"/>
-      <c r="B12" s="972"/>
-      <c r="C12" s="994"/>
+      <c r="A12" s="1000"/>
+      <c r="B12" s="960"/>
+      <c r="C12" s="995"/>
       <c r="D12" s="193"/>
-      <c r="E12" s="994"/>
+      <c r="E12" s="995"/>
       <c r="F12" s="193"/>
-      <c r="G12" s="996"/>
-      <c r="H12" s="996"/>
-      <c r="I12" s="996"/>
-      <c r="J12" s="996"/>
-      <c r="K12" s="996"/>
-      <c r="L12" s="996"/>
+      <c r="G12" s="997"/>
+      <c r="H12" s="997"/>
+      <c r="I12" s="997"/>
+      <c r="J12" s="997"/>
+      <c r="K12" s="997"/>
+      <c r="L12" s="997"/>
       <c r="M12" s="188"/>
       <c r="N12" s="256"/>
       <c r="P12" s="914"/>
@@ -11343,18 +11343,18 @@
       <c r="AF12" s="936"/>
     </row>
     <row r="13" spans="1:32" s="1" customFormat="1" ht="13.8">
-      <c r="A13" s="989"/>
-      <c r="B13" s="972"/>
-      <c r="C13" s="994"/>
+      <c r="A13" s="1000"/>
+      <c r="B13" s="960"/>
+      <c r="C13" s="995"/>
       <c r="D13" s="193"/>
-      <c r="E13" s="994"/>
+      <c r="E13" s="995"/>
       <c r="F13" s="193"/>
-      <c r="G13" s="996"/>
-      <c r="H13" s="996"/>
-      <c r="I13" s="996"/>
-      <c r="J13" s="996"/>
-      <c r="K13" s="996"/>
-      <c r="L13" s="996"/>
+      <c r="G13" s="997"/>
+      <c r="H13" s="997"/>
+      <c r="I13" s="997"/>
+      <c r="J13" s="997"/>
+      <c r="K13" s="997"/>
+      <c r="L13" s="997"/>
       <c r="M13" s="188"/>
       <c r="N13" s="256"/>
       <c r="P13" s="914"/>
@@ -11375,18 +11375,18 @@
       <c r="AF13" s="936"/>
     </row>
     <row r="14" spans="1:32" s="1" customFormat="1" ht="35.25" customHeight="1">
-      <c r="A14" s="990"/>
-      <c r="B14" s="992"/>
-      <c r="C14" s="995"/>
+      <c r="A14" s="1001"/>
+      <c r="B14" s="1003"/>
+      <c r="C14" s="996"/>
       <c r="D14" s="193"/>
-      <c r="E14" s="995"/>
+      <c r="E14" s="996"/>
       <c r="F14" s="193"/>
-      <c r="G14" s="958"/>
-      <c r="H14" s="958"/>
-      <c r="I14" s="958"/>
-      <c r="J14" s="958"/>
-      <c r="K14" s="958"/>
-      <c r="L14" s="958"/>
+      <c r="G14" s="989"/>
+      <c r="H14" s="989"/>
+      <c r="I14" s="989"/>
+      <c r="J14" s="989"/>
+      <c r="K14" s="989"/>
+      <c r="L14" s="989"/>
       <c r="M14" s="176"/>
       <c r="N14" s="264"/>
       <c r="P14" s="913"/>
@@ -13016,6 +13016,17 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="AD1:AD2"/>
+    <mergeCell ref="AF1:AF2"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="R1:R2"/>
     <mergeCell ref="T1:T2"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="K11:K14"/>
@@ -13027,17 +13038,6 @@
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="G1:L1"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="AD1:AD2"/>
-    <mergeCell ref="AF1:AF2"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="X1:X2"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:M11 G15:M22 G24:M37 G38:N38" xr:uid="{00000000-0002-0000-0A00-000000000000}">
@@ -13068,9 +13068,9 @@
   <dimension ref="A1:AF20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="D1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z14" sqref="Z14"/>
-      <selection pane="bottomLeft" activeCell="AD5" sqref="AD5"/>
+      <selection pane="bottomLeft" activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -13083,9 +13083,9 @@
     <col min="6" max="6" width="1.109375" style="269" customWidth="1"/>
     <col min="7" max="12" width="6.88671875" customWidth="1"/>
     <col min="13" max="13" width="1.6640625" style="92" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" style="1000"/>
+    <col min="14" max="14" width="11.44140625" style="939"/>
     <col min="15" max="15" width="3.5546875" customWidth="1"/>
-    <col min="16" max="16" width="11.44140625" style="1000"/>
+    <col min="16" max="16" width="11.44140625" style="939"/>
     <col min="17" max="17" width="1.5546875" customWidth="1"/>
     <col min="18" max="18" width="42" customWidth="1"/>
     <col min="19" max="19" width="1.109375" customWidth="1"/>
@@ -13095,7 +13095,7 @@
     <col min="23" max="23" width="1" customWidth="1"/>
     <col min="24" max="24" width="11.44140625" customWidth="1"/>
     <col min="25" max="25" width="1" customWidth="1"/>
-    <col min="26" max="26" width="11.44140625" style="1000" customWidth="1"/>
+    <col min="26" max="26" width="11.44140625" style="939" customWidth="1"/>
     <col min="27" max="27" width="1.5546875" customWidth="1"/>
     <col min="28" max="28" width="17.33203125" hidden="1" customWidth="1"/>
     <col min="29" max="29" width="0.88671875" customWidth="1"/>
@@ -13118,44 +13118,44 @@
         <v>191</v>
       </c>
       <c r="F1" s="271"/>
-      <c r="G1" s="944" t="s">
+      <c r="G1" s="951" t="s">
         <v>744</v>
       </c>
-      <c r="H1" s="944"/>
-      <c r="I1" s="944"/>
-      <c r="J1" s="944"/>
-      <c r="K1" s="944"/>
-      <c r="L1" s="944"/>
+      <c r="H1" s="951"/>
+      <c r="I1" s="951"/>
+      <c r="J1" s="951"/>
+      <c r="K1" s="951"/>
+      <c r="L1" s="951"/>
       <c r="M1" s="128"/>
-      <c r="N1" s="999" t="s">
+      <c r="N1" s="1004" t="s">
         <v>190</v>
       </c>
-      <c r="P1" s="999" t="s">
+      <c r="P1" s="1004" t="s">
         <v>194</v>
       </c>
-      <c r="R1" s="943" t="s">
+      <c r="R1" s="950" t="s">
         <v>219</v>
       </c>
-      <c r="T1" s="943" t="s">
+      <c r="T1" s="950" t="s">
         <v>242</v>
       </c>
-      <c r="V1" s="943" t="s">
+      <c r="V1" s="950" t="s">
         <v>243</v>
       </c>
-      <c r="X1" s="943" t="s">
+      <c r="X1" s="950" t="s">
         <v>220</v>
       </c>
-      <c r="Z1" s="999" t="s">
+      <c r="Z1" s="1004" t="s">
         <v>244</v>
       </c>
-      <c r="AB1" s="945" t="s">
+      <c r="AB1" s="952" t="s">
         <v>740</v>
       </c>
       <c r="AC1" s="123"/>
-      <c r="AD1" s="940" t="s">
+      <c r="AD1" s="947" t="s">
         <v>989</v>
       </c>
-      <c r="AF1" s="941" t="s">
+      <c r="AF1" s="948" t="s">
         <v>990</v>
       </c>
     </row>
@@ -13185,23 +13185,23 @@
         <v>7</v>
       </c>
       <c r="M2" s="129"/>
-      <c r="N2" s="999"/>
-      <c r="P2" s="999"/>
-      <c r="R2" s="943"/>
-      <c r="T2" s="943"/>
-      <c r="V2" s="943"/>
-      <c r="X2" s="943"/>
-      <c r="Z2" s="999"/>
-      <c r="AB2" s="945"/>
+      <c r="N2" s="1004"/>
+      <c r="P2" s="1004"/>
+      <c r="R2" s="950"/>
+      <c r="T2" s="950"/>
+      <c r="V2" s="950"/>
+      <c r="X2" s="950"/>
+      <c r="Z2" s="1004"/>
+      <c r="AB2" s="952"/>
       <c r="AC2" s="123"/>
-      <c r="AD2" s="940"/>
-      <c r="AF2" s="941"/>
+      <c r="AD2" s="947"/>
+      <c r="AF2" s="948"/>
     </row>
     <row r="4" spans="1:32" ht="15">
-      <c r="A4" s="984" t="s">
+      <c r="A4" s="993" t="s">
         <v>342</v>
       </c>
-      <c r="B4" s="984"/>
+      <c r="B4" s="993"/>
       <c r="AD4" s="3"/>
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
@@ -13220,12 +13220,12 @@
       <c r="K5" s="63"/>
       <c r="L5" s="63"/>
       <c r="M5" s="113"/>
-      <c r="N5" s="1001"/>
-      <c r="P5" s="1001"/>
+      <c r="N5" s="940"/>
+      <c r="P5" s="940"/>
       <c r="V5" s="315"/>
       <c r="W5" s="315"/>
       <c r="Y5" s="315"/>
-      <c r="Z5" s="1001"/>
+      <c r="Z5" s="940"/>
       <c r="AB5" s="315"/>
       <c r="AC5" s="315"/>
       <c r="AD5" s="3"/>
@@ -13266,10 +13266,10 @@
         <v>10</v>
       </c>
       <c r="M6" s="188"/>
-      <c r="N6" s="1002" t="s">
+      <c r="N6" s="941" t="s">
         <v>776</v>
       </c>
-      <c r="P6" s="1002" t="s">
+      <c r="P6" s="941" t="s">
         <v>819</v>
       </c>
       <c r="R6" s="824" t="s">
@@ -13286,9 +13286,9 @@
         <v>612</v>
       </c>
       <c r="Y6" s="425"/>
-      <c r="Z6" s="1006">
+      <c r="Z6" s="945">
         <f>IF(OR(X6="A",X7="A",X8="A"),"",IF(OR(X6="N",X7="N",X8="N"),0,1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA6" s="315"/>
       <c r="AB6" s="800" t="s">
@@ -13315,8 +13315,8 @@
       <c r="K7" s="314"/>
       <c r="L7" s="314"/>
       <c r="M7" s="188"/>
-      <c r="N7" s="1002"/>
-      <c r="P7" s="1002"/>
+      <c r="N7" s="941"/>
+      <c r="P7" s="941"/>
       <c r="R7" s="358" t="s">
         <v>248</v>
       </c>
@@ -13324,10 +13324,10 @@
       <c r="T7" s="305"/>
       <c r="V7" s="314"/>
       <c r="X7" s="590" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="Y7" s="425"/>
-      <c r="Z7" s="1002"/>
+      <c r="Z7" s="941"/>
       <c r="AB7" s="800"/>
       <c r="AD7" s="936"/>
       <c r="AE7" s="936"/>
@@ -13349,8 +13349,8 @@
       <c r="K8" s="83"/>
       <c r="L8" s="83"/>
       <c r="M8" s="176"/>
-      <c r="N8" s="1003"/>
-      <c r="P8" s="1003"/>
+      <c r="N8" s="942"/>
+      <c r="P8" s="942"/>
       <c r="R8" s="828" t="s">
         <v>731</v>
       </c>
@@ -13365,7 +13365,7 @@
         <v>612</v>
       </c>
       <c r="Y8" s="315"/>
-      <c r="Z8" s="1003"/>
+      <c r="Z8" s="942"/>
       <c r="AA8" s="315"/>
       <c r="AB8" s="798"/>
       <c r="AC8" s="315"/>
@@ -13407,10 +13407,10 @@
         <v>10</v>
       </c>
       <c r="M9" s="186"/>
-      <c r="N9" s="1004" t="s">
+      <c r="N9" s="943" t="s">
         <v>192</v>
       </c>
-      <c r="P9" s="1004" t="s">
+      <c r="P9" s="943" t="s">
         <v>819</v>
       </c>
       <c r="R9" s="890" t="s">
@@ -13429,7 +13429,7 @@
         <v>612</v>
       </c>
       <c r="Y9" s="425"/>
-      <c r="Z9" s="1006">
+      <c r="Z9" s="945">
         <f>IF(OR(X9="A",X10="A"),"",IF(OR(X9="N",X10="N"),0,1))</f>
         <v>1</v>
       </c>
@@ -13456,9 +13456,9 @@
       <c r="K10" s="307"/>
       <c r="L10" s="307"/>
       <c r="M10" s="262"/>
-      <c r="N10" s="1003"/>
+      <c r="N10" s="942"/>
       <c r="O10" s="381"/>
-      <c r="P10" s="1003"/>
+      <c r="P10" s="942"/>
       <c r="R10" s="897" t="s">
         <v>822</v>
       </c>
@@ -13473,7 +13473,7 @@
         <v>612</v>
       </c>
       <c r="Y10" s="425"/>
-      <c r="Z10" s="1002"/>
+      <c r="Z10" s="941"/>
       <c r="AB10" s="798"/>
       <c r="AD10" s="936"/>
       <c r="AE10" s="936"/>
@@ -13511,10 +13511,10 @@
         <v>10</v>
       </c>
       <c r="M11" s="186"/>
-      <c r="N11" s="1004" t="s">
+      <c r="N11" s="943" t="s">
         <v>776</v>
       </c>
-      <c r="P11" s="1004" t="s">
+      <c r="P11" s="943" t="s">
         <v>819</v>
       </c>
       <c r="R11" s="300" t="s">
@@ -13533,7 +13533,7 @@
         <v>612</v>
       </c>
       <c r="Y11" s="425"/>
-      <c r="Z11" s="1006">
+      <c r="Z11" s="945">
         <f>IF(OR(X11="A",X12="A",X13="A"),"",IF(OR(X11="N",X12="N",X13="N"),0,1))</f>
         <v>1</v>
       </c>
@@ -13560,11 +13560,11 @@
       <c r="K12" s="314"/>
       <c r="L12" s="314"/>
       <c r="M12" s="188"/>
-      <c r="N12" s="1004" t="s">
+      <c r="N12" s="943" t="s">
         <v>777</v>
       </c>
       <c r="O12" s="381"/>
-      <c r="P12" s="1002"/>
+      <c r="P12" s="941"/>
       <c r="R12" s="300" t="s">
         <v>327</v>
       </c>
@@ -13577,7 +13577,7 @@
         <v>612</v>
       </c>
       <c r="Y12" s="425"/>
-      <c r="Z12" s="1002"/>
+      <c r="Z12" s="941"/>
       <c r="AB12" s="800"/>
       <c r="AD12" s="936"/>
       <c r="AE12" s="936"/>
@@ -13597,10 +13597,10 @@
       <c r="K13" s="307"/>
       <c r="L13" s="307"/>
       <c r="M13" s="262"/>
-      <c r="N13" s="1004" t="s">
+      <c r="N13" s="943" t="s">
         <v>776</v>
       </c>
-      <c r="P13" s="1003"/>
+      <c r="P13" s="942"/>
       <c r="R13" s="828" t="s">
         <v>713</v>
       </c>
@@ -13612,7 +13612,7 @@
       <c r="X13" s="590" t="s">
         <v>612</v>
       </c>
-      <c r="Z13" s="1003"/>
+      <c r="Z13" s="942"/>
       <c r="AB13" s="798"/>
       <c r="AD13" s="936"/>
       <c r="AE13" s="936"/>
@@ -13650,11 +13650,11 @@
         <v>10</v>
       </c>
       <c r="M14" s="192"/>
-      <c r="N14" s="1005" t="s">
+      <c r="N14" s="944" t="s">
         <v>694</v>
       </c>
       <c r="O14" s="315"/>
-      <c r="P14" s="1005" t="s">
+      <c r="P14" s="944" t="s">
         <v>750</v>
       </c>
       <c r="Q14" s="315"/>
@@ -13674,7 +13674,7 @@
         <v>612</v>
       </c>
       <c r="Y14" s="425"/>
-      <c r="Z14" s="1006">
+      <c r="Z14" s="945">
         <f>IF(OR(X14="A",Size="XS"),"",IF(OR(X14="N"),0,1))</f>
         <v>1</v>
       </c>
@@ -13719,10 +13719,10 @@
         <v>10</v>
       </c>
       <c r="M15" s="192"/>
-      <c r="N15" s="1004" t="s">
+      <c r="N15" s="943" t="s">
         <v>776</v>
       </c>
-      <c r="P15" s="1005" t="s">
+      <c r="P15" s="944" t="s">
         <v>819</v>
       </c>
       <c r="R15" s="897" t="s">
@@ -13739,7 +13739,7 @@
         <v>612</v>
       </c>
       <c r="Y15" s="425"/>
-      <c r="Z15" s="1006">
+      <c r="Z15" s="945">
         <f>IF(OR(X15="A"),"",IF(OR(X15="N"),0,1))</f>
         <v>1</v>
       </c>
@@ -13786,10 +13786,10 @@
         <v>10</v>
       </c>
       <c r="M16" s="186"/>
-      <c r="N16" s="1004" t="s">
+      <c r="N16" s="943" t="s">
         <v>192</v>
       </c>
-      <c r="P16" s="1004" t="s">
+      <c r="P16" s="943" t="s">
         <v>10</v>
       </c>
       <c r="R16" s="910" t="s">
@@ -13808,7 +13808,7 @@
         <v>612</v>
       </c>
       <c r="Y16" s="425"/>
-      <c r="Z16" s="1006">
+      <c r="Z16" s="945">
         <f>IF(OR(X16="A",X17="A",X18="A",X19="A"),"",IF(OR(X16="N",X17="N",X18="N",X19="N"),0,1))</f>
         <v>1</v>
       </c>
@@ -13837,9 +13837,9 @@
       <c r="K17" s="314"/>
       <c r="L17" s="314"/>
       <c r="M17" s="188"/>
-      <c r="N17" s="1004"/>
+      <c r="N17" s="943"/>
       <c r="O17" s="381"/>
-      <c r="P17" s="1002"/>
+      <c r="P17" s="941"/>
       <c r="R17" s="824" t="s">
         <v>729</v>
       </c>
@@ -13850,7 +13850,7 @@
         <v>612</v>
       </c>
       <c r="Y17" s="425"/>
-      <c r="Z17" s="1002"/>
+      <c r="Z17" s="941"/>
       <c r="AB17" s="800"/>
       <c r="AD17" s="936"/>
       <c r="AE17" s="936"/>
@@ -13872,9 +13872,9 @@
       <c r="K18" s="314"/>
       <c r="L18" s="314"/>
       <c r="M18" s="188"/>
-      <c r="N18" s="1004"/>
+      <c r="N18" s="943"/>
       <c r="O18" s="381"/>
-      <c r="P18" s="1002"/>
+      <c r="P18" s="941"/>
       <c r="R18" s="824" t="s">
         <v>954</v>
       </c>
@@ -13884,7 +13884,7 @@
       <c r="X18" s="590" t="s">
         <v>612</v>
       </c>
-      <c r="Z18" s="1002"/>
+      <c r="Z18" s="941"/>
       <c r="AB18" s="800"/>
       <c r="AD18" s="936"/>
       <c r="AE18" s="936"/>
@@ -13904,8 +13904,8 @@
       <c r="K19" s="307"/>
       <c r="L19" s="307"/>
       <c r="M19" s="262"/>
-      <c r="N19" s="1004"/>
-      <c r="P19" s="1003"/>
+      <c r="N19" s="943"/>
+      <c r="P19" s="942"/>
       <c r="R19" s="300" t="s">
         <v>341</v>
       </c>
@@ -13917,7 +13917,7 @@
       <c r="X19" s="590" t="s">
         <v>612</v>
       </c>
-      <c r="Z19" s="1003"/>
+      <c r="Z19" s="942"/>
       <c r="AB19" s="798"/>
       <c r="AD19" s="937"/>
       <c r="AE19" s="937"/>
@@ -13957,10 +13957,10 @@
         <v>10</v>
       </c>
       <c r="M20" s="192"/>
-      <c r="N20" s="1005" t="s">
+      <c r="N20" s="944" t="s">
         <v>192</v>
       </c>
-      <c r="P20" s="1005" t="s">
+      <c r="P20" s="944" t="s">
         <v>10</v>
       </c>
       <c r="R20" s="300" t="s">
@@ -13979,7 +13979,7 @@
         <v>612</v>
       </c>
       <c r="Y20" s="425"/>
-      <c r="Z20" s="1006">
+      <c r="Z20" s="945">
         <f>IF(OR(X20="A"),"",IF(OR(X20="N"),0,1))</f>
         <v>1</v>
       </c>
@@ -14085,44 +14085,44 @@
         <v>191</v>
       </c>
       <c r="F1" s="271"/>
-      <c r="G1" s="944" t="s">
+      <c r="G1" s="951" t="s">
         <v>744</v>
       </c>
-      <c r="H1" s="944"/>
-      <c r="I1" s="944"/>
-      <c r="J1" s="944"/>
-      <c r="K1" s="944"/>
-      <c r="L1" s="944"/>
+      <c r="H1" s="951"/>
+      <c r="I1" s="951"/>
+      <c r="J1" s="951"/>
+      <c r="K1" s="951"/>
+      <c r="L1" s="951"/>
       <c r="M1" s="128"/>
-      <c r="N1" s="943" t="s">
+      <c r="N1" s="950" t="s">
         <v>190</v>
       </c>
-      <c r="P1" s="943" t="s">
+      <c r="P1" s="950" t="s">
         <v>193</v>
       </c>
-      <c r="R1" s="943" t="s">
+      <c r="R1" s="950" t="s">
         <v>219</v>
       </c>
-      <c r="T1" s="943" t="s">
+      <c r="T1" s="950" t="s">
         <v>242</v>
       </c>
-      <c r="V1" s="943" t="s">
+      <c r="V1" s="950" t="s">
         <v>243</v>
       </c>
-      <c r="X1" s="943" t="s">
+      <c r="X1" s="950" t="s">
         <v>220</v>
       </c>
-      <c r="Z1" s="943" t="s">
+      <c r="Z1" s="950" t="s">
         <v>244</v>
       </c>
-      <c r="AB1" s="945" t="s">
+      <c r="AB1" s="952" t="s">
         <v>740</v>
       </c>
       <c r="AC1" s="123"/>
-      <c r="AD1" s="940" t="s">
+      <c r="AD1" s="947" t="s">
         <v>989</v>
       </c>
-      <c r="AF1" s="941" t="s">
+      <c r="AF1" s="948" t="s">
         <v>990</v>
       </c>
     </row>
@@ -14152,24 +14152,24 @@
         <v>7</v>
       </c>
       <c r="M2" s="129"/>
-      <c r="N2" s="943"/>
-      <c r="P2" s="943"/>
-      <c r="R2" s="943"/>
-      <c r="T2" s="943"/>
-      <c r="V2" s="943"/>
-      <c r="X2" s="943"/>
-      <c r="Z2" s="943"/>
-      <c r="AB2" s="945"/>
+      <c r="N2" s="950"/>
+      <c r="P2" s="950"/>
+      <c r="R2" s="950"/>
+      <c r="T2" s="950"/>
+      <c r="V2" s="950"/>
+      <c r="X2" s="950"/>
+      <c r="Z2" s="950"/>
+      <c r="AB2" s="952"/>
       <c r="AC2" s="123"/>
-      <c r="AD2" s="940"/>
-      <c r="AF2" s="941"/>
+      <c r="AD2" s="947"/>
+      <c r="AF2" s="948"/>
     </row>
     <row r="3" spans="1:32" s="1" customFormat="1" ht="33" customHeight="1">
-      <c r="A3" s="997" t="s">
+      <c r="A3" s="1005" t="s">
         <v>792</v>
       </c>
-      <c r="B3" s="997"/>
-      <c r="C3" s="997"/>
+      <c r="B3" s="1005"/>
+      <c r="C3" s="1005"/>
       <c r="D3" s="197"/>
       <c r="E3" s="197"/>
       <c r="F3" s="197"/>
@@ -15247,12 +15247,12 @@
     </row>
     <row r="11" spans="1:22">
       <c r="A11" s="879"/>
-      <c r="B11" s="998"/>
-      <c r="C11" s="998"/>
-      <c r="D11" s="998"/>
-      <c r="E11" s="998"/>
-      <c r="F11" s="998"/>
-      <c r="G11" s="998"/>
+      <c r="B11" s="1006"/>
+      <c r="C11" s="1006"/>
+      <c r="D11" s="1006"/>
+      <c r="E11" s="1006"/>
+      <c r="F11" s="1006"/>
+      <c r="G11" s="1006"/>
       <c r="H11" s="879"/>
       <c r="I11" s="879"/>
       <c r="J11" s="879"/>
@@ -17095,11 +17095,11 @@
       </c>
       <c r="F25" s="640">
         <f>SUM('Section 9_Marketing'!Z6:Z20)-SUMIF('Section 9_Marketing'!P6:P20,"O",'Section 9_Marketing'!Z6:Z20)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H25" s="641">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="J25" s="640">
         <f>COUNTIFS('Section 9_Marketing'!P6:P20,"X",'Section 9_Marketing'!Z6:Z20,1)+COUNTIFS('Section 9_Marketing'!P6:P20,"X",'Section 9_Marketing'!Z6:Z20,0)</f>
@@ -17166,12 +17166,12 @@
       <c r="E28" s="625"/>
       <c r="F28" s="624">
         <f>SUM(F17:F26)</f>
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G28" s="625"/>
       <c r="H28" s="626">
         <f>IFERROR(F28/D28,0%)</f>
-        <v>1</v>
+        <v>0.98901098901098905</v>
       </c>
       <c r="I28" s="625"/>
       <c r="J28" s="627">
@@ -17286,43 +17286,43 @@
         <v>191</v>
       </c>
       <c r="F1" s="271"/>
-      <c r="G1" s="944" t="s">
+      <c r="G1" s="951" t="s">
         <v>744</v>
       </c>
-      <c r="H1" s="944"/>
-      <c r="I1" s="944"/>
-      <c r="J1" s="944"/>
-      <c r="K1" s="944"/>
-      <c r="L1" s="944"/>
+      <c r="H1" s="951"/>
+      <c r="I1" s="951"/>
+      <c r="J1" s="951"/>
+      <c r="K1" s="951"/>
+      <c r="L1" s="951"/>
       <c r="M1" s="128"/>
-      <c r="N1" s="943" t="s">
+      <c r="N1" s="950" t="s">
         <v>190</v>
       </c>
-      <c r="P1" s="943" t="s">
+      <c r="P1" s="950" t="s">
         <v>193</v>
       </c>
-      <c r="R1" s="943" t="s">
+      <c r="R1" s="950" t="s">
         <v>219</v>
       </c>
-      <c r="T1" s="943" t="s">
+      <c r="T1" s="950" t="s">
         <v>242</v>
       </c>
-      <c r="V1" s="943" t="s">
+      <c r="V1" s="950" t="s">
         <v>243</v>
       </c>
-      <c r="X1" s="943" t="s">
+      <c r="X1" s="950" t="s">
         <v>220</v>
       </c>
-      <c r="Z1" s="943" t="s">
+      <c r="Z1" s="950" t="s">
         <v>244</v>
       </c>
-      <c r="AB1" s="945" t="s">
+      <c r="AB1" s="952" t="s">
         <v>740</v>
       </c>
-      <c r="AC1" s="940" t="s">
+      <c r="AC1" s="947" t="s">
         <v>989</v>
       </c>
-      <c r="AE1" s="941" t="s">
+      <c r="AE1" s="948" t="s">
         <v>990</v>
       </c>
     </row>
@@ -17352,16 +17352,16 @@
         <v>7</v>
       </c>
       <c r="M2" s="129"/>
-      <c r="N2" s="943"/>
-      <c r="P2" s="943"/>
-      <c r="R2" s="943"/>
-      <c r="T2" s="943"/>
-      <c r="V2" s="943"/>
-      <c r="X2" s="943"/>
-      <c r="Z2" s="943"/>
-      <c r="AB2" s="945"/>
-      <c r="AC2" s="940"/>
-      <c r="AE2" s="941"/>
+      <c r="N2" s="950"/>
+      <c r="P2" s="950"/>
+      <c r="R2" s="950"/>
+      <c r="T2" s="950"/>
+      <c r="V2" s="950"/>
+      <c r="X2" s="950"/>
+      <c r="Z2" s="950"/>
+      <c r="AB2" s="952"/>
+      <c r="AC2" s="947"/>
+      <c r="AE2" s="948"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="203"/>
@@ -17391,11 +17391,11 @@
       <c r="M4" s="130"/>
     </row>
     <row r="5" spans="1:31" s="3" customFormat="1" ht="15">
-      <c r="A5" s="942" t="s">
+      <c r="A5" s="949" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="942"/>
-      <c r="C5" s="942"/>
+      <c r="B5" s="949"/>
+      <c r="C5" s="949"/>
       <c r="D5" s="124"/>
       <c r="E5" s="124"/>
       <c r="F5" s="124"/>
@@ -18135,44 +18135,44 @@
         <v>191</v>
       </c>
       <c r="F1" s="271"/>
-      <c r="G1" s="944" t="s">
+      <c r="G1" s="951" t="s">
         <v>744</v>
       </c>
-      <c r="H1" s="944"/>
-      <c r="I1" s="944"/>
-      <c r="J1" s="944"/>
-      <c r="K1" s="944"/>
-      <c r="L1" s="944"/>
+      <c r="H1" s="951"/>
+      <c r="I1" s="951"/>
+      <c r="J1" s="951"/>
+      <c r="K1" s="951"/>
+      <c r="L1" s="951"/>
       <c r="M1" s="128"/>
-      <c r="N1" s="943" t="s">
+      <c r="N1" s="950" t="s">
         <v>190</v>
       </c>
-      <c r="P1" s="943" t="s">
+      <c r="P1" s="950" t="s">
         <v>193</v>
       </c>
-      <c r="R1" s="943" t="s">
+      <c r="R1" s="950" t="s">
         <v>219</v>
       </c>
-      <c r="T1" s="943" t="s">
+      <c r="T1" s="950" t="s">
         <v>242</v>
       </c>
-      <c r="V1" s="943" t="s">
+      <c r="V1" s="950" t="s">
         <v>243</v>
       </c>
-      <c r="X1" s="943" t="s">
+      <c r="X1" s="950" t="s">
         <v>220</v>
       </c>
-      <c r="Z1" s="943" t="s">
+      <c r="Z1" s="950" t="s">
         <v>244</v>
       </c>
-      <c r="AB1" s="945" t="s">
+      <c r="AB1" s="952" t="s">
         <v>740</v>
       </c>
       <c r="AC1" s="123"/>
-      <c r="AD1" s="940" t="s">
+      <c r="AD1" s="947" t="s">
         <v>989</v>
       </c>
-      <c r="AF1" s="941" t="s">
+      <c r="AF1" s="948" t="s">
         <v>990</v>
       </c>
     </row>
@@ -18202,17 +18202,17 @@
         <v>7</v>
       </c>
       <c r="M2" s="129"/>
-      <c r="N2" s="943"/>
-      <c r="P2" s="943"/>
-      <c r="R2" s="943"/>
-      <c r="T2" s="943"/>
-      <c r="V2" s="943"/>
-      <c r="X2" s="943"/>
-      <c r="Z2" s="943"/>
-      <c r="AB2" s="945"/>
+      <c r="N2" s="950"/>
+      <c r="P2" s="950"/>
+      <c r="R2" s="950"/>
+      <c r="T2" s="950"/>
+      <c r="V2" s="950"/>
+      <c r="X2" s="950"/>
+      <c r="Z2" s="950"/>
+      <c r="AB2" s="952"/>
       <c r="AC2" s="123"/>
-      <c r="AD2" s="940"/>
-      <c r="AF2" s="941"/>
+      <c r="AD2" s="947"/>
+      <c r="AF2" s="948"/>
     </row>
     <row r="4" spans="1:32" ht="13.8">
       <c r="AD4" s="3"/>
@@ -18220,11 +18220,11 @@
       <c r="AF4" s="3"/>
     </row>
     <row r="5" spans="1:32" s="97" customFormat="1" ht="15">
-      <c r="A5" s="950" t="s">
+      <c r="A5" s="957" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="950"/>
-      <c r="C5" s="950"/>
+      <c r="B5" s="957"/>
+      <c r="C5" s="957"/>
       <c r="D5" s="135"/>
       <c r="E5" s="135"/>
       <c r="F5" s="135"/>
@@ -18278,11 +18278,11 @@
       <c r="B7" s="231" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="946" t="s">
+      <c r="C7" s="953" t="s">
         <v>842</v>
       </c>
       <c r="D7" s="136"/>
-      <c r="E7" s="946"/>
+      <c r="E7" s="953"/>
       <c r="F7" s="136"/>
       <c r="G7" s="225">
         <v>1</v>
@@ -18339,9 +18339,9 @@
     <row r="8" spans="1:32" s="97" customFormat="1" ht="37.5" customHeight="1">
       <c r="A8" s="226"/>
       <c r="B8" s="234"/>
-      <c r="C8" s="946"/>
+      <c r="C8" s="953"/>
       <c r="D8" s="136"/>
-      <c r="E8" s="946"/>
+      <c r="E8" s="953"/>
       <c r="F8" s="136"/>
       <c r="G8" s="226"/>
       <c r="H8" s="226"/>
@@ -18375,9 +18375,9 @@
     <row r="9" spans="1:32" s="97" customFormat="1" ht="48.75" customHeight="1">
       <c r="A9" s="226"/>
       <c r="B9" s="234"/>
-      <c r="C9" s="947"/>
+      <c r="C9" s="954"/>
       <c r="D9" s="136"/>
-      <c r="E9" s="947"/>
+      <c r="E9" s="954"/>
       <c r="F9" s="136"/>
       <c r="G9" s="226"/>
       <c r="H9" s="226"/>
@@ -18413,11 +18413,11 @@
       <c r="B10" s="230" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="948" t="s">
+      <c r="C10" s="955" t="s">
         <v>473</v>
       </c>
       <c r="D10" s="137"/>
-      <c r="E10" s="948" t="s">
+      <c r="E10" s="955" t="s">
         <v>666</v>
       </c>
       <c r="F10" s="137"/>
@@ -18476,9 +18476,9 @@
     <row r="11" spans="1:32" s="97" customFormat="1" ht="22.8">
       <c r="A11" s="226"/>
       <c r="B11" s="234"/>
-      <c r="C11" s="949"/>
+      <c r="C11" s="956"/>
       <c r="D11" s="138"/>
-      <c r="E11" s="949"/>
+      <c r="E11" s="956"/>
       <c r="F11" s="138"/>
       <c r="G11" s="226"/>
       <c r="H11" s="226"/>
@@ -18512,9 +18512,9 @@
     <row r="12" spans="1:32" s="97" customFormat="1" ht="43.5" customHeight="1">
       <c r="A12" s="226"/>
       <c r="B12" s="234"/>
-      <c r="C12" s="949"/>
+      <c r="C12" s="956"/>
       <c r="D12" s="138"/>
-      <c r="E12" s="949"/>
+      <c r="E12" s="956"/>
       <c r="F12" s="138"/>
       <c r="G12" s="226"/>
       <c r="H12" s="226"/>
@@ -20091,46 +20091,46 @@
         <v>191</v>
       </c>
       <c r="F1" s="271"/>
-      <c r="G1" s="944" t="s">
+      <c r="G1" s="951" t="s">
         <v>744</v>
       </c>
-      <c r="H1" s="944"/>
-      <c r="I1" s="944"/>
-      <c r="J1" s="944"/>
-      <c r="K1" s="944"/>
-      <c r="L1" s="944"/>
+      <c r="H1" s="951"/>
+      <c r="I1" s="951"/>
+      <c r="J1" s="951"/>
+      <c r="K1" s="951"/>
+      <c r="L1" s="951"/>
       <c r="M1" s="128"/>
-      <c r="N1" s="943" t="s">
+      <c r="N1" s="950" t="s">
         <v>190</v>
       </c>
-      <c r="P1" s="943" t="s">
+      <c r="P1" s="950" t="s">
         <v>193</v>
       </c>
-      <c r="R1" s="943" t="s">
+      <c r="R1" s="950" t="s">
         <v>219</v>
       </c>
       <c r="S1" s="424"/>
-      <c r="T1" s="943" t="s">
+      <c r="T1" s="950" t="s">
         <v>242</v>
       </c>
-      <c r="V1" s="943" t="s">
+      <c r="V1" s="950" t="s">
         <v>243</v>
       </c>
-      <c r="X1" s="943" t="s">
+      <c r="X1" s="950" t="s">
         <v>220</v>
       </c>
-      <c r="Z1" s="943" t="s">
+      <c r="Z1" s="950" t="s">
         <v>244</v>
       </c>
       <c r="AA1" s="271"/>
-      <c r="AB1" s="945" t="s">
+      <c r="AB1" s="952" t="s">
         <v>740</v>
       </c>
       <c r="AC1" s="123"/>
-      <c r="AD1" s="940" t="s">
+      <c r="AD1" s="947" t="s">
         <v>989</v>
       </c>
-      <c r="AF1" s="941" t="s">
+      <c r="AF1" s="948" t="s">
         <v>990</v>
       </c>
     </row>
@@ -20160,19 +20160,19 @@
         <v>7</v>
       </c>
       <c r="M2" s="129"/>
-      <c r="N2" s="943"/>
-      <c r="P2" s="943"/>
-      <c r="R2" s="943"/>
+      <c r="N2" s="950"/>
+      <c r="P2" s="950"/>
+      <c r="R2" s="950"/>
       <c r="S2" s="424"/>
-      <c r="T2" s="943"/>
-      <c r="V2" s="943"/>
-      <c r="X2" s="943"/>
-      <c r="Z2" s="943"/>
+      <c r="T2" s="950"/>
+      <c r="V2" s="950"/>
+      <c r="X2" s="950"/>
+      <c r="Z2" s="950"/>
       <c r="AA2" s="271"/>
-      <c r="AB2" s="945"/>
+      <c r="AB2" s="952"/>
       <c r="AC2" s="123"/>
-      <c r="AD2" s="940"/>
-      <c r="AF2" s="941"/>
+      <c r="AD2" s="947"/>
+      <c r="AF2" s="948"/>
     </row>
     <row r="4" spans="1:32">
       <c r="AD4" s="3"/>
@@ -20180,11 +20180,11 @@
       <c r="AF4" s="3"/>
     </row>
     <row r="5" spans="1:32" s="1" customFormat="1" ht="15">
-      <c r="A5" s="950" t="s">
+      <c r="A5" s="957" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="950"/>
-      <c r="C5" s="950"/>
+      <c r="B5" s="957"/>
+      <c r="C5" s="957"/>
       <c r="D5" s="135"/>
       <c r="E5" s="135"/>
       <c r="F5" s="135"/>
@@ -20240,17 +20240,17 @@
       <c r="AF6" s="3"/>
     </row>
     <row r="7" spans="1:32" s="1" customFormat="1" ht="115.5" customHeight="1">
-      <c r="A7" s="951" t="s">
+      <c r="A7" s="984" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="951" t="s">
+      <c r="B7" s="984" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="956" t="s">
+      <c r="C7" s="973" t="s">
         <v>763</v>
       </c>
       <c r="D7" s="142"/>
-      <c r="E7" s="956"/>
+      <c r="E7" s="973"/>
       <c r="F7" s="142"/>
       <c r="G7" s="24" t="s">
         <v>10</v>
@@ -20306,11 +20306,11 @@
       <c r="AF7" s="936"/>
     </row>
     <row r="8" spans="1:32" s="1" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A8" s="952"/>
-      <c r="B8" s="952"/>
-      <c r="C8" s="955"/>
+      <c r="A8" s="985"/>
+      <c r="B8" s="985"/>
+      <c r="C8" s="974"/>
       <c r="D8" s="143"/>
-      <c r="E8" s="955"/>
+      <c r="E8" s="974"/>
       <c r="F8" s="143"/>
       <c r="G8" s="30"/>
       <c r="H8" s="30"/>
@@ -20341,13 +20341,13 @@
       <c r="AF8" s="936"/>
     </row>
     <row r="9" spans="1:32" s="1" customFormat="1" ht="45.6">
-      <c r="A9" s="952"/>
-      <c r="B9" s="952"/>
-      <c r="C9" s="955" t="s">
+      <c r="A9" s="985"/>
+      <c r="B9" s="985"/>
+      <c r="C9" s="974" t="s">
         <v>677</v>
       </c>
       <c r="D9" s="143"/>
-      <c r="E9" s="955"/>
+      <c r="E9" s="974"/>
       <c r="F9" s="143"/>
       <c r="G9" s="30" t="s">
         <v>10</v>
@@ -20397,11 +20397,11 @@
       <c r="AF9" s="936"/>
     </row>
     <row r="10" spans="1:32" s="1" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A10" s="952"/>
-      <c r="B10" s="952"/>
-      <c r="C10" s="955"/>
+      <c r="A10" s="985"/>
+      <c r="B10" s="985"/>
+      <c r="C10" s="974"/>
       <c r="D10" s="143"/>
-      <c r="E10" s="955"/>
+      <c r="E10" s="974"/>
       <c r="F10" s="143"/>
       <c r="G10" s="30" t="s">
         <v>10</v>
@@ -20683,7 +20683,7 @@
         <v>747</v>
       </c>
       <c r="D16" s="840"/>
-      <c r="E16" s="957"/>
+      <c r="E16" s="988"/>
       <c r="F16" s="840"/>
       <c r="G16" s="868" t="s">
         <v>10</v>
@@ -20740,7 +20740,7 @@
         <v>746</v>
       </c>
       <c r="D17" s="841"/>
-      <c r="E17" s="958"/>
+      <c r="E17" s="989"/>
       <c r="F17" s="841"/>
       <c r="G17" s="29"/>
       <c r="H17" s="29"/>
@@ -20778,10 +20778,10 @@
       <c r="AF17" s="936"/>
     </row>
     <row r="18" spans="1:32" s="1" customFormat="1" ht="53.25" customHeight="1">
-      <c r="A18" s="951" t="s">
+      <c r="A18" s="984" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="951" t="s">
+      <c r="B18" s="984" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="839" t="s">
@@ -20844,8 +20844,8 @@
       <c r="AF18" s="936"/>
     </row>
     <row r="19" spans="1:32" s="315" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A19" s="952"/>
-      <c r="B19" s="952"/>
+      <c r="A19" s="985"/>
+      <c r="B19" s="985"/>
       <c r="C19" s="363"/>
       <c r="D19" s="143"/>
       <c r="E19" s="363"/>
@@ -20876,13 +20876,13 @@
       <c r="AF19" s="937"/>
     </row>
     <row r="20" spans="1:32" s="1" customFormat="1" ht="87" customHeight="1">
-      <c r="A20" s="952"/>
-      <c r="B20" s="952"/>
+      <c r="A20" s="985"/>
+      <c r="B20" s="985"/>
       <c r="C20" s="363" t="s">
         <v>592</v>
       </c>
       <c r="D20" s="144"/>
-      <c r="E20" s="953"/>
+      <c r="E20" s="986"/>
       <c r="F20" s="144"/>
       <c r="G20" s="24"/>
       <c r="H20" s="867" t="s">
@@ -20927,7 +20927,7 @@
       <c r="B21" s="359"/>
       <c r="C21" s="363"/>
       <c r="D21" s="433"/>
-      <c r="E21" s="953"/>
+      <c r="E21" s="986"/>
       <c r="F21" s="433"/>
       <c r="G21" s="30"/>
       <c r="H21" s="30"/>
@@ -20959,7 +20959,7 @@
       <c r="B22" s="359"/>
       <c r="C22" s="363"/>
       <c r="D22" s="433"/>
-      <c r="E22" s="953"/>
+      <c r="E22" s="986"/>
       <c r="F22" s="433"/>
       <c r="G22" s="30"/>
       <c r="H22" s="30"/>
@@ -20991,7 +20991,7 @@
       <c r="B23" s="357"/>
       <c r="C23" s="362"/>
       <c r="D23" s="433"/>
-      <c r="E23" s="954"/>
+      <c r="E23" s="987"/>
       <c r="F23" s="433"/>
       <c r="G23" s="26"/>
       <c r="H23" s="26"/>
@@ -21019,17 +21019,17 @@
       <c r="AF23" s="937"/>
     </row>
     <row r="24" spans="1:32" s="1" customFormat="1" ht="96" customHeight="1">
-      <c r="A24" s="979" t="s">
+      <c r="A24" s="967" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="981" t="s">
+      <c r="B24" s="969" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="961" t="s">
+      <c r="C24" s="975" t="s">
         <v>501</v>
       </c>
       <c r="D24" s="143"/>
-      <c r="E24" s="961"/>
+      <c r="E24" s="975"/>
       <c r="F24" s="143"/>
       <c r="G24" s="30" t="s">
         <v>10</v>
@@ -21060,7 +21060,7 @@
         <v>294</v>
       </c>
       <c r="S24" s="426"/>
-      <c r="T24" s="962" t="s">
+      <c r="T24" s="976" t="s">
         <v>475</v>
       </c>
       <c r="V24" s="429" t="s">
@@ -21085,11 +21085,11 @@
       <c r="AF24" s="937"/>
     </row>
     <row r="25" spans="1:32" s="1" customFormat="1" ht="44.25" customHeight="1">
-      <c r="A25" s="980"/>
-      <c r="B25" s="982"/>
-      <c r="C25" s="956"/>
+      <c r="A25" s="968"/>
+      <c r="B25" s="970"/>
+      <c r="C25" s="973"/>
       <c r="D25" s="143"/>
-      <c r="E25" s="956"/>
+      <c r="E25" s="973"/>
       <c r="F25" s="143"/>
       <c r="G25" s="30"/>
       <c r="H25" s="30"/>
@@ -21104,7 +21104,7 @@
         <v>555</v>
       </c>
       <c r="S25" s="426"/>
-      <c r="T25" s="963"/>
+      <c r="T25" s="977"/>
       <c r="V25" s="429"/>
       <c r="W25" s="315"/>
       <c r="X25" s="590" t="s">
@@ -21139,7 +21139,7 @@
         <v>502</v>
       </c>
       <c r="S26" s="426"/>
-      <c r="T26" s="964"/>
+      <c r="T26" s="978"/>
       <c r="V26" s="429"/>
       <c r="X26" s="590" t="s">
         <v>612</v>
@@ -21158,11 +21158,11 @@
       <c r="B27" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="959" t="s">
+      <c r="C27" s="971" t="s">
         <v>889</v>
       </c>
       <c r="D27" s="145"/>
-      <c r="E27" s="968"/>
+      <c r="E27" s="982"/>
       <c r="F27" s="145"/>
       <c r="G27" s="915">
         <v>3</v>
@@ -21220,9 +21220,9 @@
     <row r="28" spans="1:32" s="1" customFormat="1" ht="54.75" customHeight="1">
       <c r="A28" s="25"/>
       <c r="B28" s="34"/>
-      <c r="C28" s="960"/>
+      <c r="C28" s="972"/>
       <c r="D28" s="146"/>
-      <c r="E28" s="969"/>
+      <c r="E28" s="983"/>
       <c r="F28" s="146"/>
       <c r="G28" s="25"/>
       <c r="H28" s="25"/>
@@ -21255,9 +21255,9 @@
     <row r="29" spans="1:32" s="1" customFormat="1" ht="106.5" customHeight="1">
       <c r="A29" s="292"/>
       <c r="B29" s="34"/>
-      <c r="C29" s="960"/>
+      <c r="C29" s="972"/>
       <c r="D29" s="146"/>
-      <c r="E29" s="969"/>
+      <c r="E29" s="983"/>
       <c r="F29" s="146"/>
       <c r="G29" s="299"/>
       <c r="H29" s="299"/>
@@ -22104,7 +22104,7 @@
       <c r="AF43" s="937"/>
     </row>
     <row r="44" spans="1:32" s="1" customFormat="1" ht="62.25" customHeight="1">
-      <c r="A44" s="970" t="s">
+      <c r="A44" s="958" t="s">
         <v>812</v>
       </c>
       <c r="B44" s="374" t="s">
@@ -22158,7 +22158,7 @@
       <c r="AF44" s="937"/>
     </row>
     <row r="45" spans="1:32" s="1" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A45" s="971"/>
+      <c r="A45" s="959"/>
       <c r="B45" s="289"/>
       <c r="C45" s="319" t="s">
         <v>379</v>
@@ -22207,7 +22207,7 @@
       <c r="AF45" s="937"/>
     </row>
     <row r="46" spans="1:32" s="1" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A46" s="971"/>
+      <c r="A46" s="959"/>
       <c r="B46" s="289"/>
       <c r="C46" s="319" t="s">
         <v>380</v>
@@ -22826,10 +22826,10 @@
       <c r="AF58" s="937"/>
     </row>
     <row r="59" spans="1:32" s="1" customFormat="1" ht="67.5" customHeight="1">
-      <c r="A59" s="973" t="s">
+      <c r="A59" s="961" t="s">
         <v>573</v>
       </c>
-      <c r="B59" s="976" t="s">
+      <c r="B59" s="964" t="s">
         <v>211</v>
       </c>
       <c r="C59" s="455" t="s">
@@ -22893,8 +22893,8 @@
       <c r="AF59" s="937"/>
     </row>
     <row r="60" spans="1:32" s="315" customFormat="1" ht="33" customHeight="1">
-      <c r="A60" s="974"/>
-      <c r="B60" s="977"/>
+      <c r="A60" s="962"/>
+      <c r="B60" s="965"/>
       <c r="C60" s="457"/>
       <c r="D60" s="454"/>
       <c r="E60" s="457"/>
@@ -22929,8 +22929,8 @@
       <c r="AF60" s="937"/>
     </row>
     <row r="61" spans="1:32" s="315" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A61" s="974"/>
-      <c r="B61" s="977"/>
+      <c r="A61" s="962"/>
+      <c r="B61" s="965"/>
       <c r="C61" s="456" t="s">
         <v>574</v>
       </c>
@@ -22951,7 +22951,7 @@
         <v>579</v>
       </c>
       <c r="S61" s="426"/>
-      <c r="T61" s="965" t="s">
+      <c r="T61" s="979" t="s">
         <v>385</v>
       </c>
       <c r="V61" s="324"/>
@@ -22964,8 +22964,8 @@
       <c r="AF61" s="937"/>
     </row>
     <row r="62" spans="1:32" s="1" customFormat="1">
-      <c r="A62" s="974"/>
-      <c r="B62" s="977"/>
+      <c r="A62" s="962"/>
+      <c r="B62" s="965"/>
       <c r="C62" s="319" t="s">
         <v>386</v>
       </c>
@@ -22986,7 +22986,7 @@
         <v>386</v>
       </c>
       <c r="S62" s="426"/>
-      <c r="T62" s="966"/>
+      <c r="T62" s="980"/>
       <c r="V62" s="324"/>
       <c r="W62" s="315"/>
       <c r="X62" s="590" t="s">
@@ -23002,8 +23002,8 @@
       <c r="AF62" s="937"/>
     </row>
     <row r="63" spans="1:32" s="315" customFormat="1">
-      <c r="A63" s="974"/>
-      <c r="B63" s="977"/>
+      <c r="A63" s="962"/>
+      <c r="B63" s="965"/>
       <c r="C63" s="319" t="s">
         <v>575</v>
       </c>
@@ -23024,7 +23024,7 @@
         <v>575</v>
       </c>
       <c r="S63" s="426"/>
-      <c r="T63" s="966"/>
+      <c r="T63" s="980"/>
       <c r="V63" s="324"/>
       <c r="X63" s="590" t="s">
         <v>612</v>
@@ -23037,8 +23037,8 @@
       <c r="AF63" s="937"/>
     </row>
     <row r="64" spans="1:32" s="315" customFormat="1">
-      <c r="A64" s="974"/>
-      <c r="B64" s="977"/>
+      <c r="A64" s="962"/>
+      <c r="B64" s="965"/>
       <c r="C64" s="702" t="s">
         <v>576</v>
       </c>
@@ -23059,7 +23059,7 @@
         <v>576</v>
       </c>
       <c r="S64" s="426"/>
-      <c r="T64" s="966"/>
+      <c r="T64" s="980"/>
       <c r="V64" s="707"/>
       <c r="X64" s="590" t="s">
         <v>612</v>
@@ -23072,8 +23072,8 @@
       <c r="AF64" s="937"/>
     </row>
     <row r="65" spans="1:32" s="315" customFormat="1">
-      <c r="A65" s="974"/>
-      <c r="B65" s="977"/>
+      <c r="A65" s="962"/>
+      <c r="B65" s="965"/>
       <c r="C65" s="319" t="s">
         <v>387</v>
       </c>
@@ -23094,7 +23094,7 @@
         <v>387</v>
       </c>
       <c r="S65" s="426"/>
-      <c r="T65" s="966"/>
+      <c r="T65" s="980"/>
       <c r="V65" s="348"/>
       <c r="X65" s="590" t="s">
         <v>612</v>
@@ -23107,8 +23107,8 @@
       <c r="AF65" s="937"/>
     </row>
     <row r="66" spans="1:32" s="315" customFormat="1">
-      <c r="A66" s="974"/>
-      <c r="B66" s="977"/>
+      <c r="A66" s="962"/>
+      <c r="B66" s="965"/>
       <c r="C66" s="319" t="s">
         <v>500</v>
       </c>
@@ -23129,7 +23129,7 @@
         <v>500</v>
       </c>
       <c r="S66" s="426"/>
-      <c r="T66" s="966"/>
+      <c r="T66" s="980"/>
       <c r="V66" s="348"/>
       <c r="X66" s="590" t="s">
         <v>612</v>
@@ -23142,8 +23142,8 @@
       <c r="AF66" s="937"/>
     </row>
     <row r="67" spans="1:32" s="315" customFormat="1">
-      <c r="A67" s="974"/>
-      <c r="B67" s="977"/>
+      <c r="A67" s="962"/>
+      <c r="B67" s="965"/>
       <c r="C67" s="319" t="s">
         <v>388</v>
       </c>
@@ -23164,7 +23164,7 @@
         <v>388</v>
       </c>
       <c r="S67" s="426"/>
-      <c r="T67" s="966"/>
+      <c r="T67" s="980"/>
       <c r="V67" s="348"/>
       <c r="X67" s="590" t="s">
         <v>612</v>
@@ -23177,8 +23177,8 @@
       <c r="AF67" s="937"/>
     </row>
     <row r="68" spans="1:32" s="315" customFormat="1">
-      <c r="A68" s="974"/>
-      <c r="B68" s="977"/>
+      <c r="A68" s="962"/>
+      <c r="B68" s="965"/>
       <c r="C68" s="319" t="s">
         <v>389</v>
       </c>
@@ -23199,7 +23199,7 @@
         <v>389</v>
       </c>
       <c r="S68" s="426"/>
-      <c r="T68" s="966"/>
+      <c r="T68" s="980"/>
       <c r="V68" s="348"/>
       <c r="X68" s="590" t="s">
         <v>612</v>
@@ -23212,8 +23212,8 @@
       <c r="AF68" s="937"/>
     </row>
     <row r="69" spans="1:32" s="315" customFormat="1" ht="45" customHeight="1">
-      <c r="A69" s="974"/>
-      <c r="B69" s="977"/>
+      <c r="A69" s="962"/>
+      <c r="B69" s="965"/>
       <c r="C69" s="319" t="s">
         <v>390</v>
       </c>
@@ -23234,7 +23234,7 @@
         <v>391</v>
       </c>
       <c r="S69" s="426"/>
-      <c r="T69" s="966"/>
+      <c r="T69" s="980"/>
       <c r="V69" s="348"/>
       <c r="X69" s="590" t="s">
         <v>612</v>
@@ -23247,8 +23247,8 @@
       <c r="AF69" s="937"/>
     </row>
     <row r="70" spans="1:32" s="315" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A70" s="974"/>
-      <c r="B70" s="977"/>
+      <c r="A70" s="962"/>
+      <c r="B70" s="965"/>
       <c r="C70" s="319" t="s">
         <v>392</v>
       </c>
@@ -23269,7 +23269,7 @@
         <v>392</v>
       </c>
       <c r="S70" s="426"/>
-      <c r="T70" s="966"/>
+      <c r="T70" s="980"/>
       <c r="V70" s="348"/>
       <c r="X70" s="590" t="s">
         <v>612</v>
@@ -23282,8 +23282,8 @@
       <c r="AF70" s="937"/>
     </row>
     <row r="71" spans="1:32" s="1" customFormat="1">
-      <c r="A71" s="974"/>
-      <c r="B71" s="977"/>
+      <c r="A71" s="962"/>
+      <c r="B71" s="965"/>
       <c r="C71" s="319" t="s">
         <v>577</v>
       </c>
@@ -23304,7 +23304,7 @@
         <v>577</v>
       </c>
       <c r="S71" s="426"/>
-      <c r="T71" s="966"/>
+      <c r="T71" s="980"/>
       <c r="V71" s="324"/>
       <c r="W71" s="315"/>
       <c r="X71" s="590" t="s">
@@ -23320,8 +23320,8 @@
       <c r="AF71" s="937"/>
     </row>
     <row r="72" spans="1:32" s="1" customFormat="1">
-      <c r="A72" s="974"/>
-      <c r="B72" s="977"/>
+      <c r="A72" s="962"/>
+      <c r="B72" s="965"/>
       <c r="C72" s="319" t="s">
         <v>578</v>
       </c>
@@ -23342,7 +23342,7 @@
         <v>578</v>
       </c>
       <c r="S72" s="426"/>
-      <c r="T72" s="966"/>
+      <c r="T72" s="980"/>
       <c r="V72" s="324"/>
       <c r="W72" s="315"/>
       <c r="X72" s="590" t="s">
@@ -23358,8 +23358,8 @@
       <c r="AF72" s="937"/>
     </row>
     <row r="73" spans="1:32" s="1" customFormat="1">
-      <c r="A73" s="974"/>
-      <c r="B73" s="977"/>
+      <c r="A73" s="962"/>
+      <c r="B73" s="965"/>
       <c r="C73" s="319" t="s">
         <v>393</v>
       </c>
@@ -23380,7 +23380,7 @@
         <v>393</v>
       </c>
       <c r="S73" s="426"/>
-      <c r="T73" s="966"/>
+      <c r="T73" s="980"/>
       <c r="V73" s="324"/>
       <c r="W73" s="315"/>
       <c r="X73" s="590" t="s">
@@ -23396,8 +23396,8 @@
       <c r="AF73" s="937"/>
     </row>
     <row r="74" spans="1:32" s="1" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A74" s="974"/>
-      <c r="B74" s="977"/>
+      <c r="A74" s="962"/>
+      <c r="B74" s="965"/>
       <c r="C74" s="319" t="s">
         <v>546</v>
       </c>
@@ -23418,7 +23418,7 @@
         <v>546</v>
       </c>
       <c r="S74" s="426"/>
-      <c r="T74" s="966"/>
+      <c r="T74" s="980"/>
       <c r="V74" s="324"/>
       <c r="W74" s="315"/>
       <c r="X74" s="590" t="s">
@@ -23434,8 +23434,8 @@
       <c r="AF74" s="937"/>
     </row>
     <row r="75" spans="1:32" s="315" customFormat="1" ht="22.8">
-      <c r="A75" s="974"/>
-      <c r="B75" s="977"/>
+      <c r="A75" s="962"/>
+      <c r="B75" s="965"/>
       <c r="C75" s="815" t="s">
         <v>813</v>
       </c>
@@ -23468,7 +23468,7 @@
         <v>813</v>
       </c>
       <c r="S75" s="426"/>
-      <c r="T75" s="967"/>
+      <c r="T75" s="981"/>
       <c r="V75" s="324"/>
       <c r="X75" s="590" t="s">
         <v>612</v>
@@ -23481,8 +23481,8 @@
       <c r="AF75" s="937"/>
     </row>
     <row r="76" spans="1:32" s="315" customFormat="1" ht="61.5" customHeight="1">
-      <c r="A76" s="974"/>
-      <c r="B76" s="977"/>
+      <c r="A76" s="962"/>
+      <c r="B76" s="965"/>
       <c r="C76" s="815" t="s">
         <v>814</v>
       </c>
@@ -23530,8 +23530,8 @@
       <c r="AF76" s="937"/>
     </row>
     <row r="77" spans="1:32" s="1" customFormat="1" ht="150" customHeight="1">
-      <c r="A77" s="974"/>
-      <c r="B77" s="977"/>
+      <c r="A77" s="962"/>
+      <c r="B77" s="965"/>
       <c r="C77" s="815" t="s">
         <v>869</v>
       </c>
@@ -23584,8 +23584,8 @@
       <c r="AF77" s="937"/>
     </row>
     <row r="78" spans="1:32" s="1" customFormat="1" ht="121.5" customHeight="1">
-      <c r="A78" s="975"/>
-      <c r="B78" s="978"/>
+      <c r="A78" s="963"/>
+      <c r="B78" s="966"/>
       <c r="C78" s="815" t="s">
         <v>870</v>
       </c>
@@ -23622,10 +23622,10 @@
       <c r="AF78" s="937"/>
     </row>
     <row r="79" spans="1:32" s="1" customFormat="1" ht="60" customHeight="1">
-      <c r="A79" s="970" t="s">
+      <c r="A79" s="958" t="s">
         <v>228</v>
       </c>
-      <c r="B79" s="972" t="s">
+      <c r="B79" s="960" t="s">
         <v>212</v>
       </c>
       <c r="C79" s="326" t="s">
@@ -23676,8 +23676,8 @@
       <c r="AF79" s="937"/>
     </row>
     <row r="80" spans="1:32" s="315" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A80" s="971"/>
-      <c r="B80" s="972"/>
+      <c r="A80" s="959"/>
+      <c r="B80" s="960"/>
       <c r="C80" s="326" t="s">
         <v>598</v>
       </c>
@@ -23724,8 +23724,8 @@
       <c r="AF80" s="937"/>
     </row>
     <row r="81" spans="1:32" s="276" customFormat="1" ht="126" customHeight="1">
-      <c r="A81" s="971"/>
-      <c r="B81" s="972"/>
+      <c r="A81" s="959"/>
+      <c r="B81" s="960"/>
       <c r="C81" s="326" t="s">
         <v>832</v>
       </c>
@@ -23773,8 +23773,8 @@
       <c r="AF81" s="937"/>
     </row>
     <row r="82" spans="1:32" s="315" customFormat="1" ht="69" customHeight="1">
-      <c r="A82" s="971"/>
-      <c r="B82" s="972"/>
+      <c r="A82" s="959"/>
+      <c r="B82" s="960"/>
       <c r="C82" s="326" t="s">
         <v>580</v>
       </c>
@@ -23820,8 +23820,8 @@
       <c r="AF82" s="937"/>
     </row>
     <row r="83" spans="1:32" s="315" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A83" s="971"/>
-      <c r="B83" s="972"/>
+      <c r="A83" s="959"/>
+      <c r="B83" s="960"/>
       <c r="C83" s="319" t="s">
         <v>394</v>
       </c>
@@ -23867,8 +23867,8 @@
       <c r="AF83" s="937"/>
     </row>
     <row r="84" spans="1:32" s="315" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A84" s="971"/>
-      <c r="B84" s="972"/>
+      <c r="A84" s="959"/>
+      <c r="B84" s="960"/>
       <c r="C84" s="319" t="s">
         <v>664</v>
       </c>
@@ -23916,8 +23916,8 @@
       <c r="AF84" s="937"/>
     </row>
     <row r="85" spans="1:32" s="276" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A85" s="971"/>
-      <c r="B85" s="972"/>
+      <c r="A85" s="959"/>
+      <c r="B85" s="960"/>
       <c r="C85" s="326" t="s">
         <v>396</v>
       </c>
@@ -24916,27 +24916,6 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="A79:A85"/>
-    <mergeCell ref="B79:B85"/>
-    <mergeCell ref="A59:A78"/>
-    <mergeCell ref="B59:B78"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="T24:T26"/>
-    <mergeCell ref="T61:T75"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="E27:E29"/>
     <mergeCell ref="AD1:AD2"/>
     <mergeCell ref="AF1:AF2"/>
     <mergeCell ref="A7:A8"/>
@@ -24953,6 +24932,27 @@
     <mergeCell ref="G1:L1"/>
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="N1:N2"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="T24:T26"/>
+    <mergeCell ref="T61:T75"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="A79:A85"/>
+    <mergeCell ref="B79:B85"/>
+    <mergeCell ref="A59:A78"/>
+    <mergeCell ref="B59:B78"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="X1:X2"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7 G89:M93 E86:E88 R83:R84 C33:M39 C12:D24 C40:C41 G31:M32 E24 R62:R78 E12:E20 F12:F24 R33:R38 G44:M49 E47 C83:C84 C59:F78 G79:M85 G27:M27 C7:F11 G59:M61 D40:M43 C31:F31 A59:A61" xr:uid="{00000000-0002-0000-0500-000000000000}">
@@ -25034,44 +25034,44 @@
         <v>191</v>
       </c>
       <c r="F1" s="271"/>
-      <c r="G1" s="944" t="s">
+      <c r="G1" s="951" t="s">
         <v>744</v>
       </c>
-      <c r="H1" s="944"/>
-      <c r="I1" s="944"/>
-      <c r="J1" s="944"/>
-      <c r="K1" s="944"/>
-      <c r="L1" s="944"/>
+      <c r="H1" s="951"/>
+      <c r="I1" s="951"/>
+      <c r="J1" s="951"/>
+      <c r="K1" s="951"/>
+      <c r="L1" s="951"/>
       <c r="M1" s="128"/>
-      <c r="N1" s="943" t="s">
+      <c r="N1" s="950" t="s">
         <v>190</v>
       </c>
-      <c r="P1" s="943" t="s">
+      <c r="P1" s="950" t="s">
         <v>194</v>
       </c>
-      <c r="R1" s="943" t="s">
+      <c r="R1" s="950" t="s">
         <v>219</v>
       </c>
-      <c r="T1" s="943" t="s">
+      <c r="T1" s="950" t="s">
         <v>242</v>
       </c>
-      <c r="V1" s="943" t="s">
+      <c r="V1" s="950" t="s">
         <v>243</v>
       </c>
-      <c r="X1" s="943" t="s">
+      <c r="X1" s="950" t="s">
         <v>220</v>
       </c>
-      <c r="Z1" s="943" t="s">
+      <c r="Z1" s="950" t="s">
         <v>244</v>
       </c>
-      <c r="AB1" s="945" t="s">
+      <c r="AB1" s="952" t="s">
         <v>740</v>
       </c>
       <c r="AC1" s="123"/>
-      <c r="AE1" s="940" t="s">
+      <c r="AE1" s="947" t="s">
         <v>989</v>
       </c>
-      <c r="AG1" s="941" t="s">
+      <c r="AG1" s="948" t="s">
         <v>990</v>
       </c>
     </row>
@@ -25101,17 +25101,17 @@
         <v>7</v>
       </c>
       <c r="M2" s="129"/>
-      <c r="N2" s="943"/>
-      <c r="P2" s="943"/>
-      <c r="R2" s="943"/>
-      <c r="T2" s="943"/>
-      <c r="V2" s="943"/>
-      <c r="X2" s="943"/>
-      <c r="Z2" s="943"/>
-      <c r="AB2" s="945"/>
+      <c r="N2" s="950"/>
+      <c r="P2" s="950"/>
+      <c r="R2" s="950"/>
+      <c r="T2" s="950"/>
+      <c r="V2" s="950"/>
+      <c r="X2" s="950"/>
+      <c r="Z2" s="950"/>
+      <c r="AB2" s="952"/>
       <c r="AC2" s="123"/>
-      <c r="AE2" s="940"/>
-      <c r="AG2" s="941"/>
+      <c r="AE2" s="947"/>
+      <c r="AG2" s="948"/>
     </row>
     <row r="3" spans="1:33">
       <c r="A3" s="203"/>
@@ -25129,11 +25129,11 @@
       <c r="M3" s="243"/>
     </row>
     <row r="4" spans="1:33" ht="19.5" customHeight="1">
-      <c r="A4" s="984" t="s">
+      <c r="A4" s="993" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="984"/>
-      <c r="C4" s="984"/>
+      <c r="B4" s="993"/>
+      <c r="C4" s="993"/>
       <c r="D4" s="243"/>
       <c r="E4" s="243"/>
       <c r="F4" s="243"/>
@@ -25151,9 +25151,9 @@
       <c r="AG4" s="3"/>
     </row>
     <row r="5" spans="1:33" s="1" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A5" s="983"/>
-      <c r="B5" s="983"/>
-      <c r="C5" s="983"/>
+      <c r="A5" s="992"/>
+      <c r="B5" s="992"/>
+      <c r="C5" s="992"/>
       <c r="D5" s="113"/>
       <c r="E5" s="270"/>
       <c r="F5" s="270"/>
@@ -26909,7 +26909,7 @@
         <v>283</v>
       </c>
       <c r="D40" s="183"/>
-      <c r="E40" s="985"/>
+      <c r="E40" s="990"/>
       <c r="F40" s="273"/>
       <c r="G40" s="404" t="s">
         <v>10</v>
@@ -26967,7 +26967,7 @@
         <v>414</v>
       </c>
       <c r="D41" s="273"/>
-      <c r="E41" s="955"/>
+      <c r="E41" s="974"/>
       <c r="F41" s="273"/>
       <c r="G41" s="370"/>
       <c r="H41" s="370"/>
@@ -27000,7 +27000,7 @@
         <v>415</v>
       </c>
       <c r="D42" s="273"/>
-      <c r="E42" s="955"/>
+      <c r="E42" s="974"/>
       <c r="F42" s="273"/>
       <c r="G42" s="370"/>
       <c r="H42" s="370"/>
@@ -27034,7 +27034,7 @@
         <v>658</v>
       </c>
       <c r="D43" s="273"/>
-      <c r="E43" s="986"/>
+      <c r="E43" s="991"/>
       <c r="F43" s="273"/>
       <c r="G43" s="369"/>
       <c r="H43" s="369"/>
@@ -27896,6 +27896,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="AE1:AE2"/>
+    <mergeCell ref="AG1:AG2"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="G1:L1"/>
     <mergeCell ref="E40:E43"/>
     <mergeCell ref="R1:R2"/>
     <mergeCell ref="T1:T2"/>
@@ -27903,13 +27910,6 @@
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="V1:V2"/>
-    <mergeCell ref="AE1:AE2"/>
-    <mergeCell ref="AG1:AG2"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="G1:L1"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G15:M15 G40:M44 G30:M37 E38:E39 G56:K60" xr:uid="{00000000-0002-0000-0600-000000000000}">
@@ -27992,45 +27992,45 @@
         <v>191</v>
       </c>
       <c r="F1" s="271"/>
-      <c r="G1" s="944" t="s">
+      <c r="G1" s="951" t="s">
         <v>744</v>
       </c>
-      <c r="H1" s="944"/>
-      <c r="I1" s="944"/>
-      <c r="J1" s="944"/>
-      <c r="K1" s="944"/>
-      <c r="L1" s="944"/>
+      <c r="H1" s="951"/>
+      <c r="I1" s="951"/>
+      <c r="J1" s="951"/>
+      <c r="K1" s="951"/>
+      <c r="L1" s="951"/>
       <c r="M1" s="128"/>
-      <c r="N1" s="943" t="s">
+      <c r="N1" s="950" t="s">
         <v>190</v>
       </c>
-      <c r="P1" s="943" t="s">
+      <c r="P1" s="950" t="s">
         <v>194</v>
       </c>
-      <c r="R1" s="943" t="s">
+      <c r="R1" s="950" t="s">
         <v>219</v>
       </c>
-      <c r="T1" s="943" t="s">
+      <c r="T1" s="950" t="s">
         <v>242</v>
       </c>
-      <c r="V1" s="943" t="s">
+      <c r="V1" s="950" t="s">
         <v>243</v>
       </c>
-      <c r="X1" s="943" t="s">
+      <c r="X1" s="950" t="s">
         <v>220</v>
       </c>
-      <c r="Z1" s="943" t="s">
+      <c r="Z1" s="950" t="s">
         <v>244</v>
       </c>
       <c r="AA1" s="271"/>
-      <c r="AB1" s="945" t="s">
+      <c r="AB1" s="952" t="s">
         <v>740</v>
       </c>
       <c r="AC1" s="123"/>
-      <c r="AD1" s="940" t="s">
+      <c r="AD1" s="947" t="s">
         <v>989</v>
       </c>
-      <c r="AF1" s="941" t="s">
+      <c r="AF1" s="948" t="s">
         <v>990</v>
       </c>
     </row>
@@ -28060,25 +28060,25 @@
         <v>7</v>
       </c>
       <c r="M2" s="129"/>
-      <c r="N2" s="943"/>
-      <c r="P2" s="943"/>
-      <c r="R2" s="943"/>
-      <c r="T2" s="943"/>
-      <c r="V2" s="943"/>
-      <c r="X2" s="943"/>
-      <c r="Z2" s="943"/>
+      <c r="N2" s="950"/>
+      <c r="P2" s="950"/>
+      <c r="R2" s="950"/>
+      <c r="T2" s="950"/>
+      <c r="V2" s="950"/>
+      <c r="X2" s="950"/>
+      <c r="Z2" s="950"/>
       <c r="AA2" s="271"/>
-      <c r="AB2" s="945"/>
+      <c r="AB2" s="952"/>
       <c r="AC2" s="123"/>
-      <c r="AD2" s="940"/>
-      <c r="AF2" s="941"/>
+      <c r="AD2" s="947"/>
+      <c r="AF2" s="948"/>
     </row>
     <row r="4" spans="1:32" ht="15">
-      <c r="A4" s="984" t="s">
+      <c r="A4" s="993" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="984"/>
-      <c r="C4" s="984"/>
+      <c r="B4" s="993"/>
+      <c r="C4" s="993"/>
       <c r="AD4" s="3"/>
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
@@ -28968,45 +28968,45 @@
         <v>191</v>
       </c>
       <c r="F1" s="271"/>
-      <c r="G1" s="944" t="s">
+      <c r="G1" s="951" t="s">
         <v>744</v>
       </c>
-      <c r="H1" s="944"/>
-      <c r="I1" s="944"/>
-      <c r="J1" s="944"/>
-      <c r="K1" s="944"/>
-      <c r="L1" s="944"/>
+      <c r="H1" s="951"/>
+      <c r="I1" s="951"/>
+      <c r="J1" s="951"/>
+      <c r="K1" s="951"/>
+      <c r="L1" s="951"/>
       <c r="M1" s="128"/>
-      <c r="N1" s="943" t="s">
+      <c r="N1" s="950" t="s">
         <v>190</v>
       </c>
-      <c r="P1" s="943" t="s">
+      <c r="P1" s="950" t="s">
         <v>194</v>
       </c>
-      <c r="R1" s="943" t="s">
+      <c r="R1" s="950" t="s">
         <v>219</v>
       </c>
-      <c r="T1" s="943" t="s">
+      <c r="T1" s="950" t="s">
         <v>242</v>
       </c>
-      <c r="V1" s="943" t="s">
+      <c r="V1" s="950" t="s">
         <v>243</v>
       </c>
-      <c r="X1" s="943" t="s">
+      <c r="X1" s="950" t="s">
         <v>220</v>
       </c>
-      <c r="Z1" s="943" t="s">
+      <c r="Z1" s="950" t="s">
         <v>244</v>
       </c>
       <c r="AA1" s="271"/>
-      <c r="AB1" s="945" t="s">
+      <c r="AB1" s="952" t="s">
         <v>740</v>
       </c>
       <c r="AC1" s="123"/>
-      <c r="AD1" s="940" t="s">
+      <c r="AD1" s="947" t="s">
         <v>989</v>
       </c>
-      <c r="AF1" s="941" t="s">
+      <c r="AF1" s="948" t="s">
         <v>990</v>
       </c>
     </row>
@@ -29036,24 +29036,24 @@
         <v>7</v>
       </c>
       <c r="M2" s="129"/>
-      <c r="N2" s="943"/>
-      <c r="P2" s="943"/>
-      <c r="R2" s="943"/>
-      <c r="T2" s="943"/>
-      <c r="V2" s="943"/>
-      <c r="X2" s="943"/>
-      <c r="Z2" s="943"/>
+      <c r="N2" s="950"/>
+      <c r="P2" s="950"/>
+      <c r="R2" s="950"/>
+      <c r="T2" s="950"/>
+      <c r="V2" s="950"/>
+      <c r="X2" s="950"/>
+      <c r="Z2" s="950"/>
       <c r="AA2" s="271"/>
-      <c r="AB2" s="945"/>
+      <c r="AB2" s="952"/>
       <c r="AC2" s="123"/>
-      <c r="AD2" s="940"/>
-      <c r="AF2" s="941"/>
+      <c r="AD2" s="947"/>
+      <c r="AF2" s="948"/>
     </row>
     <row r="4" spans="1:32" ht="15">
-      <c r="A4" s="984" t="s">
+      <c r="A4" s="993" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="984"/>
+      <c r="B4" s="993"/>
       <c r="AD4" s="3"/>
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>

</xml_diff>

<commit_message>
Finishing demo and exporting file with results
</commit_message>
<xml_diff>
--- a/xlsx/BMW_Sales_Standards_2016_ME.xlsx
+++ b/xlsx/BMW_Sales_Standards_2016_ME.xlsx
@@ -8043,6 +8043,63 @@
     <xf numFmtId="0" fontId="60" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="11" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -8082,62 +8139,11 @@
     <xf numFmtId="49" fontId="11" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="56" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -8145,11 +8151,23 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="60" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -8162,24 +8180,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="64" fillId="18" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -9339,11 +9339,11 @@
       <c r="AF2" s="948"/>
     </row>
     <row r="4" spans="1:32" ht="15">
-      <c r="A4" s="993" t="s">
+      <c r="A4" s="991" t="s">
         <v>96</v>
       </c>
-      <c r="B4" s="993"/>
-      <c r="C4" s="993"/>
+      <c r="B4" s="991"/>
+      <c r="C4" s="991"/>
       <c r="AD4" s="3"/>
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
@@ -10924,11 +10924,11 @@
       <c r="AF2" s="948"/>
     </row>
     <row r="4" spans="1:32" ht="15.6">
-      <c r="A4" s="998" t="s">
+      <c r="A4" s="994" t="s">
         <v>155</v>
       </c>
-      <c r="B4" s="998"/>
-      <c r="C4" s="998"/>
+      <c r="B4" s="994"/>
+      <c r="C4" s="994"/>
       <c r="AD4" s="3"/>
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
@@ -11248,34 +11248,34 @@
       <c r="AF10" s="936"/>
     </row>
     <row r="11" spans="1:32" s="1" customFormat="1" ht="191.25" customHeight="1">
-      <c r="A11" s="999" t="s">
+      <c r="A11" s="995" t="s">
         <v>107</v>
       </c>
-      <c r="B11" s="1002" t="s">
+      <c r="B11" s="998" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="994" t="s">
+      <c r="C11" s="1000" t="s">
         <v>997</v>
       </c>
       <c r="D11" s="193"/>
-      <c r="E11" s="994"/>
+      <c r="E11" s="1000"/>
       <c r="F11" s="193"/>
-      <c r="G11" s="988" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="988" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="988" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" s="988" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" s="988" t="s">
-        <v>10</v>
-      </c>
-      <c r="L11" s="988" t="s">
+      <c r="G11" s="964" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="964" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="964" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="964" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="964" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" s="964" t="s">
         <v>10</v>
       </c>
       <c r="M11" s="186"/>
@@ -11311,18 +11311,18 @@
       <c r="AF11" s="936"/>
     </row>
     <row r="12" spans="1:32" s="1" customFormat="1" ht="13.8">
-      <c r="A12" s="1000"/>
-      <c r="B12" s="960"/>
-      <c r="C12" s="995"/>
+      <c r="A12" s="996"/>
+      <c r="B12" s="979"/>
+      <c r="C12" s="1001"/>
       <c r="D12" s="193"/>
-      <c r="E12" s="995"/>
+      <c r="E12" s="1001"/>
       <c r="F12" s="193"/>
-      <c r="G12" s="997"/>
-      <c r="H12" s="997"/>
-      <c r="I12" s="997"/>
-      <c r="J12" s="997"/>
-      <c r="K12" s="997"/>
-      <c r="L12" s="997"/>
+      <c r="G12" s="1003"/>
+      <c r="H12" s="1003"/>
+      <c r="I12" s="1003"/>
+      <c r="J12" s="1003"/>
+      <c r="K12" s="1003"/>
+      <c r="L12" s="1003"/>
       <c r="M12" s="188"/>
       <c r="N12" s="256"/>
       <c r="P12" s="914"/>
@@ -11343,18 +11343,18 @@
       <c r="AF12" s="936"/>
     </row>
     <row r="13" spans="1:32" s="1" customFormat="1" ht="13.8">
-      <c r="A13" s="1000"/>
-      <c r="B13" s="960"/>
-      <c r="C13" s="995"/>
+      <c r="A13" s="996"/>
+      <c r="B13" s="979"/>
+      <c r="C13" s="1001"/>
       <c r="D13" s="193"/>
-      <c r="E13" s="995"/>
+      <c r="E13" s="1001"/>
       <c r="F13" s="193"/>
-      <c r="G13" s="997"/>
-      <c r="H13" s="997"/>
-      <c r="I13" s="997"/>
-      <c r="J13" s="997"/>
-      <c r="K13" s="997"/>
-      <c r="L13" s="997"/>
+      <c r="G13" s="1003"/>
+      <c r="H13" s="1003"/>
+      <c r="I13" s="1003"/>
+      <c r="J13" s="1003"/>
+      <c r="K13" s="1003"/>
+      <c r="L13" s="1003"/>
       <c r="M13" s="188"/>
       <c r="N13" s="256"/>
       <c r="P13" s="914"/>
@@ -11375,18 +11375,18 @@
       <c r="AF13" s="936"/>
     </row>
     <row r="14" spans="1:32" s="1" customFormat="1" ht="35.25" customHeight="1">
-      <c r="A14" s="1001"/>
-      <c r="B14" s="1003"/>
-      <c r="C14" s="996"/>
+      <c r="A14" s="997"/>
+      <c r="B14" s="999"/>
+      <c r="C14" s="1002"/>
       <c r="D14" s="193"/>
-      <c r="E14" s="996"/>
+      <c r="E14" s="1002"/>
       <c r="F14" s="193"/>
-      <c r="G14" s="989"/>
-      <c r="H14" s="989"/>
-      <c r="I14" s="989"/>
-      <c r="J14" s="989"/>
-      <c r="K14" s="989"/>
-      <c r="L14" s="989"/>
+      <c r="G14" s="965"/>
+      <c r="H14" s="965"/>
+      <c r="I14" s="965"/>
+      <c r="J14" s="965"/>
+      <c r="K14" s="965"/>
+      <c r="L14" s="965"/>
       <c r="M14" s="176"/>
       <c r="N14" s="264"/>
       <c r="P14" s="913"/>
@@ -13016,17 +13016,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="AD1:AD2"/>
-    <mergeCell ref="AF1:AF2"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="R1:R2"/>
     <mergeCell ref="T1:T2"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="K11:K14"/>
@@ -13038,6 +13027,17 @@
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="G1:L1"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="AD1:AD2"/>
+    <mergeCell ref="AF1:AF2"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="X1:X2"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:M11 G15:M22 G24:M37 G38:N38" xr:uid="{00000000-0002-0000-0A00-000000000000}">
@@ -13070,7 +13070,7 @@
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="D1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z14" sqref="Z14"/>
-      <selection pane="bottomLeft" activeCell="X7" sqref="X7"/>
+      <selection pane="bottomLeft" activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -13198,10 +13198,10 @@
       <c r="AF2" s="948"/>
     </row>
     <row r="4" spans="1:32" ht="15">
-      <c r="A4" s="993" t="s">
+      <c r="A4" s="991" t="s">
         <v>342</v>
       </c>
-      <c r="B4" s="993"/>
+      <c r="B4" s="991"/>
       <c r="AD4" s="3"/>
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
@@ -13288,7 +13288,7 @@
       <c r="Y6" s="425"/>
       <c r="Z6" s="945">
         <f>IF(OR(X6="A",X7="A",X8="A"),"",IF(OR(X6="N",X7="N",X8="N"),0,1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA6" s="315"/>
       <c r="AB6" s="800" t="s">
@@ -13324,7 +13324,7 @@
       <c r="T7" s="305"/>
       <c r="V7" s="314"/>
       <c r="X7" s="590" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="Y7" s="425"/>
       <c r="Z7" s="941"/>
@@ -13426,12 +13426,12 @@
       </c>
       <c r="W9" s="315"/>
       <c r="X9" s="590" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="Y9" s="425"/>
       <c r="Z9" s="945">
         <f>IF(OR(X9="A",X10="A"),"",IF(OR(X9="N",X10="N"),0,1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA9" s="315"/>
       <c r="AB9" s="801" t="s">
@@ -20240,17 +20240,17 @@
       <c r="AF6" s="3"/>
     </row>
     <row r="7" spans="1:32" s="1" customFormat="1" ht="115.5" customHeight="1">
-      <c r="A7" s="984" t="s">
+      <c r="A7" s="958" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="984" t="s">
+      <c r="B7" s="958" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="973" t="s">
+      <c r="C7" s="963" t="s">
         <v>763</v>
       </c>
       <c r="D7" s="142"/>
-      <c r="E7" s="973"/>
+      <c r="E7" s="963"/>
       <c r="F7" s="142"/>
       <c r="G7" s="24" t="s">
         <v>10</v>
@@ -20306,11 +20306,11 @@
       <c r="AF7" s="936"/>
     </row>
     <row r="8" spans="1:32" s="1" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A8" s="985"/>
-      <c r="B8" s="985"/>
-      <c r="C8" s="974"/>
+      <c r="A8" s="959"/>
+      <c r="B8" s="959"/>
+      <c r="C8" s="962"/>
       <c r="D8" s="143"/>
-      <c r="E8" s="974"/>
+      <c r="E8" s="962"/>
       <c r="F8" s="143"/>
       <c r="G8" s="30"/>
       <c r="H8" s="30"/>
@@ -20341,13 +20341,13 @@
       <c r="AF8" s="936"/>
     </row>
     <row r="9" spans="1:32" s="1" customFormat="1" ht="45.6">
-      <c r="A9" s="985"/>
-      <c r="B9" s="985"/>
-      <c r="C9" s="974" t="s">
+      <c r="A9" s="959"/>
+      <c r="B9" s="959"/>
+      <c r="C9" s="962" t="s">
         <v>677</v>
       </c>
       <c r="D9" s="143"/>
-      <c r="E9" s="974"/>
+      <c r="E9" s="962"/>
       <c r="F9" s="143"/>
       <c r="G9" s="30" t="s">
         <v>10</v>
@@ -20397,11 +20397,11 @@
       <c r="AF9" s="936"/>
     </row>
     <row r="10" spans="1:32" s="1" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A10" s="985"/>
-      <c r="B10" s="985"/>
-      <c r="C10" s="974"/>
+      <c r="A10" s="959"/>
+      <c r="B10" s="959"/>
+      <c r="C10" s="962"/>
       <c r="D10" s="143"/>
-      <c r="E10" s="974"/>
+      <c r="E10" s="962"/>
       <c r="F10" s="143"/>
       <c r="G10" s="30" t="s">
         <v>10</v>
@@ -20683,7 +20683,7 @@
         <v>747</v>
       </c>
       <c r="D16" s="840"/>
-      <c r="E16" s="988"/>
+      <c r="E16" s="964"/>
       <c r="F16" s="840"/>
       <c r="G16" s="868" t="s">
         <v>10</v>
@@ -20740,7 +20740,7 @@
         <v>746</v>
       </c>
       <c r="D17" s="841"/>
-      <c r="E17" s="989"/>
+      <c r="E17" s="965"/>
       <c r="F17" s="841"/>
       <c r="G17" s="29"/>
       <c r="H17" s="29"/>
@@ -20778,10 +20778,10 @@
       <c r="AF17" s="936"/>
     </row>
     <row r="18" spans="1:32" s="1" customFormat="1" ht="53.25" customHeight="1">
-      <c r="A18" s="984" t="s">
+      <c r="A18" s="958" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="984" t="s">
+      <c r="B18" s="958" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="839" t="s">
@@ -20844,8 +20844,8 @@
       <c r="AF18" s="936"/>
     </row>
     <row r="19" spans="1:32" s="315" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A19" s="985"/>
-      <c r="B19" s="985"/>
+      <c r="A19" s="959"/>
+      <c r="B19" s="959"/>
       <c r="C19" s="363"/>
       <c r="D19" s="143"/>
       <c r="E19" s="363"/>
@@ -20876,13 +20876,13 @@
       <c r="AF19" s="937"/>
     </row>
     <row r="20" spans="1:32" s="1" customFormat="1" ht="87" customHeight="1">
-      <c r="A20" s="985"/>
-      <c r="B20" s="985"/>
+      <c r="A20" s="959"/>
+      <c r="B20" s="959"/>
       <c r="C20" s="363" t="s">
         <v>592</v>
       </c>
       <c r="D20" s="144"/>
-      <c r="E20" s="986"/>
+      <c r="E20" s="960"/>
       <c r="F20" s="144"/>
       <c r="G20" s="24"/>
       <c r="H20" s="867" t="s">
@@ -20927,7 +20927,7 @@
       <c r="B21" s="359"/>
       <c r="C21" s="363"/>
       <c r="D21" s="433"/>
-      <c r="E21" s="986"/>
+      <c r="E21" s="960"/>
       <c r="F21" s="433"/>
       <c r="G21" s="30"/>
       <c r="H21" s="30"/>
@@ -20959,7 +20959,7 @@
       <c r="B22" s="359"/>
       <c r="C22" s="363"/>
       <c r="D22" s="433"/>
-      <c r="E22" s="986"/>
+      <c r="E22" s="960"/>
       <c r="F22" s="433"/>
       <c r="G22" s="30"/>
       <c r="H22" s="30"/>
@@ -20991,7 +20991,7 @@
       <c r="B23" s="357"/>
       <c r="C23" s="362"/>
       <c r="D23" s="433"/>
-      <c r="E23" s="987"/>
+      <c r="E23" s="961"/>
       <c r="F23" s="433"/>
       <c r="G23" s="26"/>
       <c r="H23" s="26"/>
@@ -21019,17 +21019,17 @@
       <c r="AF23" s="937"/>
     </row>
     <row r="24" spans="1:32" s="1" customFormat="1" ht="96" customHeight="1">
-      <c r="A24" s="967" t="s">
+      <c r="A24" s="986" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="969" t="s">
+      <c r="B24" s="988" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="975" t="s">
+      <c r="C24" s="968" t="s">
         <v>501</v>
       </c>
       <c r="D24" s="143"/>
-      <c r="E24" s="975"/>
+      <c r="E24" s="968"/>
       <c r="F24" s="143"/>
       <c r="G24" s="30" t="s">
         <v>10</v>
@@ -21060,7 +21060,7 @@
         <v>294</v>
       </c>
       <c r="S24" s="426"/>
-      <c r="T24" s="976" t="s">
+      <c r="T24" s="969" t="s">
         <v>475</v>
       </c>
       <c r="V24" s="429" t="s">
@@ -21085,11 +21085,11 @@
       <c r="AF24" s="937"/>
     </row>
     <row r="25" spans="1:32" s="1" customFormat="1" ht="44.25" customHeight="1">
-      <c r="A25" s="968"/>
-      <c r="B25" s="970"/>
-      <c r="C25" s="973"/>
+      <c r="A25" s="987"/>
+      <c r="B25" s="989"/>
+      <c r="C25" s="963"/>
       <c r="D25" s="143"/>
-      <c r="E25" s="973"/>
+      <c r="E25" s="963"/>
       <c r="F25" s="143"/>
       <c r="G25" s="30"/>
       <c r="H25" s="30"/>
@@ -21104,7 +21104,7 @@
         <v>555</v>
       </c>
       <c r="S25" s="426"/>
-      <c r="T25" s="977"/>
+      <c r="T25" s="970"/>
       <c r="V25" s="429"/>
       <c r="W25" s="315"/>
       <c r="X25" s="590" t="s">
@@ -21139,7 +21139,7 @@
         <v>502</v>
       </c>
       <c r="S26" s="426"/>
-      <c r="T26" s="978"/>
+      <c r="T26" s="971"/>
       <c r="V26" s="429"/>
       <c r="X26" s="590" t="s">
         <v>612</v>
@@ -21158,11 +21158,11 @@
       <c r="B27" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="971" t="s">
+      <c r="C27" s="966" t="s">
         <v>889</v>
       </c>
       <c r="D27" s="145"/>
-      <c r="E27" s="982"/>
+      <c r="E27" s="975"/>
       <c r="F27" s="145"/>
       <c r="G27" s="915">
         <v>3</v>
@@ -21220,9 +21220,9 @@
     <row r="28" spans="1:32" s="1" customFormat="1" ht="54.75" customHeight="1">
       <c r="A28" s="25"/>
       <c r="B28" s="34"/>
-      <c r="C28" s="972"/>
+      <c r="C28" s="967"/>
       <c r="D28" s="146"/>
-      <c r="E28" s="983"/>
+      <c r="E28" s="976"/>
       <c r="F28" s="146"/>
       <c r="G28" s="25"/>
       <c r="H28" s="25"/>
@@ -21255,9 +21255,9 @@
     <row r="29" spans="1:32" s="1" customFormat="1" ht="106.5" customHeight="1">
       <c r="A29" s="292"/>
       <c r="B29" s="34"/>
-      <c r="C29" s="972"/>
+      <c r="C29" s="967"/>
       <c r="D29" s="146"/>
-      <c r="E29" s="983"/>
+      <c r="E29" s="976"/>
       <c r="F29" s="146"/>
       <c r="G29" s="299"/>
       <c r="H29" s="299"/>
@@ -22104,7 +22104,7 @@
       <c r="AF43" s="937"/>
     </row>
     <row r="44" spans="1:32" s="1" customFormat="1" ht="62.25" customHeight="1">
-      <c r="A44" s="958" t="s">
+      <c r="A44" s="977" t="s">
         <v>812</v>
       </c>
       <c r="B44" s="374" t="s">
@@ -22158,7 +22158,7 @@
       <c r="AF44" s="937"/>
     </row>
     <row r="45" spans="1:32" s="1" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A45" s="959"/>
+      <c r="A45" s="978"/>
       <c r="B45" s="289"/>
       <c r="C45" s="319" t="s">
         <v>379</v>
@@ -22207,7 +22207,7 @@
       <c r="AF45" s="937"/>
     </row>
     <row r="46" spans="1:32" s="1" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A46" s="959"/>
+      <c r="A46" s="978"/>
       <c r="B46" s="289"/>
       <c r="C46" s="319" t="s">
         <v>380</v>
@@ -22826,10 +22826,10 @@
       <c r="AF58" s="937"/>
     </row>
     <row r="59" spans="1:32" s="1" customFormat="1" ht="67.5" customHeight="1">
-      <c r="A59" s="961" t="s">
+      <c r="A59" s="980" t="s">
         <v>573</v>
       </c>
-      <c r="B59" s="964" t="s">
+      <c r="B59" s="983" t="s">
         <v>211</v>
       </c>
       <c r="C59" s="455" t="s">
@@ -22893,8 +22893,8 @@
       <c r="AF59" s="937"/>
     </row>
     <row r="60" spans="1:32" s="315" customFormat="1" ht="33" customHeight="1">
-      <c r="A60" s="962"/>
-      <c r="B60" s="965"/>
+      <c r="A60" s="981"/>
+      <c r="B60" s="984"/>
       <c r="C60" s="457"/>
       <c r="D60" s="454"/>
       <c r="E60" s="457"/>
@@ -22929,8 +22929,8 @@
       <c r="AF60" s="937"/>
     </row>
     <row r="61" spans="1:32" s="315" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A61" s="962"/>
-      <c r="B61" s="965"/>
+      <c r="A61" s="981"/>
+      <c r="B61" s="984"/>
       <c r="C61" s="456" t="s">
         <v>574</v>
       </c>
@@ -22951,7 +22951,7 @@
         <v>579</v>
       </c>
       <c r="S61" s="426"/>
-      <c r="T61" s="979" t="s">
+      <c r="T61" s="972" t="s">
         <v>385</v>
       </c>
       <c r="V61" s="324"/>
@@ -22964,8 +22964,8 @@
       <c r="AF61" s="937"/>
     </row>
     <row r="62" spans="1:32" s="1" customFormat="1">
-      <c r="A62" s="962"/>
-      <c r="B62" s="965"/>
+      <c r="A62" s="981"/>
+      <c r="B62" s="984"/>
       <c r="C62" s="319" t="s">
         <v>386</v>
       </c>
@@ -22986,7 +22986,7 @@
         <v>386</v>
       </c>
       <c r="S62" s="426"/>
-      <c r="T62" s="980"/>
+      <c r="T62" s="973"/>
       <c r="V62" s="324"/>
       <c r="W62" s="315"/>
       <c r="X62" s="590" t="s">
@@ -23002,8 +23002,8 @@
       <c r="AF62" s="937"/>
     </row>
     <row r="63" spans="1:32" s="315" customFormat="1">
-      <c r="A63" s="962"/>
-      <c r="B63" s="965"/>
+      <c r="A63" s="981"/>
+      <c r="B63" s="984"/>
       <c r="C63" s="319" t="s">
         <v>575</v>
       </c>
@@ -23024,7 +23024,7 @@
         <v>575</v>
       </c>
       <c r="S63" s="426"/>
-      <c r="T63" s="980"/>
+      <c r="T63" s="973"/>
       <c r="V63" s="324"/>
       <c r="X63" s="590" t="s">
         <v>612</v>
@@ -23037,8 +23037,8 @@
       <c r="AF63" s="937"/>
     </row>
     <row r="64" spans="1:32" s="315" customFormat="1">
-      <c r="A64" s="962"/>
-      <c r="B64" s="965"/>
+      <c r="A64" s="981"/>
+      <c r="B64" s="984"/>
       <c r="C64" s="702" t="s">
         <v>576</v>
       </c>
@@ -23059,7 +23059,7 @@
         <v>576</v>
       </c>
       <c r="S64" s="426"/>
-      <c r="T64" s="980"/>
+      <c r="T64" s="973"/>
       <c r="V64" s="707"/>
       <c r="X64" s="590" t="s">
         <v>612</v>
@@ -23072,8 +23072,8 @@
       <c r="AF64" s="937"/>
     </row>
     <row r="65" spans="1:32" s="315" customFormat="1">
-      <c r="A65" s="962"/>
-      <c r="B65" s="965"/>
+      <c r="A65" s="981"/>
+      <c r="B65" s="984"/>
       <c r="C65" s="319" t="s">
         <v>387</v>
       </c>
@@ -23094,7 +23094,7 @@
         <v>387</v>
       </c>
       <c r="S65" s="426"/>
-      <c r="T65" s="980"/>
+      <c r="T65" s="973"/>
       <c r="V65" s="348"/>
       <c r="X65" s="590" t="s">
         <v>612</v>
@@ -23107,8 +23107,8 @@
       <c r="AF65" s="937"/>
     </row>
     <row r="66" spans="1:32" s="315" customFormat="1">
-      <c r="A66" s="962"/>
-      <c r="B66" s="965"/>
+      <c r="A66" s="981"/>
+      <c r="B66" s="984"/>
       <c r="C66" s="319" t="s">
         <v>500</v>
       </c>
@@ -23129,7 +23129,7 @@
         <v>500</v>
       </c>
       <c r="S66" s="426"/>
-      <c r="T66" s="980"/>
+      <c r="T66" s="973"/>
       <c r="V66" s="348"/>
       <c r="X66" s="590" t="s">
         <v>612</v>
@@ -23142,8 +23142,8 @@
       <c r="AF66" s="937"/>
     </row>
     <row r="67" spans="1:32" s="315" customFormat="1">
-      <c r="A67" s="962"/>
-      <c r="B67" s="965"/>
+      <c r="A67" s="981"/>
+      <c r="B67" s="984"/>
       <c r="C67" s="319" t="s">
         <v>388</v>
       </c>
@@ -23164,7 +23164,7 @@
         <v>388</v>
       </c>
       <c r="S67" s="426"/>
-      <c r="T67" s="980"/>
+      <c r="T67" s="973"/>
       <c r="V67" s="348"/>
       <c r="X67" s="590" t="s">
         <v>612</v>
@@ -23177,8 +23177,8 @@
       <c r="AF67" s="937"/>
     </row>
     <row r="68" spans="1:32" s="315" customFormat="1">
-      <c r="A68" s="962"/>
-      <c r="B68" s="965"/>
+      <c r="A68" s="981"/>
+      <c r="B68" s="984"/>
       <c r="C68" s="319" t="s">
         <v>389</v>
       </c>
@@ -23199,7 +23199,7 @@
         <v>389</v>
       </c>
       <c r="S68" s="426"/>
-      <c r="T68" s="980"/>
+      <c r="T68" s="973"/>
       <c r="V68" s="348"/>
       <c r="X68" s="590" t="s">
         <v>612</v>
@@ -23212,8 +23212,8 @@
       <c r="AF68" s="937"/>
     </row>
     <row r="69" spans="1:32" s="315" customFormat="1" ht="45" customHeight="1">
-      <c r="A69" s="962"/>
-      <c r="B69" s="965"/>
+      <c r="A69" s="981"/>
+      <c r="B69" s="984"/>
       <c r="C69" s="319" t="s">
         <v>390</v>
       </c>
@@ -23234,7 +23234,7 @@
         <v>391</v>
       </c>
       <c r="S69" s="426"/>
-      <c r="T69" s="980"/>
+      <c r="T69" s="973"/>
       <c r="V69" s="348"/>
       <c r="X69" s="590" t="s">
         <v>612</v>
@@ -23247,8 +23247,8 @@
       <c r="AF69" s="937"/>
     </row>
     <row r="70" spans="1:32" s="315" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A70" s="962"/>
-      <c r="B70" s="965"/>
+      <c r="A70" s="981"/>
+      <c r="B70" s="984"/>
       <c r="C70" s="319" t="s">
         <v>392</v>
       </c>
@@ -23269,7 +23269,7 @@
         <v>392</v>
       </c>
       <c r="S70" s="426"/>
-      <c r="T70" s="980"/>
+      <c r="T70" s="973"/>
       <c r="V70" s="348"/>
       <c r="X70" s="590" t="s">
         <v>612</v>
@@ -23282,8 +23282,8 @@
       <c r="AF70" s="937"/>
     </row>
     <row r="71" spans="1:32" s="1" customFormat="1">
-      <c r="A71" s="962"/>
-      <c r="B71" s="965"/>
+      <c r="A71" s="981"/>
+      <c r="B71" s="984"/>
       <c r="C71" s="319" t="s">
         <v>577</v>
       </c>
@@ -23304,7 +23304,7 @@
         <v>577</v>
       </c>
       <c r="S71" s="426"/>
-      <c r="T71" s="980"/>
+      <c r="T71" s="973"/>
       <c r="V71" s="324"/>
       <c r="W71" s="315"/>
       <c r="X71" s="590" t="s">
@@ -23320,8 +23320,8 @@
       <c r="AF71" s="937"/>
     </row>
     <row r="72" spans="1:32" s="1" customFormat="1">
-      <c r="A72" s="962"/>
-      <c r="B72" s="965"/>
+      <c r="A72" s="981"/>
+      <c r="B72" s="984"/>
       <c r="C72" s="319" t="s">
         <v>578</v>
       </c>
@@ -23342,7 +23342,7 @@
         <v>578</v>
       </c>
       <c r="S72" s="426"/>
-      <c r="T72" s="980"/>
+      <c r="T72" s="973"/>
       <c r="V72" s="324"/>
       <c r="W72" s="315"/>
       <c r="X72" s="590" t="s">
@@ -23358,8 +23358,8 @@
       <c r="AF72" s="937"/>
     </row>
     <row r="73" spans="1:32" s="1" customFormat="1">
-      <c r="A73" s="962"/>
-      <c r="B73" s="965"/>
+      <c r="A73" s="981"/>
+      <c r="B73" s="984"/>
       <c r="C73" s="319" t="s">
         <v>393</v>
       </c>
@@ -23380,7 +23380,7 @@
         <v>393</v>
       </c>
       <c r="S73" s="426"/>
-      <c r="T73" s="980"/>
+      <c r="T73" s="973"/>
       <c r="V73" s="324"/>
       <c r="W73" s="315"/>
       <c r="X73" s="590" t="s">
@@ -23396,8 +23396,8 @@
       <c r="AF73" s="937"/>
     </row>
     <row r="74" spans="1:32" s="1" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A74" s="962"/>
-      <c r="B74" s="965"/>
+      <c r="A74" s="981"/>
+      <c r="B74" s="984"/>
       <c r="C74" s="319" t="s">
         <v>546</v>
       </c>
@@ -23418,7 +23418,7 @@
         <v>546</v>
       </c>
       <c r="S74" s="426"/>
-      <c r="T74" s="980"/>
+      <c r="T74" s="973"/>
       <c r="V74" s="324"/>
       <c r="W74" s="315"/>
       <c r="X74" s="590" t="s">
@@ -23434,8 +23434,8 @@
       <c r="AF74" s="937"/>
     </row>
     <row r="75" spans="1:32" s="315" customFormat="1" ht="22.8">
-      <c r="A75" s="962"/>
-      <c r="B75" s="965"/>
+      <c r="A75" s="981"/>
+      <c r="B75" s="984"/>
       <c r="C75" s="815" t="s">
         <v>813</v>
       </c>
@@ -23468,7 +23468,7 @@
         <v>813</v>
       </c>
       <c r="S75" s="426"/>
-      <c r="T75" s="981"/>
+      <c r="T75" s="974"/>
       <c r="V75" s="324"/>
       <c r="X75" s="590" t="s">
         <v>612</v>
@@ -23481,8 +23481,8 @@
       <c r="AF75" s="937"/>
     </row>
     <row r="76" spans="1:32" s="315" customFormat="1" ht="61.5" customHeight="1">
-      <c r="A76" s="962"/>
-      <c r="B76" s="965"/>
+      <c r="A76" s="981"/>
+      <c r="B76" s="984"/>
       <c r="C76" s="815" t="s">
         <v>814</v>
       </c>
@@ -23530,8 +23530,8 @@
       <c r="AF76" s="937"/>
     </row>
     <row r="77" spans="1:32" s="1" customFormat="1" ht="150" customHeight="1">
-      <c r="A77" s="962"/>
-      <c r="B77" s="965"/>
+      <c r="A77" s="981"/>
+      <c r="B77" s="984"/>
       <c r="C77" s="815" t="s">
         <v>869</v>
       </c>
@@ -23584,8 +23584,8 @@
       <c r="AF77" s="937"/>
     </row>
     <row r="78" spans="1:32" s="1" customFormat="1" ht="121.5" customHeight="1">
-      <c r="A78" s="963"/>
-      <c r="B78" s="966"/>
+      <c r="A78" s="982"/>
+      <c r="B78" s="985"/>
       <c r="C78" s="815" t="s">
         <v>870</v>
       </c>
@@ -23622,10 +23622,10 @@
       <c r="AF78" s="937"/>
     </row>
     <row r="79" spans="1:32" s="1" customFormat="1" ht="60" customHeight="1">
-      <c r="A79" s="958" t="s">
+      <c r="A79" s="977" t="s">
         <v>228</v>
       </c>
-      <c r="B79" s="960" t="s">
+      <c r="B79" s="979" t="s">
         <v>212</v>
       </c>
       <c r="C79" s="326" t="s">
@@ -23676,8 +23676,8 @@
       <c r="AF79" s="937"/>
     </row>
     <row r="80" spans="1:32" s="315" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A80" s="959"/>
-      <c r="B80" s="960"/>
+      <c r="A80" s="978"/>
+      <c r="B80" s="979"/>
       <c r="C80" s="326" t="s">
         <v>598</v>
       </c>
@@ -23724,8 +23724,8 @@
       <c r="AF80" s="937"/>
     </row>
     <row r="81" spans="1:32" s="276" customFormat="1" ht="126" customHeight="1">
-      <c r="A81" s="959"/>
-      <c r="B81" s="960"/>
+      <c r="A81" s="978"/>
+      <c r="B81" s="979"/>
       <c r="C81" s="326" t="s">
         <v>832</v>
       </c>
@@ -23773,8 +23773,8 @@
       <c r="AF81" s="937"/>
     </row>
     <row r="82" spans="1:32" s="315" customFormat="1" ht="69" customHeight="1">
-      <c r="A82" s="959"/>
-      <c r="B82" s="960"/>
+      <c r="A82" s="978"/>
+      <c r="B82" s="979"/>
       <c r="C82" s="326" t="s">
         <v>580</v>
       </c>
@@ -23820,8 +23820,8 @@
       <c r="AF82" s="937"/>
     </row>
     <row r="83" spans="1:32" s="315" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A83" s="959"/>
-      <c r="B83" s="960"/>
+      <c r="A83" s="978"/>
+      <c r="B83" s="979"/>
       <c r="C83" s="319" t="s">
         <v>394</v>
       </c>
@@ -23867,8 +23867,8 @@
       <c r="AF83" s="937"/>
     </row>
     <row r="84" spans="1:32" s="315" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A84" s="959"/>
-      <c r="B84" s="960"/>
+      <c r="A84" s="978"/>
+      <c r="B84" s="979"/>
       <c r="C84" s="319" t="s">
         <v>664</v>
       </c>
@@ -23916,8 +23916,8 @@
       <c r="AF84" s="937"/>
     </row>
     <row r="85" spans="1:32" s="276" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A85" s="959"/>
-      <c r="B85" s="960"/>
+      <c r="A85" s="978"/>
+      <c r="B85" s="979"/>
       <c r="C85" s="326" t="s">
         <v>396</v>
       </c>
@@ -24916,6 +24916,27 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="A79:A85"/>
+    <mergeCell ref="B79:B85"/>
+    <mergeCell ref="A59:A78"/>
+    <mergeCell ref="B59:B78"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="T24:T26"/>
+    <mergeCell ref="T61:T75"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="E27:E29"/>
     <mergeCell ref="AD1:AD2"/>
     <mergeCell ref="AF1:AF2"/>
     <mergeCell ref="A7:A8"/>
@@ -24932,27 +24953,6 @@
     <mergeCell ref="G1:L1"/>
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="N1:N2"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="T24:T26"/>
-    <mergeCell ref="T61:T75"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="A79:A85"/>
-    <mergeCell ref="B79:B85"/>
-    <mergeCell ref="A59:A78"/>
-    <mergeCell ref="B59:B78"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="X1:X2"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7 G89:M93 E86:E88 R83:R84 C33:M39 C12:D24 C40:C41 G31:M32 E24 R62:R78 E12:E20 F12:F24 R33:R38 G44:M49 E47 C83:C84 C59:F78 G79:M85 G27:M27 C7:F11 G59:M61 D40:M43 C31:F31 A59:A61" xr:uid="{00000000-0002-0000-0500-000000000000}">
@@ -25129,11 +25129,11 @@
       <c r="M3" s="243"/>
     </row>
     <row r="4" spans="1:33" ht="19.5" customHeight="1">
-      <c r="A4" s="993" t="s">
+      <c r="A4" s="991" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="993"/>
-      <c r="C4" s="993"/>
+      <c r="B4" s="991"/>
+      <c r="C4" s="991"/>
       <c r="D4" s="243"/>
       <c r="E4" s="243"/>
       <c r="F4" s="243"/>
@@ -25151,9 +25151,9 @@
       <c r="AG4" s="3"/>
     </row>
     <row r="5" spans="1:33" s="1" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A5" s="992"/>
-      <c r="B5" s="992"/>
-      <c r="C5" s="992"/>
+      <c r="A5" s="990"/>
+      <c r="B5" s="990"/>
+      <c r="C5" s="990"/>
       <c r="D5" s="113"/>
       <c r="E5" s="270"/>
       <c r="F5" s="270"/>
@@ -26909,7 +26909,7 @@
         <v>283</v>
       </c>
       <c r="D40" s="183"/>
-      <c r="E40" s="990"/>
+      <c r="E40" s="992"/>
       <c r="F40" s="273"/>
       <c r="G40" s="404" t="s">
         <v>10</v>
@@ -26967,7 +26967,7 @@
         <v>414</v>
       </c>
       <c r="D41" s="273"/>
-      <c r="E41" s="974"/>
+      <c r="E41" s="962"/>
       <c r="F41" s="273"/>
       <c r="G41" s="370"/>
       <c r="H41" s="370"/>
@@ -27000,7 +27000,7 @@
         <v>415</v>
       </c>
       <c r="D42" s="273"/>
-      <c r="E42" s="974"/>
+      <c r="E42" s="962"/>
       <c r="F42" s="273"/>
       <c r="G42" s="370"/>
       <c r="H42" s="370"/>
@@ -27034,7 +27034,7 @@
         <v>658</v>
       </c>
       <c r="D43" s="273"/>
-      <c r="E43" s="991"/>
+      <c r="E43" s="993"/>
       <c r="F43" s="273"/>
       <c r="G43" s="369"/>
       <c r="H43" s="369"/>
@@ -27896,6 +27896,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="V1:V2"/>
     <mergeCell ref="AE1:AE2"/>
     <mergeCell ref="AG1:AG2"/>
     <mergeCell ref="A5:C5"/>
@@ -27903,13 +27910,6 @@
     <mergeCell ref="AB1:AB2"/>
     <mergeCell ref="Z1:Z2"/>
     <mergeCell ref="G1:L1"/>
-    <mergeCell ref="E40:E43"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="V1:V2"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G15:M15 G40:M44 G30:M37 E38:E39 G56:K60" xr:uid="{00000000-0002-0000-0600-000000000000}">
@@ -28074,11 +28074,11 @@
       <c r="AF2" s="948"/>
     </row>
     <row r="4" spans="1:32" ht="15">
-      <c r="A4" s="993" t="s">
+      <c r="A4" s="991" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="993"/>
-      <c r="C4" s="993"/>
+      <c r="B4" s="991"/>
+      <c r="C4" s="991"/>
       <c r="AD4" s="3"/>
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
@@ -29050,10 +29050,10 @@
       <c r="AF2" s="948"/>
     </row>
     <row r="4" spans="1:32" ht="15">
-      <c r="A4" s="993" t="s">
+      <c r="A4" s="991" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="993"/>
+      <c r="B4" s="991"/>
       <c r="AD4" s="3"/>
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>

</xml_diff>

<commit_message>
read some N values of column
</commit_message>
<xml_diff>
--- a/xlsx/BMW_Sales_Standards_2016_ME.xlsx
+++ b/xlsx/BMW_Sales_Standards_2016_ME.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Camilo\Desktop\python\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KAPTA Camilo\python\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12708" yWindow="348" windowWidth="2688" windowHeight="7440" tabRatio="870" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12708" yWindow="348" windowWidth="2688" windowHeight="7440" tabRatio="870" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="21" r:id="rId1"/>
@@ -8043,6 +8043,84 @@
     <xf numFmtId="0" fontId="60" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="11" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -8055,89 +8133,17 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="56" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -8145,11 +8151,17 @@
     <xf numFmtId="0" fontId="60" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -8168,18 +8180,6 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="64" fillId="18" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -9339,11 +9339,11 @@
       <c r="AF2" s="948"/>
     </row>
     <row r="4" spans="1:32" ht="15">
-      <c r="A4" s="991" t="s">
+      <c r="A4" s="993" t="s">
         <v>96</v>
       </c>
-      <c r="B4" s="991"/>
-      <c r="C4" s="991"/>
+      <c r="B4" s="993"/>
+      <c r="C4" s="993"/>
       <c r="AD4" s="3"/>
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
@@ -10924,11 +10924,11 @@
       <c r="AF2" s="948"/>
     </row>
     <row r="4" spans="1:32" ht="15.6">
-      <c r="A4" s="994" t="s">
+      <c r="A4" s="998" t="s">
         <v>155</v>
       </c>
-      <c r="B4" s="994"/>
-      <c r="C4" s="994"/>
+      <c r="B4" s="998"/>
+      <c r="C4" s="998"/>
       <c r="AD4" s="3"/>
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
@@ -11248,34 +11248,34 @@
       <c r="AF10" s="936"/>
     </row>
     <row r="11" spans="1:32" s="1" customFormat="1" ht="191.25" customHeight="1">
-      <c r="A11" s="995" t="s">
+      <c r="A11" s="999" t="s">
         <v>107</v>
       </c>
-      <c r="B11" s="998" t="s">
+      <c r="B11" s="1002" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="1000" t="s">
+      <c r="C11" s="994" t="s">
         <v>997</v>
       </c>
       <c r="D11" s="193"/>
-      <c r="E11" s="1000"/>
+      <c r="E11" s="994"/>
       <c r="F11" s="193"/>
-      <c r="G11" s="964" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="964" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="964" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" s="964" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" s="964" t="s">
-        <v>10</v>
-      </c>
-      <c r="L11" s="964" t="s">
+      <c r="G11" s="988" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="988" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="988" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="988" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="988" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" s="988" t="s">
         <v>10</v>
       </c>
       <c r="M11" s="186"/>
@@ -11311,18 +11311,18 @@
       <c r="AF11" s="936"/>
     </row>
     <row r="12" spans="1:32" s="1" customFormat="1" ht="13.8">
-      <c r="A12" s="996"/>
-      <c r="B12" s="979"/>
-      <c r="C12" s="1001"/>
+      <c r="A12" s="1000"/>
+      <c r="B12" s="960"/>
+      <c r="C12" s="995"/>
       <c r="D12" s="193"/>
-      <c r="E12" s="1001"/>
+      <c r="E12" s="995"/>
       <c r="F12" s="193"/>
-      <c r="G12" s="1003"/>
-      <c r="H12" s="1003"/>
-      <c r="I12" s="1003"/>
-      <c r="J12" s="1003"/>
-      <c r="K12" s="1003"/>
-      <c r="L12" s="1003"/>
+      <c r="G12" s="997"/>
+      <c r="H12" s="997"/>
+      <c r="I12" s="997"/>
+      <c r="J12" s="997"/>
+      <c r="K12" s="997"/>
+      <c r="L12" s="997"/>
       <c r="M12" s="188"/>
       <c r="N12" s="256"/>
       <c r="P12" s="914"/>
@@ -11343,18 +11343,18 @@
       <c r="AF12" s="936"/>
     </row>
     <row r="13" spans="1:32" s="1" customFormat="1" ht="13.8">
-      <c r="A13" s="996"/>
-      <c r="B13" s="979"/>
-      <c r="C13" s="1001"/>
+      <c r="A13" s="1000"/>
+      <c r="B13" s="960"/>
+      <c r="C13" s="995"/>
       <c r="D13" s="193"/>
-      <c r="E13" s="1001"/>
+      <c r="E13" s="995"/>
       <c r="F13" s="193"/>
-      <c r="G13" s="1003"/>
-      <c r="H13" s="1003"/>
-      <c r="I13" s="1003"/>
-      <c r="J13" s="1003"/>
-      <c r="K13" s="1003"/>
-      <c r="L13" s="1003"/>
+      <c r="G13" s="997"/>
+      <c r="H13" s="997"/>
+      <c r="I13" s="997"/>
+      <c r="J13" s="997"/>
+      <c r="K13" s="997"/>
+      <c r="L13" s="997"/>
       <c r="M13" s="188"/>
       <c r="N13" s="256"/>
       <c r="P13" s="914"/>
@@ -11375,18 +11375,18 @@
       <c r="AF13" s="936"/>
     </row>
     <row r="14" spans="1:32" s="1" customFormat="1" ht="35.25" customHeight="1">
-      <c r="A14" s="997"/>
-      <c r="B14" s="999"/>
-      <c r="C14" s="1002"/>
+      <c r="A14" s="1001"/>
+      <c r="B14" s="1003"/>
+      <c r="C14" s="996"/>
       <c r="D14" s="193"/>
-      <c r="E14" s="1002"/>
+      <c r="E14" s="996"/>
       <c r="F14" s="193"/>
-      <c r="G14" s="965"/>
-      <c r="H14" s="965"/>
-      <c r="I14" s="965"/>
-      <c r="J14" s="965"/>
-      <c r="K14" s="965"/>
-      <c r="L14" s="965"/>
+      <c r="G14" s="989"/>
+      <c r="H14" s="989"/>
+      <c r="I14" s="989"/>
+      <c r="J14" s="989"/>
+      <c r="K14" s="989"/>
+      <c r="L14" s="989"/>
       <c r="M14" s="176"/>
       <c r="N14" s="264"/>
       <c r="P14" s="913"/>
@@ -13016,6 +13016,17 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="AD1:AD2"/>
+    <mergeCell ref="AF1:AF2"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="R1:R2"/>
     <mergeCell ref="T1:T2"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="K11:K14"/>
@@ -13027,17 +13038,6 @@
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="G1:L1"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="AD1:AD2"/>
-    <mergeCell ref="AF1:AF2"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="X1:X2"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:M11 G15:M22 G24:M37 G38:N38" xr:uid="{00000000-0002-0000-0A00-000000000000}">
@@ -13067,10 +13067,10 @@
   </sheetPr>
   <dimension ref="A1:AF20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="D1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="F1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z14" sqref="Z14"/>
-      <selection pane="bottomLeft" activeCell="T7" sqref="T7"/>
+      <selection pane="bottomLeft" activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -13198,10 +13198,10 @@
       <c r="AF2" s="948"/>
     </row>
     <row r="4" spans="1:32" ht="15">
-      <c r="A4" s="991" t="s">
+      <c r="A4" s="993" t="s">
         <v>342</v>
       </c>
-      <c r="B4" s="991"/>
+      <c r="B4" s="993"/>
       <c r="AD4" s="3"/>
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
@@ -13810,7 +13810,7 @@
       <c r="Y16" s="425"/>
       <c r="Z16" s="945">
         <f>IF(OR(X16="A",X17="A",X18="A",X19="A"),"",IF(OR(X16="N",X17="N",X18="N",X19="N"),0,1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA16" s="315"/>
       <c r="AB16" s="801" t="s">
@@ -13882,7 +13882,7 @@
       <c r="T18" s="300"/>
       <c r="V18" s="314"/>
       <c r="X18" s="590" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="Z18" s="941"/>
       <c r="AB18" s="800"/>
@@ -13915,7 +13915,7 @@
       </c>
       <c r="V19" s="307"/>
       <c r="X19" s="590" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="Z19" s="942"/>
       <c r="AB19" s="798"/>
@@ -16897,11 +16897,11 @@
       </c>
       <c r="F19" s="640">
         <f>SUM('Section 3_Sales Area'!Z7:Z101)-SUMIF('Section 3_Sales Area'!P7:P101,"O",'Section 3_Sales Area'!Z7:Z101)</f>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H19" s="641">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.96296296296296291</v>
       </c>
       <c r="J19" s="640">
         <f>COUNTIFS('Section 3_Sales Area'!P7:P101,"X",'Section 3_Sales Area'!Z7:Z101,1)+COUNTIFS('Section 3_Sales Area'!P7:P101,"X",'Section 3_Sales Area'!Z7:Z101,0)</f>
@@ -16910,12 +16910,12 @@
       <c r="K19"/>
       <c r="L19" s="640">
         <f>SUMIF('Section 3_Sales Area'!P7:P101,"X",'Section 3_Sales Area'!Z7:Z101)</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M19" s="633"/>
       <c r="N19" s="641">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="O19" s="633"/>
       <c r="P19" s="771"/>
@@ -17095,11 +17095,11 @@
       </c>
       <c r="F25" s="640">
         <f>SUM('Section 9_Marketing'!Z6:Z20)-SUMIF('Section 9_Marketing'!P6:P20,"O",'Section 9_Marketing'!Z6:Z20)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H25" s="641">
         <f t="shared" si="1"/>
-        <v>0.83333333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="J25" s="640">
         <f>COUNTIFS('Section 9_Marketing'!P6:P20,"X",'Section 9_Marketing'!Z6:Z20,1)+COUNTIFS('Section 9_Marketing'!P6:P20,"X",'Section 9_Marketing'!Z6:Z20,0)</f>
@@ -17108,12 +17108,12 @@
       <c r="K25"/>
       <c r="L25" s="640">
         <f>SUMIF('Section 9_Marketing'!P6:P20,"X",'Section 9_Marketing'!Z6:Z20)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M25" s="633"/>
       <c r="N25" s="641">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O25" s="633"/>
       <c r="P25" s="772"/>
@@ -17166,12 +17166,12 @@
       <c r="E28" s="625"/>
       <c r="F28" s="624">
         <f>SUM(F17:F26)</f>
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G28" s="625"/>
       <c r="H28" s="626">
         <f>IFERROR(F28/D28,0%)</f>
-        <v>0.98901098901098905</v>
+        <v>0.96703296703296704</v>
       </c>
       <c r="I28" s="625"/>
       <c r="J28" s="627">
@@ -17181,12 +17181,12 @@
       <c r="K28" s="625"/>
       <c r="L28" s="627">
         <f>SUM(L17:L26)</f>
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="M28" s="625"/>
       <c r="N28" s="628">
         <f>IFERROR(L28/J28,0%)</f>
-        <v>1</v>
+        <v>0.93939393939393945</v>
       </c>
       <c r="O28" s="625"/>
       <c r="P28" s="625"/>
@@ -18083,10 +18083,10 @@
   </sheetPr>
   <dimension ref="A1:AF44"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="P1" sqref="P1:P1048576"/>
-      <selection pane="bottomLeft" activeCell="X7" sqref="X7"/>
+      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -20041,10 +20041,10 @@
   </sheetPr>
   <dimension ref="A1:AF101"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" topLeftCell="Q1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="P1" sqref="P1:P1048576"/>
-      <selection pane="bottomLeft" activeCell="H85" sqref="H85"/>
+      <selection pane="bottomLeft" activeCell="Z56" sqref="Z56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -20240,17 +20240,17 @@
       <c r="AF6" s="3"/>
     </row>
     <row r="7" spans="1:32" s="1" customFormat="1" ht="115.5" customHeight="1">
-      <c r="A7" s="958" t="s">
+      <c r="A7" s="984" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="958" t="s">
+      <c r="B7" s="984" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="963" t="s">
+      <c r="C7" s="973" t="s">
         <v>763</v>
       </c>
       <c r="D7" s="142"/>
-      <c r="E7" s="963"/>
+      <c r="E7" s="973"/>
       <c r="F7" s="142"/>
       <c r="G7" s="24" t="s">
         <v>10</v>
@@ -20306,11 +20306,11 @@
       <c r="AF7" s="936"/>
     </row>
     <row r="8" spans="1:32" s="1" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A8" s="959"/>
-      <c r="B8" s="959"/>
-      <c r="C8" s="962"/>
+      <c r="A8" s="985"/>
+      <c r="B8" s="985"/>
+      <c r="C8" s="974"/>
       <c r="D8" s="143"/>
-      <c r="E8" s="962"/>
+      <c r="E8" s="974"/>
       <c r="F8" s="143"/>
       <c r="G8" s="30"/>
       <c r="H8" s="30"/>
@@ -20341,13 +20341,13 @@
       <c r="AF8" s="936"/>
     </row>
     <row r="9" spans="1:32" s="1" customFormat="1" ht="45.6">
-      <c r="A9" s="959"/>
-      <c r="B9" s="959"/>
-      <c r="C9" s="962" t="s">
+      <c r="A9" s="985"/>
+      <c r="B9" s="985"/>
+      <c r="C9" s="974" t="s">
         <v>677</v>
       </c>
       <c r="D9" s="143"/>
-      <c r="E9" s="962"/>
+      <c r="E9" s="974"/>
       <c r="F9" s="143"/>
       <c r="G9" s="30" t="s">
         <v>10</v>
@@ -20397,11 +20397,11 @@
       <c r="AF9" s="936"/>
     </row>
     <row r="10" spans="1:32" s="1" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A10" s="959"/>
-      <c r="B10" s="959"/>
-      <c r="C10" s="962"/>
+      <c r="A10" s="985"/>
+      <c r="B10" s="985"/>
+      <c r="C10" s="974"/>
       <c r="D10" s="143"/>
-      <c r="E10" s="962"/>
+      <c r="E10" s="974"/>
       <c r="F10" s="143"/>
       <c r="G10" s="30" t="s">
         <v>10</v>
@@ -20683,7 +20683,7 @@
         <v>747</v>
       </c>
       <c r="D16" s="840"/>
-      <c r="E16" s="964"/>
+      <c r="E16" s="988"/>
       <c r="F16" s="840"/>
       <c r="G16" s="868" t="s">
         <v>10</v>
@@ -20740,7 +20740,7 @@
         <v>746</v>
       </c>
       <c r="D17" s="841"/>
-      <c r="E17" s="965"/>
+      <c r="E17" s="989"/>
       <c r="F17" s="841"/>
       <c r="G17" s="29"/>
       <c r="H17" s="29"/>
@@ -20778,10 +20778,10 @@
       <c r="AF17" s="936"/>
     </row>
     <row r="18" spans="1:32" s="1" customFormat="1" ht="53.25" customHeight="1">
-      <c r="A18" s="958" t="s">
+      <c r="A18" s="984" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="958" t="s">
+      <c r="B18" s="984" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="839" t="s">
@@ -20844,8 +20844,8 @@
       <c r="AF18" s="936"/>
     </row>
     <row r="19" spans="1:32" s="315" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A19" s="959"/>
-      <c r="B19" s="959"/>
+      <c r="A19" s="985"/>
+      <c r="B19" s="985"/>
       <c r="C19" s="363"/>
       <c r="D19" s="143"/>
       <c r="E19" s="363"/>
@@ -20876,13 +20876,13 @@
       <c r="AF19" s="937"/>
     </row>
     <row r="20" spans="1:32" s="1" customFormat="1" ht="87" customHeight="1">
-      <c r="A20" s="959"/>
-      <c r="B20" s="959"/>
+      <c r="A20" s="985"/>
+      <c r="B20" s="985"/>
       <c r="C20" s="363" t="s">
         <v>592</v>
       </c>
       <c r="D20" s="144"/>
-      <c r="E20" s="960"/>
+      <c r="E20" s="986"/>
       <c r="F20" s="144"/>
       <c r="G20" s="24"/>
       <c r="H20" s="867" t="s">
@@ -20927,7 +20927,7 @@
       <c r="B21" s="359"/>
       <c r="C21" s="363"/>
       <c r="D21" s="433"/>
-      <c r="E21" s="960"/>
+      <c r="E21" s="986"/>
       <c r="F21" s="433"/>
       <c r="G21" s="30"/>
       <c r="H21" s="30"/>
@@ -20959,7 +20959,7 @@
       <c r="B22" s="359"/>
       <c r="C22" s="363"/>
       <c r="D22" s="433"/>
-      <c r="E22" s="960"/>
+      <c r="E22" s="986"/>
       <c r="F22" s="433"/>
       <c r="G22" s="30"/>
       <c r="H22" s="30"/>
@@ -20991,7 +20991,7 @@
       <c r="B23" s="357"/>
       <c r="C23" s="362"/>
       <c r="D23" s="433"/>
-      <c r="E23" s="961"/>
+      <c r="E23" s="987"/>
       <c r="F23" s="433"/>
       <c r="G23" s="26"/>
       <c r="H23" s="26"/>
@@ -21019,17 +21019,17 @@
       <c r="AF23" s="937"/>
     </row>
     <row r="24" spans="1:32" s="1" customFormat="1" ht="96" customHeight="1">
-      <c r="A24" s="986" t="s">
+      <c r="A24" s="967" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="988" t="s">
+      <c r="B24" s="969" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="968" t="s">
+      <c r="C24" s="975" t="s">
         <v>501</v>
       </c>
       <c r="D24" s="143"/>
-      <c r="E24" s="968"/>
+      <c r="E24" s="975"/>
       <c r="F24" s="143"/>
       <c r="G24" s="30" t="s">
         <v>10</v>
@@ -21060,7 +21060,7 @@
         <v>294</v>
       </c>
       <c r="S24" s="426"/>
-      <c r="T24" s="969" t="s">
+      <c r="T24" s="976" t="s">
         <v>475</v>
       </c>
       <c r="V24" s="429" t="s">
@@ -21085,11 +21085,11 @@
       <c r="AF24" s="937"/>
     </row>
     <row r="25" spans="1:32" s="1" customFormat="1" ht="44.25" customHeight="1">
-      <c r="A25" s="987"/>
-      <c r="B25" s="989"/>
-      <c r="C25" s="963"/>
+      <c r="A25" s="968"/>
+      <c r="B25" s="970"/>
+      <c r="C25" s="973"/>
       <c r="D25" s="143"/>
-      <c r="E25" s="963"/>
+      <c r="E25" s="973"/>
       <c r="F25" s="143"/>
       <c r="G25" s="30"/>
       <c r="H25" s="30"/>
@@ -21104,7 +21104,7 @@
         <v>555</v>
       </c>
       <c r="S25" s="426"/>
-      <c r="T25" s="970"/>
+      <c r="T25" s="977"/>
       <c r="V25" s="429"/>
       <c r="W25" s="315"/>
       <c r="X25" s="590" t="s">
@@ -21139,7 +21139,7 @@
         <v>502</v>
       </c>
       <c r="S26" s="426"/>
-      <c r="T26" s="971"/>
+      <c r="T26" s="978"/>
       <c r="V26" s="429"/>
       <c r="X26" s="590" t="s">
         <v>612</v>
@@ -21158,11 +21158,11 @@
       <c r="B27" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="966" t="s">
+      <c r="C27" s="971" t="s">
         <v>889</v>
       </c>
       <c r="D27" s="145"/>
-      <c r="E27" s="975"/>
+      <c r="E27" s="982"/>
       <c r="F27" s="145"/>
       <c r="G27" s="915">
         <v>3</v>
@@ -21220,9 +21220,9 @@
     <row r="28" spans="1:32" s="1" customFormat="1" ht="54.75" customHeight="1">
       <c r="A28" s="25"/>
       <c r="B28" s="34"/>
-      <c r="C28" s="967"/>
+      <c r="C28" s="972"/>
       <c r="D28" s="146"/>
-      <c r="E28" s="976"/>
+      <c r="E28" s="983"/>
       <c r="F28" s="146"/>
       <c r="G28" s="25"/>
       <c r="H28" s="25"/>
@@ -21255,9 +21255,9 @@
     <row r="29" spans="1:32" s="1" customFormat="1" ht="106.5" customHeight="1">
       <c r="A29" s="292"/>
       <c r="B29" s="34"/>
-      <c r="C29" s="967"/>
+      <c r="C29" s="972"/>
       <c r="D29" s="146"/>
-      <c r="E29" s="976"/>
+      <c r="E29" s="983"/>
       <c r="F29" s="146"/>
       <c r="G29" s="299"/>
       <c r="H29" s="299"/>
@@ -22104,7 +22104,7 @@
       <c r="AF43" s="937"/>
     </row>
     <row r="44" spans="1:32" s="1" customFormat="1" ht="62.25" customHeight="1">
-      <c r="A44" s="977" t="s">
+      <c r="A44" s="958" t="s">
         <v>812</v>
       </c>
       <c r="B44" s="374" t="s">
@@ -22158,7 +22158,7 @@
       <c r="AF44" s="937"/>
     </row>
     <row r="45" spans="1:32" s="1" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A45" s="978"/>
+      <c r="A45" s="959"/>
       <c r="B45" s="289"/>
       <c r="C45" s="319" t="s">
         <v>379</v>
@@ -22207,7 +22207,7 @@
       <c r="AF45" s="937"/>
     </row>
     <row r="46" spans="1:32" s="1" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A46" s="978"/>
+      <c r="A46" s="959"/>
       <c r="B46" s="289"/>
       <c r="C46" s="319" t="s">
         <v>380</v>
@@ -22711,7 +22711,7 @@
       <c r="Y55" s="315"/>
       <c r="Z55" s="582">
         <f>IF(OR(X55="A",X56="A",X57="A",X58="A"),"",IF(OR(X55="N",X56="N",X57="N",X58="N"),0,1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA55" s="761"/>
       <c r="AB55" s="787" t="s">
@@ -22781,7 +22781,7 @@
       <c r="T57" s="402"/>
       <c r="V57" s="324"/>
       <c r="X57" s="590" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="Z57" s="591"/>
       <c r="AA57" s="762"/>
@@ -22826,10 +22826,10 @@
       <c r="AF58" s="937"/>
     </row>
     <row r="59" spans="1:32" s="1" customFormat="1" ht="67.5" customHeight="1">
-      <c r="A59" s="980" t="s">
+      <c r="A59" s="961" t="s">
         <v>573</v>
       </c>
-      <c r="B59" s="983" t="s">
+      <c r="B59" s="964" t="s">
         <v>211</v>
       </c>
       <c r="C59" s="455" t="s">
@@ -22893,8 +22893,8 @@
       <c r="AF59" s="937"/>
     </row>
     <row r="60" spans="1:32" s="315" customFormat="1" ht="33" customHeight="1">
-      <c r="A60" s="981"/>
-      <c r="B60" s="984"/>
+      <c r="A60" s="962"/>
+      <c r="B60" s="965"/>
       <c r="C60" s="457"/>
       <c r="D60" s="454"/>
       <c r="E60" s="457"/>
@@ -22929,8 +22929,8 @@
       <c r="AF60" s="937"/>
     </row>
     <row r="61" spans="1:32" s="315" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A61" s="981"/>
-      <c r="B61" s="984"/>
+      <c r="A61" s="962"/>
+      <c r="B61" s="965"/>
       <c r="C61" s="456" t="s">
         <v>574</v>
       </c>
@@ -22951,7 +22951,7 @@
         <v>579</v>
       </c>
       <c r="S61" s="426"/>
-      <c r="T61" s="972" t="s">
+      <c r="T61" s="979" t="s">
         <v>385</v>
       </c>
       <c r="V61" s="324"/>
@@ -22964,8 +22964,8 @@
       <c r="AF61" s="937"/>
     </row>
     <row r="62" spans="1:32" s="1" customFormat="1">
-      <c r="A62" s="981"/>
-      <c r="B62" s="984"/>
+      <c r="A62" s="962"/>
+      <c r="B62" s="965"/>
       <c r="C62" s="319" t="s">
         <v>386</v>
       </c>
@@ -22986,7 +22986,7 @@
         <v>386</v>
       </c>
       <c r="S62" s="426"/>
-      <c r="T62" s="973"/>
+      <c r="T62" s="980"/>
       <c r="V62" s="324"/>
       <c r="W62" s="315"/>
       <c r="X62" s="590" t="s">
@@ -23002,8 +23002,8 @@
       <c r="AF62" s="937"/>
     </row>
     <row r="63" spans="1:32" s="315" customFormat="1">
-      <c r="A63" s="981"/>
-      <c r="B63" s="984"/>
+      <c r="A63" s="962"/>
+      <c r="B63" s="965"/>
       <c r="C63" s="319" t="s">
         <v>575</v>
       </c>
@@ -23024,7 +23024,7 @@
         <v>575</v>
       </c>
       <c r="S63" s="426"/>
-      <c r="T63" s="973"/>
+      <c r="T63" s="980"/>
       <c r="V63" s="324"/>
       <c r="X63" s="590" t="s">
         <v>612</v>
@@ -23037,8 +23037,8 @@
       <c r="AF63" s="937"/>
     </row>
     <row r="64" spans="1:32" s="315" customFormat="1">
-      <c r="A64" s="981"/>
-      <c r="B64" s="984"/>
+      <c r="A64" s="962"/>
+      <c r="B64" s="965"/>
       <c r="C64" s="702" t="s">
         <v>576</v>
       </c>
@@ -23059,7 +23059,7 @@
         <v>576</v>
       </c>
       <c r="S64" s="426"/>
-      <c r="T64" s="973"/>
+      <c r="T64" s="980"/>
       <c r="V64" s="707"/>
       <c r="X64" s="590" t="s">
         <v>612</v>
@@ -23072,8 +23072,8 @@
       <c r="AF64" s="937"/>
     </row>
     <row r="65" spans="1:32" s="315" customFormat="1">
-      <c r="A65" s="981"/>
-      <c r="B65" s="984"/>
+      <c r="A65" s="962"/>
+      <c r="B65" s="965"/>
       <c r="C65" s="319" t="s">
         <v>387</v>
       </c>
@@ -23094,7 +23094,7 @@
         <v>387</v>
       </c>
       <c r="S65" s="426"/>
-      <c r="T65" s="973"/>
+      <c r="T65" s="980"/>
       <c r="V65" s="348"/>
       <c r="X65" s="590" t="s">
         <v>612</v>
@@ -23107,8 +23107,8 @@
       <c r="AF65" s="937"/>
     </row>
     <row r="66" spans="1:32" s="315" customFormat="1">
-      <c r="A66" s="981"/>
-      <c r="B66" s="984"/>
+      <c r="A66" s="962"/>
+      <c r="B66" s="965"/>
       <c r="C66" s="319" t="s">
         <v>500</v>
       </c>
@@ -23129,7 +23129,7 @@
         <v>500</v>
       </c>
       <c r="S66" s="426"/>
-      <c r="T66" s="973"/>
+      <c r="T66" s="980"/>
       <c r="V66" s="348"/>
       <c r="X66" s="590" t="s">
         <v>612</v>
@@ -23142,8 +23142,8 @@
       <c r="AF66" s="937"/>
     </row>
     <row r="67" spans="1:32" s="315" customFormat="1">
-      <c r="A67" s="981"/>
-      <c r="B67" s="984"/>
+      <c r="A67" s="962"/>
+      <c r="B67" s="965"/>
       <c r="C67" s="319" t="s">
         <v>388</v>
       </c>
@@ -23164,7 +23164,7 @@
         <v>388</v>
       </c>
       <c r="S67" s="426"/>
-      <c r="T67" s="973"/>
+      <c r="T67" s="980"/>
       <c r="V67" s="348"/>
       <c r="X67" s="590" t="s">
         <v>612</v>
@@ -23177,8 +23177,8 @@
       <c r="AF67" s="937"/>
     </row>
     <row r="68" spans="1:32" s="315" customFormat="1">
-      <c r="A68" s="981"/>
-      <c r="B68" s="984"/>
+      <c r="A68" s="962"/>
+      <c r="B68" s="965"/>
       <c r="C68" s="319" t="s">
         <v>389</v>
       </c>
@@ -23199,7 +23199,7 @@
         <v>389</v>
       </c>
       <c r="S68" s="426"/>
-      <c r="T68" s="973"/>
+      <c r="T68" s="980"/>
       <c r="V68" s="348"/>
       <c r="X68" s="590" t="s">
         <v>612</v>
@@ -23212,8 +23212,8 @@
       <c r="AF68" s="937"/>
     </row>
     <row r="69" spans="1:32" s="315" customFormat="1" ht="45" customHeight="1">
-      <c r="A69" s="981"/>
-      <c r="B69" s="984"/>
+      <c r="A69" s="962"/>
+      <c r="B69" s="965"/>
       <c r="C69" s="319" t="s">
         <v>390</v>
       </c>
@@ -23234,7 +23234,7 @@
         <v>391</v>
       </c>
       <c r="S69" s="426"/>
-      <c r="T69" s="973"/>
+      <c r="T69" s="980"/>
       <c r="V69" s="348"/>
       <c r="X69" s="590" t="s">
         <v>612</v>
@@ -23247,8 +23247,8 @@
       <c r="AF69" s="937"/>
     </row>
     <row r="70" spans="1:32" s="315" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A70" s="981"/>
-      <c r="B70" s="984"/>
+      <c r="A70" s="962"/>
+      <c r="B70" s="965"/>
       <c r="C70" s="319" t="s">
         <v>392</v>
       </c>
@@ -23269,7 +23269,7 @@
         <v>392</v>
       </c>
       <c r="S70" s="426"/>
-      <c r="T70" s="973"/>
+      <c r="T70" s="980"/>
       <c r="V70" s="348"/>
       <c r="X70" s="590" t="s">
         <v>612</v>
@@ -23282,8 +23282,8 @@
       <c r="AF70" s="937"/>
     </row>
     <row r="71" spans="1:32" s="1" customFormat="1">
-      <c r="A71" s="981"/>
-      <c r="B71" s="984"/>
+      <c r="A71" s="962"/>
+      <c r="B71" s="965"/>
       <c r="C71" s="319" t="s">
         <v>577</v>
       </c>
@@ -23304,7 +23304,7 @@
         <v>577</v>
       </c>
       <c r="S71" s="426"/>
-      <c r="T71" s="973"/>
+      <c r="T71" s="980"/>
       <c r="V71" s="324"/>
       <c r="W71" s="315"/>
       <c r="X71" s="590" t="s">
@@ -23320,8 +23320,8 @@
       <c r="AF71" s="937"/>
     </row>
     <row r="72" spans="1:32" s="1" customFormat="1">
-      <c r="A72" s="981"/>
-      <c r="B72" s="984"/>
+      <c r="A72" s="962"/>
+      <c r="B72" s="965"/>
       <c r="C72" s="319" t="s">
         <v>578</v>
       </c>
@@ -23342,7 +23342,7 @@
         <v>578</v>
       </c>
       <c r="S72" s="426"/>
-      <c r="T72" s="973"/>
+      <c r="T72" s="980"/>
       <c r="V72" s="324"/>
       <c r="W72" s="315"/>
       <c r="X72" s="590" t="s">
@@ -23358,8 +23358,8 @@
       <c r="AF72" s="937"/>
     </row>
     <row r="73" spans="1:32" s="1" customFormat="1">
-      <c r="A73" s="981"/>
-      <c r="B73" s="984"/>
+      <c r="A73" s="962"/>
+      <c r="B73" s="965"/>
       <c r="C73" s="319" t="s">
         <v>393</v>
       </c>
@@ -23380,7 +23380,7 @@
         <v>393</v>
       </c>
       <c r="S73" s="426"/>
-      <c r="T73" s="973"/>
+      <c r="T73" s="980"/>
       <c r="V73" s="324"/>
       <c r="W73" s="315"/>
       <c r="X73" s="590" t="s">
@@ -23396,8 +23396,8 @@
       <c r="AF73" s="937"/>
     </row>
     <row r="74" spans="1:32" s="1" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A74" s="981"/>
-      <c r="B74" s="984"/>
+      <c r="A74" s="962"/>
+      <c r="B74" s="965"/>
       <c r="C74" s="319" t="s">
         <v>546</v>
       </c>
@@ -23418,7 +23418,7 @@
         <v>546</v>
       </c>
       <c r="S74" s="426"/>
-      <c r="T74" s="973"/>
+      <c r="T74" s="980"/>
       <c r="V74" s="324"/>
       <c r="W74" s="315"/>
       <c r="X74" s="590" t="s">
@@ -23434,8 +23434,8 @@
       <c r="AF74" s="937"/>
     </row>
     <row r="75" spans="1:32" s="315" customFormat="1" ht="22.8">
-      <c r="A75" s="981"/>
-      <c r="B75" s="984"/>
+      <c r="A75" s="962"/>
+      <c r="B75" s="965"/>
       <c r="C75" s="815" t="s">
         <v>813</v>
       </c>
@@ -23468,7 +23468,7 @@
         <v>813</v>
       </c>
       <c r="S75" s="426"/>
-      <c r="T75" s="974"/>
+      <c r="T75" s="981"/>
       <c r="V75" s="324"/>
       <c r="X75" s="590" t="s">
         <v>612</v>
@@ -23481,8 +23481,8 @@
       <c r="AF75" s="937"/>
     </row>
     <row r="76" spans="1:32" s="315" customFormat="1" ht="61.5" customHeight="1">
-      <c r="A76" s="981"/>
-      <c r="B76" s="984"/>
+      <c r="A76" s="962"/>
+      <c r="B76" s="965"/>
       <c r="C76" s="815" t="s">
         <v>814</v>
       </c>
@@ -23530,8 +23530,8 @@
       <c r="AF76" s="937"/>
     </row>
     <row r="77" spans="1:32" s="1" customFormat="1" ht="150" customHeight="1">
-      <c r="A77" s="981"/>
-      <c r="B77" s="984"/>
+      <c r="A77" s="962"/>
+      <c r="B77" s="965"/>
       <c r="C77" s="815" t="s">
         <v>869</v>
       </c>
@@ -23584,8 +23584,8 @@
       <c r="AF77" s="937"/>
     </row>
     <row r="78" spans="1:32" s="1" customFormat="1" ht="121.5" customHeight="1">
-      <c r="A78" s="982"/>
-      <c r="B78" s="985"/>
+      <c r="A78" s="963"/>
+      <c r="B78" s="966"/>
       <c r="C78" s="815" t="s">
         <v>870</v>
       </c>
@@ -23622,10 +23622,10 @@
       <c r="AF78" s="937"/>
     </row>
     <row r="79" spans="1:32" s="1" customFormat="1" ht="60" customHeight="1">
-      <c r="A79" s="977" t="s">
+      <c r="A79" s="958" t="s">
         <v>228</v>
       </c>
-      <c r="B79" s="979" t="s">
+      <c r="B79" s="960" t="s">
         <v>212</v>
       </c>
       <c r="C79" s="326" t="s">
@@ -23676,8 +23676,8 @@
       <c r="AF79" s="937"/>
     </row>
     <row r="80" spans="1:32" s="315" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A80" s="978"/>
-      <c r="B80" s="979"/>
+      <c r="A80" s="959"/>
+      <c r="B80" s="960"/>
       <c r="C80" s="326" t="s">
         <v>598</v>
       </c>
@@ -23724,8 +23724,8 @@
       <c r="AF80" s="937"/>
     </row>
     <row r="81" spans="1:32" s="276" customFormat="1" ht="126" customHeight="1">
-      <c r="A81" s="978"/>
-      <c r="B81" s="979"/>
+      <c r="A81" s="959"/>
+      <c r="B81" s="960"/>
       <c r="C81" s="326" t="s">
         <v>832</v>
       </c>
@@ -23773,8 +23773,8 @@
       <c r="AF81" s="937"/>
     </row>
     <row r="82" spans="1:32" s="315" customFormat="1" ht="69" customHeight="1">
-      <c r="A82" s="978"/>
-      <c r="B82" s="979"/>
+      <c r="A82" s="959"/>
+      <c r="B82" s="960"/>
       <c r="C82" s="326" t="s">
         <v>580</v>
       </c>
@@ -23820,8 +23820,8 @@
       <c r="AF82" s="937"/>
     </row>
     <row r="83" spans="1:32" s="315" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A83" s="978"/>
-      <c r="B83" s="979"/>
+      <c r="A83" s="959"/>
+      <c r="B83" s="960"/>
       <c r="C83" s="319" t="s">
         <v>394</v>
       </c>
@@ -23867,8 +23867,8 @@
       <c r="AF83" s="937"/>
     </row>
     <row r="84" spans="1:32" s="315" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A84" s="978"/>
-      <c r="B84" s="979"/>
+      <c r="A84" s="959"/>
+      <c r="B84" s="960"/>
       <c r="C84" s="319" t="s">
         <v>664</v>
       </c>
@@ -23916,8 +23916,8 @@
       <c r="AF84" s="937"/>
     </row>
     <row r="85" spans="1:32" s="276" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A85" s="978"/>
-      <c r="B85" s="979"/>
+      <c r="A85" s="959"/>
+      <c r="B85" s="960"/>
       <c r="C85" s="326" t="s">
         <v>396</v>
       </c>
@@ -24916,27 +24916,6 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="A79:A85"/>
-    <mergeCell ref="B79:B85"/>
-    <mergeCell ref="A59:A78"/>
-    <mergeCell ref="B59:B78"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="T24:T26"/>
-    <mergeCell ref="T61:T75"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="E27:E29"/>
     <mergeCell ref="AD1:AD2"/>
     <mergeCell ref="AF1:AF2"/>
     <mergeCell ref="A7:A8"/>
@@ -24953,6 +24932,27 @@
     <mergeCell ref="G1:L1"/>
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="N1:N2"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="T24:T26"/>
+    <mergeCell ref="T61:T75"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="A79:A85"/>
+    <mergeCell ref="B79:B85"/>
+    <mergeCell ref="A59:A78"/>
+    <mergeCell ref="B59:B78"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="X1:X2"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7 G89:M93 E86:E88 R83:R84 C33:M39 C12:D24 C40:C41 G31:M32 E24 R62:R78 E12:E20 F12:F24 R33:R38 G44:M49 E47 C83:C84 C59:F78 G79:M85 G27:M27 C7:F11 G59:M61 D40:M43 C31:F31 A59:A61" xr:uid="{00000000-0002-0000-0500-000000000000}">
@@ -24985,7 +24985,7 @@
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="P1" sqref="P1:P1048576"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -25129,11 +25129,11 @@
       <c r="M3" s="243"/>
     </row>
     <row r="4" spans="1:33" ht="19.5" customHeight="1">
-      <c r="A4" s="991" t="s">
+      <c r="A4" s="993" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="991"/>
-      <c r="C4" s="991"/>
+      <c r="B4" s="993"/>
+      <c r="C4" s="993"/>
       <c r="D4" s="243"/>
       <c r="E4" s="243"/>
       <c r="F4" s="243"/>
@@ -25151,9 +25151,9 @@
       <c r="AG4" s="3"/>
     </row>
     <row r="5" spans="1:33" s="1" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A5" s="990"/>
-      <c r="B5" s="990"/>
-      <c r="C5" s="990"/>
+      <c r="A5" s="992"/>
+      <c r="B5" s="992"/>
+      <c r="C5" s="992"/>
       <c r="D5" s="113"/>
       <c r="E5" s="270"/>
       <c r="F5" s="270"/>
@@ -26909,7 +26909,7 @@
         <v>283</v>
       </c>
       <c r="D40" s="183"/>
-      <c r="E40" s="992"/>
+      <c r="E40" s="990"/>
       <c r="F40" s="273"/>
       <c r="G40" s="404" t="s">
         <v>10</v>
@@ -26967,7 +26967,7 @@
         <v>414</v>
       </c>
       <c r="D41" s="273"/>
-      <c r="E41" s="962"/>
+      <c r="E41" s="974"/>
       <c r="F41" s="273"/>
       <c r="G41" s="370"/>
       <c r="H41" s="370"/>
@@ -27000,7 +27000,7 @@
         <v>415</v>
       </c>
       <c r="D42" s="273"/>
-      <c r="E42" s="962"/>
+      <c r="E42" s="974"/>
       <c r="F42" s="273"/>
       <c r="G42" s="370"/>
       <c r="H42" s="370"/>
@@ -27034,7 +27034,7 @@
         <v>658</v>
       </c>
       <c r="D43" s="273"/>
-      <c r="E43" s="993"/>
+      <c r="E43" s="991"/>
       <c r="F43" s="273"/>
       <c r="G43" s="369"/>
       <c r="H43" s="369"/>
@@ -27896,6 +27896,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="AE1:AE2"/>
+    <mergeCell ref="AG1:AG2"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="G1:L1"/>
     <mergeCell ref="E40:E43"/>
     <mergeCell ref="R1:R2"/>
     <mergeCell ref="T1:T2"/>
@@ -27903,13 +27910,6 @@
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="V1:V2"/>
-    <mergeCell ref="AE1:AE2"/>
-    <mergeCell ref="AG1:AG2"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="G1:L1"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G15:M15 G40:M44 G30:M37 E38:E39 G56:K60" xr:uid="{00000000-0002-0000-0600-000000000000}">
@@ -28074,11 +28074,11 @@
       <c r="AF2" s="948"/>
     </row>
     <row r="4" spans="1:32" ht="15">
-      <c r="A4" s="991" t="s">
+      <c r="A4" s="993" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="991"/>
-      <c r="C4" s="991"/>
+      <c r="B4" s="993"/>
+      <c r="C4" s="993"/>
       <c r="AD4" s="3"/>
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
@@ -29050,10 +29050,10 @@
       <c r="AF2" s="948"/>
     </row>
     <row r="4" spans="1:32" ht="15">
-      <c r="A4" s="991" t="s">
+      <c r="A4" s="993" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="991"/>
+      <c r="B4" s="993"/>
       <c r="AD4" s="3"/>
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>

</xml_diff>

<commit_message>
calling data for all array  with N values
</commit_message>
<xml_diff>
--- a/xlsx/BMW_Sales_Standards_2016_ME.xlsx
+++ b/xlsx/BMW_Sales_Standards_2016_ME.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12708" yWindow="348" windowWidth="2688" windowHeight="7440" tabRatio="870" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12708" yWindow="348" windowWidth="2688" windowHeight="7440" tabRatio="870" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="21" r:id="rId1"/>
@@ -27,9 +27,10 @@
     <sheet name="Section 10_Business Corp Sales" sheetId="11" r:id="rId13"/>
     <sheet name="BMW Outlet Size Scaling" sheetId="12" r:id="rId14"/>
     <sheet name="Brand Architecture Elements" sheetId="13" r:id="rId15"/>
+    <sheet name="Sheet1" sheetId="31" r:id="rId16"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId16"/>
+    <externalReference r:id="rId17"/>
   </externalReferences>
   <definedNames>
     <definedName name="Auswahl">#REF!</definedName>
@@ -10797,7 +10798,7 @@
     <sheetView showGridLines="0" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z14" sqref="Z14"/>
-      <selection pane="bottomLeft" activeCell="AF22" sqref="AF22"/>
+      <selection pane="bottomLeft" activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -11168,12 +11169,12 @@
       <c r="V9" s="267"/>
       <c r="W9" s="315"/>
       <c r="X9" s="590" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="Y9" s="425"/>
       <c r="Z9" s="600">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA9" s="315"/>
       <c r="AB9" s="807" t="s">
@@ -13067,10 +13068,10 @@
   </sheetPr>
   <dimension ref="A1:AF20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="F1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="F1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z14" sqref="Z14"/>
-      <selection pane="bottomLeft" activeCell="X9" sqref="X9"/>
+      <selection pane="bottomLeft" activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -13283,12 +13284,12 @@
       </c>
       <c r="W6" s="315"/>
       <c r="X6" s="590" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="Y6" s="425"/>
       <c r="Z6" s="945">
         <f>IF(OR(X6="A",X7="A",X8="A"),"",IF(OR(X6="N",X7="N",X8="N"),0,1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA6" s="315"/>
       <c r="AB6" s="800" t="s">
@@ -16288,6 +16289,18 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D5CB58D-67F9-43C6-88CB-7F2BC3E80913}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Tabelle1">
@@ -16930,11 +16943,11 @@
       </c>
       <c r="F20" s="640">
         <f>SUM('Section 4_Customer Area'!Z6:Z60)-SUMIF('Section 4_Customer Area'!P6:P60,"O",'Section 4_Customer Area'!Z6:Z60)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H20" s="641">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="J20" s="640">
         <f>COUNTIFS('Section 4_Customer Area'!P6:P60,"X",'Section 4_Customer Area'!Z6:Z60,1)+COUNTIFS('Section 4_Customer Area'!P6:P60,"X",'Section 4_Customer Area'!Z6:Z60,0)</f>
@@ -16943,12 +16956,12 @@
       <c r="K20"/>
       <c r="L20" s="640">
         <f>SUMIF('Section 4_Customer Area'!P6:P60,"X",'Section 4_Customer Area'!Z6:Z60)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M20" s="633"/>
       <c r="N20" s="641">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="O20" s="633"/>
       <c r="P20" s="771"/>
@@ -16963,11 +16976,11 @@
       </c>
       <c r="F21" s="640">
         <f>SUM('Section 5_IT'!Z6:Z14)-SUMIF('Section 5_IT'!P6:P14,"O",'Section 5_IT'!Z6:Z14)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H21" s="641">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="J21" s="640">
         <f>COUNTIFS('Section 5_IT'!P6:P14,"X",'Section 5_IT'!Z6:Z14,1)+COUNTIFS('Section 5_IT'!P6:P14,"X",'Section 5_IT'!Z6:Z14,0)</f>
@@ -17062,11 +17075,11 @@
       </c>
       <c r="F24" s="640">
         <f>SUM('Section 8_Customer Processes'!Z6:Z38)-SUMIF('Section 8_Customer Processes'!P6:P38,"O",'Section 8_Customer Processes'!Z6:Z38)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H24" s="641">
         <f t="shared" si="1"/>
-        <v>0.95833333333333337</v>
+        <v>1</v>
       </c>
       <c r="J24" s="640">
         <f>COUNTIFS('Section 8_Customer Processes'!P6:P38,"X",'Section 8_Customer Processes'!Z6:Z38,1)+COUNTIFS('Section 8_Customer Processes'!P6:P38,"X",'Section 8_Customer Processes'!Z6:Z38,0)</f>
@@ -17075,12 +17088,12 @@
       <c r="K24"/>
       <c r="L24" s="640">
         <f>SUMIF('Section 8_Customer Processes'!P6:P38,"X",'Section 8_Customer Processes'!Z6:Z38)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M24" s="633"/>
       <c r="N24" s="641">
         <f t="shared" si="0"/>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="O24" s="633"/>
       <c r="P24" s="772"/>
@@ -17095,11 +17108,11 @@
       </c>
       <c r="F25" s="640">
         <f>SUM('Section 9_Marketing'!Z6:Z20)-SUMIF('Section 9_Marketing'!P6:P20,"O",'Section 9_Marketing'!Z6:Z20)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H25" s="641">
         <f t="shared" si="1"/>
-        <v>0.83333333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="J25" s="640">
         <f>COUNTIFS('Section 9_Marketing'!P6:P20,"X",'Section 9_Marketing'!Z6:Z20,1)+COUNTIFS('Section 9_Marketing'!P6:P20,"X",'Section 9_Marketing'!Z6:Z20,0)</f>
@@ -17166,12 +17179,12 @@
       <c r="E28" s="625"/>
       <c r="F28" s="624">
         <f>SUM(F17:F26)</f>
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G28" s="625"/>
       <c r="H28" s="626">
         <f>IFERROR(F28/D28,0%)</f>
-        <v>0.96703296703296704</v>
+        <v>0.93406593406593408</v>
       </c>
       <c r="I28" s="625"/>
       <c r="J28" s="627">
@@ -20044,7 +20057,7 @@
     <sheetView showGridLines="0" topLeftCell="Q1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="P1" sqref="P1:P1048576"/>
-      <selection pane="bottomLeft" activeCell="Z56" sqref="Z56"/>
+      <selection pane="bottomLeft" activeCell="X56" sqref="X56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -24985,7 +24998,7 @@
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="P1" sqref="P1:P1048576"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="X8" sqref="X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -25211,12 +25224,12 @@
       </c>
       <c r="W6" s="346"/>
       <c r="X6" s="582" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="Y6" s="346"/>
       <c r="Z6" s="582">
         <f>IF(OR(X6="A",X10="A"),"",IF(OR(X6="N",X10="N"),0,1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB6" s="801" t="s">
         <v>639</v>
@@ -27940,10 +27953,10 @@
   </sheetPr>
   <dimension ref="A1:AF61"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z14" sqref="Z14"/>
-      <selection pane="bottomLeft" activeCell="AD1" sqref="AD1:AF1048576"/>
+      <selection pane="bottomLeft" activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -28163,7 +28176,7 @@
       <c r="Y6" s="425"/>
       <c r="Z6" s="600">
         <f>IF(OR(X6="A",X7="A"),"",IF(OR(X6="N",X7="N"),0,1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA6" s="757"/>
       <c r="AB6" s="800" t="s">
@@ -28208,7 +28221,7 @@
       </c>
       <c r="W7" s="397"/>
       <c r="X7" s="590" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="Y7" s="425"/>
       <c r="Z7" s="601"/>
@@ -28304,12 +28317,12 @@
       <c r="V9" s="267"/>
       <c r="W9" s="315"/>
       <c r="X9" s="590" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="Y9" s="425"/>
       <c r="Z9" s="600">
         <f t="shared" ref="Z9:Z13" si="0">IF(OR(X9="A"),"",IF(OR(X9="N"),0,1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA9" s="770"/>
       <c r="AB9" s="807" t="s">

</xml_diff>

<commit_message>
Filter all excel file
</commit_message>
<xml_diff>
--- a/xlsx/BMW_Sales_Standards_2016_ME.xlsx
+++ b/xlsx/BMW_Sales_Standards_2016_ME.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12708" yWindow="348" windowWidth="2688" windowHeight="7440" tabRatio="870" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12708" yWindow="348" windowWidth="2688" windowHeight="7440" tabRatio="870" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="21" r:id="rId1"/>
@@ -9209,9 +9209,9 @@
   <dimension ref="A1:AF61"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z14" sqref="Z14"/>
-      <selection pane="bottomLeft" activeCell="R37" sqref="R37"/>
+      <selection pane="bottomLeft" activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -10247,7 +10247,7 @@
       <c r="Y22" s="425"/>
       <c r="Z22" s="600">
         <f>IF(OR(X22="A",X23="A"),"",IF(OR(X22="N",X23="N"),0,1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA22" s="379"/>
       <c r="AB22" s="801" t="s">
@@ -10286,7 +10286,7 @@
       <c r="V23" s="400"/>
       <c r="W23" s="379"/>
       <c r="X23" s="590" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="Y23" s="425"/>
       <c r="Z23" s="603"/>
@@ -10796,9 +10796,9 @@
   <dimension ref="A1:AF39"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z14" sqref="Z14"/>
-      <selection pane="bottomLeft" activeCell="X6" sqref="X6"/>
+      <selection pane="bottomLeft" activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -13069,9 +13069,9 @@
   <dimension ref="A1:AF20"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="F1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z14" sqref="Z14"/>
-      <selection pane="bottomLeft" activeCell="X6" sqref="X6"/>
+      <selection pane="bottomLeft" activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -13363,7 +13363,7 @@
       </c>
       <c r="W8" s="315"/>
       <c r="X8" s="590" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="Y8" s="315"/>
       <c r="Z8" s="942"/>
@@ -14037,7 +14037,7 @@
   <dimension ref="A1:AF16"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z14" sqref="Z14"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
@@ -16910,11 +16910,11 @@
       </c>
       <c r="F19" s="640">
         <f>SUM('Section 3_Sales Area'!Z7:Z101)-SUMIF('Section 3_Sales Area'!P7:P101,"O",'Section 3_Sales Area'!Z7:Z101)</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H19" s="641">
         <f t="shared" si="1"/>
-        <v>0.96296296296296291</v>
+        <v>1</v>
       </c>
       <c r="J19" s="640">
         <f>COUNTIFS('Section 3_Sales Area'!P7:P101,"X",'Section 3_Sales Area'!Z7:Z101,1)+COUNTIFS('Section 3_Sales Area'!P7:P101,"X",'Section 3_Sales Area'!Z7:Z101,0)</f>
@@ -16923,12 +16923,12 @@
       <c r="K19"/>
       <c r="L19" s="640">
         <f>SUMIF('Section 3_Sales Area'!P7:P101,"X",'Section 3_Sales Area'!Z7:Z101)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M19" s="633"/>
       <c r="N19" s="641">
         <f t="shared" si="0"/>
-        <v>0.9285714285714286</v>
+        <v>1</v>
       </c>
       <c r="O19" s="633"/>
       <c r="P19" s="771"/>
@@ -16976,11 +16976,11 @@
       </c>
       <c r="F21" s="640">
         <f>SUM('Section 5_IT'!Z6:Z14)-SUMIF('Section 5_IT'!P6:P14,"O",'Section 5_IT'!Z6:Z14)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H21" s="641">
         <f t="shared" si="1"/>
-        <v>0.7142857142857143</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="J21" s="640">
         <f>COUNTIFS('Section 5_IT'!P6:P14,"X",'Section 5_IT'!Z6:Z14,1)+COUNTIFS('Section 5_IT'!P6:P14,"X",'Section 5_IT'!Z6:Z14,0)</f>
@@ -17042,11 +17042,11 @@
       </c>
       <c r="F23" s="640">
         <f>SUM('Section 7_Personnel  Training'!Z6:Z28)-SUMIF('Section 7_Personnel  Training'!P6:P28,"O",'Section 7_Personnel  Training'!Z6:Z28)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H23" s="641">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="J23" s="640">
         <f>COUNTIFS('Section 7_Personnel  Training'!P6:P28,"X",'Section 7_Personnel  Training'!Z6:Z28,1)+COUNTIFS('Section 7_Personnel  Training'!P6:P28,"X",'Section 7_Personnel  Training'!Z6:Z28,0)</f>
@@ -17179,12 +17179,12 @@
       <c r="E28" s="625"/>
       <c r="F28" s="624">
         <f>SUM(F17:F26)</f>
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G28" s="625"/>
       <c r="H28" s="626">
         <f>IFERROR(F28/D28,0%)</f>
-        <v>0.93406593406593408</v>
+        <v>0.94505494505494503</v>
       </c>
       <c r="I28" s="625"/>
       <c r="J28" s="627">
@@ -17194,12 +17194,12 @@
       <c r="K28" s="625"/>
       <c r="L28" s="627">
         <f>SUM(L17:L26)</f>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M28" s="625"/>
       <c r="N28" s="628">
         <f>IFERROR(L28/J28,0%)</f>
-        <v>0.90909090909090906</v>
+        <v>0.93939393939393945</v>
       </c>
       <c r="O28" s="625"/>
       <c r="P28" s="625"/>
@@ -20054,10 +20054,10 @@
   </sheetPr>
   <dimension ref="A1:AF101"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="Q1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="P1" sqref="P1:P1048576"/>
-      <selection pane="bottomLeft" activeCell="X56" sqref="X56"/>
+      <selection pane="bottomLeft" activeCell="N51" sqref="N51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -22723,8 +22723,7 @@
       </c>
       <c r="Y55" s="315"/>
       <c r="Z55" s="582">
-        <f>IF(OR(X55="A",X56="A",X57="A",X58="A"),"",IF(OR(X55="N",X56="N",X57="N",X58="N"),0,1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA55" s="761"/>
       <c r="AB55" s="787" t="s">
@@ -27953,10 +27952,10 @@
   </sheetPr>
   <dimension ref="A1:AF61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z14" sqref="Z14"/>
-      <selection pane="bottomLeft" activeCell="Q8" sqref="Q8"/>
+      <selection pane="bottomLeft" activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -28176,7 +28175,7 @@
       <c r="Y6" s="425"/>
       <c r="Z6" s="600">
         <f>IF(OR(X6="A",X7="A"),"",IF(OR(X6="N",X7="N"),0,1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA6" s="757"/>
       <c r="AB6" s="800" t="s">
@@ -28221,7 +28220,7 @@
       </c>
       <c r="W7" s="397"/>
       <c r="X7" s="590" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="Y7" s="425"/>
       <c r="Z7" s="601"/>
@@ -28931,9 +28930,9 @@
   <dimension ref="A1:AF61"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z14" sqref="Z14"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
It string contains specific word
</commit_message>
<xml_diff>
--- a/xlsx/BMW_Sales_Standards_2016_ME.xlsx
+++ b/xlsx/BMW_Sales_Standards_2016_ME.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12708" yWindow="348" windowWidth="2688" windowHeight="7440" tabRatio="870" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12708" yWindow="348" windowWidth="2688" windowHeight="7440" tabRatio="870" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="21" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2869" uniqueCount="1018">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2869" uniqueCount="1019">
   <si>
     <t>Standard</t>
   </si>
@@ -3764,6 +3764,9 @@
   </si>
   <si>
     <t>No Audit</t>
+  </si>
+  <si>
+    <t>Audit / Regional Office or Importer</t>
   </si>
 </sst>
 </file>
@@ -7960,123 +7963,144 @@
     <xf numFmtId="0" fontId="56" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="63" fillId="3" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="71" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="71" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="2" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="63" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="72" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="2" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="71" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="71" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="68" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="71" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="71" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="71" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="68" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="68" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="68" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="71" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="71" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="71" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="71" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="67" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="65" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="71" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="71" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="68" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="71" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="71" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="71" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="68" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="68" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="68" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="71" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="71" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="71" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="71" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="69" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="69" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="69" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="2" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="75" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="75" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="63" fillId="3" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="63" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="71" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="71" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="2" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="63" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="56" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="56" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -8094,27 +8118,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="18" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -11369,11 +11372,11 @@
       <c r="AF2" s="894"/>
     </row>
     <row r="4" spans="1:32" ht="15.6">
-      <c r="A4" s="949" t="s">
+      <c r="A4" s="943" t="s">
         <v>155</v>
       </c>
-      <c r="B4" s="949"/>
-      <c r="C4" s="949"/>
+      <c r="B4" s="943"/>
+      <c r="C4" s="943"/>
       <c r="AD4" s="3"/>
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
@@ -11693,34 +11696,34 @@
       <c r="AF10" s="573"/>
     </row>
     <row r="11" spans="1:32" s="1" customFormat="1" ht="191.25" customHeight="1">
-      <c r="A11" s="950" t="s">
+      <c r="A11" s="944" t="s">
         <v>107</v>
       </c>
-      <c r="B11" s="953" t="s">
+      <c r="B11" s="947" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="943" t="s">
+      <c r="C11" s="950" t="s">
         <v>988</v>
       </c>
       <c r="D11" s="114"/>
-      <c r="E11" s="943"/>
+      <c r="E11" s="950"/>
       <c r="F11" s="114"/>
-      <c r="G11" s="946" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="946" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="946" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" s="946" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" s="946" t="s">
-        <v>10</v>
-      </c>
-      <c r="L11" s="946" t="s">
+      <c r="G11" s="953" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="953" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="953" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="953" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="953" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" s="953" t="s">
         <v>10</v>
       </c>
       <c r="M11" s="110"/>
@@ -11756,18 +11759,18 @@
       <c r="AF11" s="573"/>
     </row>
     <row r="12" spans="1:32" s="1" customFormat="1" ht="13.8">
-      <c r="A12" s="951"/>
-      <c r="B12" s="954"/>
-      <c r="C12" s="944"/>
+      <c r="A12" s="945"/>
+      <c r="B12" s="948"/>
+      <c r="C12" s="951"/>
       <c r="D12" s="114"/>
-      <c r="E12" s="944"/>
+      <c r="E12" s="951"/>
       <c r="F12" s="114"/>
-      <c r="G12" s="947"/>
-      <c r="H12" s="947"/>
-      <c r="I12" s="947"/>
-      <c r="J12" s="947"/>
-      <c r="K12" s="947"/>
-      <c r="L12" s="947"/>
+      <c r="G12" s="954"/>
+      <c r="H12" s="954"/>
+      <c r="I12" s="954"/>
+      <c r="J12" s="954"/>
+      <c r="K12" s="954"/>
+      <c r="L12" s="954"/>
       <c r="M12" s="111"/>
       <c r="N12" s="165"/>
       <c r="P12" s="555"/>
@@ -11788,18 +11791,18 @@
       <c r="AF12" s="573"/>
     </row>
     <row r="13" spans="1:32" s="1" customFormat="1" ht="13.8">
-      <c r="A13" s="951"/>
-      <c r="B13" s="954"/>
-      <c r="C13" s="944"/>
+      <c r="A13" s="945"/>
+      <c r="B13" s="948"/>
+      <c r="C13" s="951"/>
       <c r="D13" s="114"/>
-      <c r="E13" s="944"/>
+      <c r="E13" s="951"/>
       <c r="F13" s="114"/>
-      <c r="G13" s="947"/>
-      <c r="H13" s="947"/>
-      <c r="I13" s="947"/>
-      <c r="J13" s="947"/>
-      <c r="K13" s="947"/>
-      <c r="L13" s="947"/>
+      <c r="G13" s="954"/>
+      <c r="H13" s="954"/>
+      <c r="I13" s="954"/>
+      <c r="J13" s="954"/>
+      <c r="K13" s="954"/>
+      <c r="L13" s="954"/>
       <c r="M13" s="111"/>
       <c r="N13" s="165"/>
       <c r="P13" s="555"/>
@@ -11820,18 +11823,18 @@
       <c r="AF13" s="573"/>
     </row>
     <row r="14" spans="1:32" s="1" customFormat="1" ht="35.25" customHeight="1">
-      <c r="A14" s="952"/>
-      <c r="B14" s="955"/>
-      <c r="C14" s="945"/>
+      <c r="A14" s="946"/>
+      <c r="B14" s="949"/>
+      <c r="C14" s="952"/>
       <c r="D14" s="114"/>
-      <c r="E14" s="945"/>
+      <c r="E14" s="952"/>
       <c r="F14" s="114"/>
-      <c r="G14" s="948"/>
-      <c r="H14" s="948"/>
-      <c r="I14" s="948"/>
-      <c r="J14" s="948"/>
-      <c r="K14" s="948"/>
-      <c r="L14" s="948"/>
+      <c r="G14" s="955"/>
+      <c r="H14" s="955"/>
+      <c r="I14" s="955"/>
+      <c r="J14" s="955"/>
+      <c r="K14" s="955"/>
+      <c r="L14" s="955"/>
       <c r="M14" s="104"/>
       <c r="N14" s="170"/>
       <c r="P14" s="554"/>
@@ -13461,17 +13464,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="AD1:AD2"/>
-    <mergeCell ref="AF1:AF2"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="R1:R2"/>
     <mergeCell ref="T1:T2"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="K11:K14"/>
@@ -13483,6 +13475,17 @@
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="G1:L1"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="AD1:AD2"/>
+    <mergeCell ref="AF1:AF2"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="X1:X2"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:M11 G15:M22 G24:M37 G38:N38" xr:uid="{00000000-0002-0000-0A00-000000000000}">
@@ -13515,7 +13518,7 @@
     <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="F1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z14" sqref="Z14"/>
-      <selection pane="bottomLeft" activeCell="N19" sqref="N19"/>
+      <selection pane="bottomLeft" activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -13957,7 +13960,7 @@
       </c>
       <c r="M11" s="110"/>
       <c r="N11" s="580" t="s">
-        <v>773</v>
+        <v>1018</v>
       </c>
       <c r="P11" s="580" t="s">
         <v>815</v>
@@ -17453,11 +17456,11 @@
       </c>
       <c r="F22" s="415">
         <f>SUM('Section 6_Management'!Z6:Z14)-SUMIF('Section 6_Management'!P6:P14,"O",'Section 6_Management'!Z6:Z14)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H22" s="416">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="J22" s="415">
         <f>COUNTIFS('Section 6_Management'!P6:P14,"X",'Section 6_Management'!Z6:Z14,1)+COUNTIFS('Section 6_Management'!P6:P14,"X",'Section 6_Management'!Z6:Z14,0)</f>
@@ -17466,12 +17469,12 @@
       <c r="K22"/>
       <c r="L22" s="415">
         <f>SUMIF('Section 6_Management'!P6:P14,"X",'Section 6_Management'!Z6:Z14)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M22" s="408"/>
       <c r="N22" s="416">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O22" s="408"/>
       <c r="P22" s="478"/>
@@ -17623,12 +17626,12 @@
       <c r="E28" s="400"/>
       <c r="F28" s="399">
         <f>SUM(F17:F26)</f>
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G28" s="400"/>
       <c r="H28" s="401">
         <f>IFERROR(F28/D28,0%)</f>
-        <v>0.94505494505494503</v>
+        <v>0.93406593406593408</v>
       </c>
       <c r="I28" s="400"/>
       <c r="J28" s="402">
@@ -17638,12 +17641,12 @@
       <c r="K28" s="400"/>
       <c r="L28" s="402">
         <f>SUM(L17:L26)</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M28" s="400"/>
       <c r="N28" s="403">
         <f>IFERROR(L28/J28,0%)</f>
-        <v>0.93939393939393945</v>
+        <v>0.90909090909090906</v>
       </c>
       <c r="O28" s="400"/>
       <c r="P28" s="400"/>
@@ -20550,46 +20553,46 @@
         <v>191</v>
       </c>
       <c r="F1" s="585"/>
-      <c r="G1" s="941" t="s">
+      <c r="G1" s="914" t="s">
         <v>742</v>
       </c>
-      <c r="H1" s="941"/>
-      <c r="I1" s="941"/>
-      <c r="J1" s="941"/>
-      <c r="K1" s="941"/>
-      <c r="L1" s="941"/>
+      <c r="H1" s="914"/>
+      <c r="I1" s="914"/>
+      <c r="J1" s="914"/>
+      <c r="K1" s="914"/>
+      <c r="L1" s="914"/>
       <c r="M1" s="586"/>
-      <c r="N1" s="904" t="s">
+      <c r="N1" s="915" t="s">
         <v>190</v>
       </c>
-      <c r="P1" s="904" t="s">
+      <c r="P1" s="915" t="s">
         <v>193</v>
       </c>
-      <c r="R1" s="904" t="s">
+      <c r="R1" s="915" t="s">
         <v>218</v>
       </c>
       <c r="S1" s="588"/>
-      <c r="T1" s="904" t="s">
+      <c r="T1" s="915" t="s">
         <v>241</v>
       </c>
-      <c r="V1" s="904" t="s">
+      <c r="V1" s="915" t="s">
         <v>242</v>
       </c>
-      <c r="X1" s="904" t="s">
+      <c r="X1" s="915" t="s">
         <v>219</v>
       </c>
-      <c r="Z1" s="904" t="s">
+      <c r="Z1" s="915" t="s">
         <v>243</v>
       </c>
       <c r="AA1" s="585"/>
-      <c r="AB1" s="906" t="s">
+      <c r="AB1" s="941" t="s">
         <v>738</v>
       </c>
       <c r="AC1" s="589"/>
-      <c r="AD1" s="933" t="s">
+      <c r="AD1" s="904" t="s">
         <v>980</v>
       </c>
-      <c r="AF1" s="934" t="s">
+      <c r="AF1" s="905" t="s">
         <v>981</v>
       </c>
     </row>
@@ -20619,19 +20622,19 @@
         <v>7</v>
       </c>
       <c r="M2" s="594"/>
-      <c r="N2" s="904"/>
-      <c r="P2" s="904"/>
-      <c r="R2" s="904"/>
+      <c r="N2" s="915"/>
+      <c r="P2" s="915"/>
+      <c r="R2" s="915"/>
       <c r="S2" s="588"/>
-      <c r="T2" s="904"/>
-      <c r="V2" s="904"/>
-      <c r="X2" s="904"/>
-      <c r="Z2" s="904"/>
+      <c r="T2" s="915"/>
+      <c r="V2" s="915"/>
+      <c r="X2" s="915"/>
+      <c r="Z2" s="915"/>
       <c r="AA2" s="585"/>
-      <c r="AB2" s="906"/>
+      <c r="AB2" s="941"/>
       <c r="AC2" s="589"/>
-      <c r="AD2" s="933"/>
-      <c r="AF2" s="934"/>
+      <c r="AD2" s="904"/>
+      <c r="AF2" s="905"/>
     </row>
     <row r="4" spans="1:32">
       <c r="AD4" s="587"/>
@@ -20639,11 +20642,11 @@
       <c r="AF4" s="587"/>
     </row>
     <row r="5" spans="1:32" s="601" customFormat="1" ht="15">
-      <c r="A5" s="905" t="s">
+      <c r="A5" s="940" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="905"/>
-      <c r="C5" s="905"/>
+      <c r="B5" s="940"/>
+      <c r="C5" s="940"/>
       <c r="D5" s="598"/>
       <c r="E5" s="598"/>
       <c r="F5" s="598"/>
@@ -20687,17 +20690,17 @@
       <c r="AF6" s="587"/>
     </row>
     <row r="7" spans="1:32" s="601" customFormat="1" ht="115.5" customHeight="1">
-      <c r="A7" s="935" t="s">
+      <c r="A7" s="906" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="935" t="s">
+      <c r="B7" s="906" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="922" t="s">
+      <c r="C7" s="911" t="s">
         <v>1008</v>
       </c>
       <c r="D7" s="605"/>
-      <c r="E7" s="922"/>
+      <c r="E7" s="911"/>
       <c r="F7" s="605"/>
       <c r="G7" s="606" t="s">
         <v>10</v>
@@ -20750,11 +20753,11 @@
       <c r="AF7" s="616"/>
     </row>
     <row r="8" spans="1:32" s="601" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A8" s="936"/>
-      <c r="B8" s="936"/>
-      <c r="C8" s="923"/>
+      <c r="A8" s="907"/>
+      <c r="B8" s="907"/>
+      <c r="C8" s="910"/>
       <c r="D8" s="617"/>
-      <c r="E8" s="923"/>
+      <c r="E8" s="910"/>
       <c r="F8" s="617"/>
       <c r="G8" s="618"/>
       <c r="H8" s="618"/>
@@ -20782,13 +20785,13 @@
       <c r="AF8" s="616"/>
     </row>
     <row r="9" spans="1:32" s="601" customFormat="1" ht="45.6">
-      <c r="A9" s="936"/>
-      <c r="B9" s="936"/>
-      <c r="C9" s="923" t="s">
+      <c r="A9" s="907"/>
+      <c r="B9" s="907"/>
+      <c r="C9" s="910" t="s">
         <v>675</v>
       </c>
       <c r="D9" s="617"/>
-      <c r="E9" s="923"/>
+      <c r="E9" s="910"/>
       <c r="F9" s="617"/>
       <c r="G9" s="618" t="s">
         <v>10</v>
@@ -20833,11 +20836,11 @@
       <c r="AF9" s="616"/>
     </row>
     <row r="10" spans="1:32" s="601" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A10" s="936"/>
-      <c r="B10" s="936"/>
-      <c r="C10" s="923"/>
+      <c r="A10" s="907"/>
+      <c r="B10" s="907"/>
+      <c r="C10" s="910"/>
       <c r="D10" s="617"/>
-      <c r="E10" s="923"/>
+      <c r="E10" s="910"/>
       <c r="F10" s="617"/>
       <c r="G10" s="618" t="s">
         <v>10</v>
@@ -21105,7 +21108,7 @@
         <v>745</v>
       </c>
       <c r="D16" s="650"/>
-      <c r="E16" s="939"/>
+      <c r="E16" s="912"/>
       <c r="F16" s="650"/>
       <c r="G16" s="651" t="s">
         <v>10</v>
@@ -21156,7 +21159,7 @@
         <v>744</v>
       </c>
       <c r="D17" s="657"/>
-      <c r="E17" s="940"/>
+      <c r="E17" s="913"/>
       <c r="F17" s="657"/>
       <c r="G17" s="658"/>
       <c r="H17" s="658"/>
@@ -21194,10 +21197,10 @@
       <c r="AF17" s="616"/>
     </row>
     <row r="18" spans="1:32" s="601" customFormat="1" ht="53.25" customHeight="1">
-      <c r="A18" s="935" t="s">
+      <c r="A18" s="906" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="935" t="s">
+      <c r="B18" s="906" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="638" t="s">
@@ -21257,8 +21260,8 @@
       <c r="AF18" s="616"/>
     </row>
     <row r="19" spans="1:32" s="601" customFormat="1" ht="50.25" customHeight="1">
-      <c r="A19" s="936"/>
-      <c r="B19" s="936"/>
+      <c r="A19" s="907"/>
+      <c r="B19" s="907"/>
       <c r="C19" s="632"/>
       <c r="D19" s="617"/>
       <c r="E19" s="632"/>
@@ -21289,13 +21292,13 @@
       <c r="AF19" s="665"/>
     </row>
     <row r="20" spans="1:32" s="601" customFormat="1" ht="87" customHeight="1">
-      <c r="A20" s="936"/>
-      <c r="B20" s="936"/>
+      <c r="A20" s="907"/>
+      <c r="B20" s="907"/>
       <c r="C20" s="632" t="s">
         <v>591</v>
       </c>
       <c r="D20" s="666"/>
-      <c r="E20" s="937"/>
+      <c r="E20" s="908"/>
       <c r="F20" s="666"/>
       <c r="G20" s="606"/>
       <c r="H20" s="667" t="s">
@@ -21337,7 +21340,7 @@
       <c r="B21" s="631"/>
       <c r="C21" s="632"/>
       <c r="D21" s="668"/>
-      <c r="E21" s="937"/>
+      <c r="E21" s="908"/>
       <c r="F21" s="668"/>
       <c r="G21" s="618"/>
       <c r="H21" s="618"/>
@@ -21369,7 +21372,7 @@
       <c r="B22" s="631"/>
       <c r="C22" s="632"/>
       <c r="D22" s="668"/>
-      <c r="E22" s="937"/>
+      <c r="E22" s="908"/>
       <c r="F22" s="668"/>
       <c r="G22" s="618"/>
       <c r="H22" s="618"/>
@@ -21401,7 +21404,7 @@
       <c r="B23" s="669"/>
       <c r="C23" s="670"/>
       <c r="D23" s="668"/>
-      <c r="E23" s="938"/>
+      <c r="E23" s="909"/>
       <c r="F23" s="668"/>
       <c r="G23" s="645"/>
       <c r="H23" s="645"/>
@@ -21429,17 +21432,17 @@
       <c r="AF23" s="665"/>
     </row>
     <row r="24" spans="1:32" s="601" customFormat="1" ht="96" customHeight="1">
-      <c r="A24" s="916" t="s">
+      <c r="A24" s="936" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="918" t="s">
+      <c r="B24" s="938" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="924" t="s">
+      <c r="C24" s="918" t="s">
         <v>500</v>
       </c>
       <c r="D24" s="617"/>
-      <c r="E24" s="924"/>
+      <c r="E24" s="918"/>
       <c r="F24" s="617"/>
       <c r="G24" s="618" t="s">
         <v>10</v>
@@ -21470,7 +21473,7 @@
         <v>293</v>
       </c>
       <c r="S24" s="609"/>
-      <c r="T24" s="925" t="s">
+      <c r="T24" s="919" t="s">
         <v>474</v>
       </c>
       <c r="V24" s="622" t="s">
@@ -21492,11 +21495,11 @@
       <c r="AF24" s="665"/>
     </row>
     <row r="25" spans="1:32" s="601" customFormat="1" ht="44.25" customHeight="1">
-      <c r="A25" s="917"/>
-      <c r="B25" s="919"/>
-      <c r="C25" s="922"/>
+      <c r="A25" s="937"/>
+      <c r="B25" s="939"/>
+      <c r="C25" s="911"/>
       <c r="D25" s="617"/>
-      <c r="E25" s="922"/>
+      <c r="E25" s="911"/>
       <c r="F25" s="617"/>
       <c r="G25" s="618"/>
       <c r="H25" s="618"/>
@@ -21511,7 +21514,7 @@
         <v>554</v>
       </c>
       <c r="S25" s="609"/>
-      <c r="T25" s="926"/>
+      <c r="T25" s="920"/>
       <c r="V25" s="622"/>
       <c r="X25" s="612" t="s">
         <v>610</v>
@@ -21543,7 +21546,7 @@
         <v>501</v>
       </c>
       <c r="S26" s="609"/>
-      <c r="T26" s="927"/>
+      <c r="T26" s="921"/>
       <c r="V26" s="622"/>
       <c r="X26" s="612" t="s">
         <v>610</v>
@@ -21562,11 +21565,11 @@
       <c r="B27" s="637" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="920" t="s">
+      <c r="C27" s="916" t="s">
         <v>1010</v>
       </c>
       <c r="D27" s="676"/>
-      <c r="E27" s="931"/>
+      <c r="E27" s="925"/>
       <c r="F27" s="676"/>
       <c r="G27" s="677">
         <v>3</v>
@@ -21621,9 +21624,9 @@
     <row r="28" spans="1:32" s="601" customFormat="1" ht="54.75" customHeight="1">
       <c r="A28" s="681"/>
       <c r="B28" s="682"/>
-      <c r="C28" s="921"/>
+      <c r="C28" s="917"/>
       <c r="D28" s="683"/>
-      <c r="E28" s="932"/>
+      <c r="E28" s="926"/>
       <c r="F28" s="683"/>
       <c r="G28" s="681"/>
       <c r="H28" s="681"/>
@@ -21653,9 +21656,9 @@
     <row r="29" spans="1:32" s="601" customFormat="1" ht="106.5" customHeight="1">
       <c r="A29" s="681"/>
       <c r="B29" s="682"/>
-      <c r="C29" s="921"/>
+      <c r="C29" s="917"/>
       <c r="D29" s="683"/>
-      <c r="E29" s="932"/>
+      <c r="E29" s="926"/>
       <c r="F29" s="683"/>
       <c r="G29" s="681"/>
       <c r="H29" s="681"/>
@@ -22456,7 +22459,7 @@
       <c r="AF43" s="665"/>
     </row>
     <row r="44" spans="1:32" s="601" customFormat="1" ht="62.25" customHeight="1">
-      <c r="A44" s="907" t="s">
+      <c r="A44" s="927" t="s">
         <v>808</v>
       </c>
       <c r="B44" s="772" t="s">
@@ -22507,7 +22510,7 @@
       <c r="AF44" s="665"/>
     </row>
     <row r="45" spans="1:32" s="601" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A45" s="908"/>
+      <c r="A45" s="928"/>
       <c r="B45" s="758"/>
       <c r="C45" s="719" t="s">
         <v>378</v>
@@ -22553,7 +22556,7 @@
       <c r="AF45" s="665"/>
     </row>
     <row r="46" spans="1:32" s="601" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A46" s="908"/>
+      <c r="A46" s="928"/>
       <c r="B46" s="758"/>
       <c r="C46" s="719" t="s">
         <v>379</v>
@@ -23154,10 +23157,10 @@
       <c r="AF58" s="665"/>
     </row>
     <row r="59" spans="1:32" s="601" customFormat="1" ht="67.5" customHeight="1">
-      <c r="A59" s="910" t="s">
+      <c r="A59" s="930" t="s">
         <v>572</v>
       </c>
-      <c r="B59" s="913" t="s">
+      <c r="B59" s="933" t="s">
         <v>210</v>
       </c>
       <c r="C59" s="797" t="s">
@@ -23219,8 +23222,8 @@
       <c r="AF59" s="665"/>
     </row>
     <row r="60" spans="1:32" s="601" customFormat="1" ht="33" customHeight="1">
-      <c r="A60" s="911"/>
-      <c r="B60" s="914"/>
+      <c r="A60" s="931"/>
+      <c r="B60" s="934"/>
       <c r="C60" s="803"/>
       <c r="D60" s="804"/>
       <c r="E60" s="803"/>
@@ -23255,8 +23258,8 @@
       <c r="AF60" s="665"/>
     </row>
     <row r="61" spans="1:32" s="601" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A61" s="911"/>
-      <c r="B61" s="914"/>
+      <c r="A61" s="931"/>
+      <c r="B61" s="934"/>
       <c r="C61" s="809" t="s">
         <v>573</v>
       </c>
@@ -23277,7 +23280,7 @@
         <v>578</v>
       </c>
       <c r="S61" s="609"/>
-      <c r="T61" s="928" t="s">
+      <c r="T61" s="922" t="s">
         <v>384</v>
       </c>
       <c r="V61" s="709"/>
@@ -23290,8 +23293,8 @@
       <c r="AF61" s="665"/>
     </row>
     <row r="62" spans="1:32" s="601" customFormat="1">
-      <c r="A62" s="911"/>
-      <c r="B62" s="914"/>
+      <c r="A62" s="931"/>
+      <c r="B62" s="934"/>
       <c r="C62" s="719" t="s">
         <v>385</v>
       </c>
@@ -23312,7 +23315,7 @@
         <v>385</v>
       </c>
       <c r="S62" s="609"/>
-      <c r="T62" s="929"/>
+      <c r="T62" s="923"/>
       <c r="V62" s="709"/>
       <c r="X62" s="612" t="s">
         <v>610</v>
@@ -23325,8 +23328,8 @@
       <c r="AF62" s="665"/>
     </row>
     <row r="63" spans="1:32" s="601" customFormat="1">
-      <c r="A63" s="911"/>
-      <c r="B63" s="914"/>
+      <c r="A63" s="931"/>
+      <c r="B63" s="934"/>
       <c r="C63" s="719" t="s">
         <v>574</v>
       </c>
@@ -23347,7 +23350,7 @@
         <v>574</v>
       </c>
       <c r="S63" s="609"/>
-      <c r="T63" s="929"/>
+      <c r="T63" s="923"/>
       <c r="V63" s="709"/>
       <c r="X63" s="612" t="s">
         <v>610</v>
@@ -23360,8 +23363,8 @@
       <c r="AF63" s="665"/>
     </row>
     <row r="64" spans="1:32" s="601" customFormat="1">
-      <c r="A64" s="911"/>
-      <c r="B64" s="914"/>
+      <c r="A64" s="931"/>
+      <c r="B64" s="934"/>
       <c r="C64" s="815" t="s">
         <v>575</v>
       </c>
@@ -23382,7 +23385,7 @@
         <v>575</v>
       </c>
       <c r="S64" s="609"/>
-      <c r="T64" s="929"/>
+      <c r="T64" s="923"/>
       <c r="V64" s="817"/>
       <c r="X64" s="612" t="s">
         <v>610</v>
@@ -23395,8 +23398,8 @@
       <c r="AF64" s="665"/>
     </row>
     <row r="65" spans="1:32" s="601" customFormat="1">
-      <c r="A65" s="911"/>
-      <c r="B65" s="914"/>
+      <c r="A65" s="931"/>
+      <c r="B65" s="934"/>
       <c r="C65" s="719" t="s">
         <v>386</v>
       </c>
@@ -23417,7 +23420,7 @@
         <v>386</v>
       </c>
       <c r="S65" s="609"/>
-      <c r="T65" s="929"/>
+      <c r="T65" s="923"/>
       <c r="V65" s="820"/>
       <c r="X65" s="612" t="s">
         <v>610</v>
@@ -23430,8 +23433,8 @@
       <c r="AF65" s="665"/>
     </row>
     <row r="66" spans="1:32" s="601" customFormat="1">
-      <c r="A66" s="911"/>
-      <c r="B66" s="914"/>
+      <c r="A66" s="931"/>
+      <c r="B66" s="934"/>
       <c r="C66" s="719" t="s">
         <v>499</v>
       </c>
@@ -23452,7 +23455,7 @@
         <v>499</v>
       </c>
       <c r="S66" s="609"/>
-      <c r="T66" s="929"/>
+      <c r="T66" s="923"/>
       <c r="V66" s="820"/>
       <c r="X66" s="612" t="s">
         <v>610</v>
@@ -23465,8 +23468,8 @@
       <c r="AF66" s="665"/>
     </row>
     <row r="67" spans="1:32" s="601" customFormat="1">
-      <c r="A67" s="911"/>
-      <c r="B67" s="914"/>
+      <c r="A67" s="931"/>
+      <c r="B67" s="934"/>
       <c r="C67" s="719" t="s">
         <v>387</v>
       </c>
@@ -23487,7 +23490,7 @@
         <v>387</v>
       </c>
       <c r="S67" s="609"/>
-      <c r="T67" s="929"/>
+      <c r="T67" s="923"/>
       <c r="V67" s="820"/>
       <c r="X67" s="612" t="s">
         <v>610</v>
@@ -23500,8 +23503,8 @@
       <c r="AF67" s="665"/>
     </row>
     <row r="68" spans="1:32" s="601" customFormat="1">
-      <c r="A68" s="911"/>
-      <c r="B68" s="914"/>
+      <c r="A68" s="931"/>
+      <c r="B68" s="934"/>
       <c r="C68" s="719" t="s">
         <v>388</v>
       </c>
@@ -23522,7 +23525,7 @@
         <v>388</v>
       </c>
       <c r="S68" s="609"/>
-      <c r="T68" s="929"/>
+      <c r="T68" s="923"/>
       <c r="V68" s="820"/>
       <c r="X68" s="612" t="s">
         <v>610</v>
@@ -23535,8 +23538,8 @@
       <c r="AF68" s="665"/>
     </row>
     <row r="69" spans="1:32" s="601" customFormat="1" ht="45" customHeight="1">
-      <c r="A69" s="911"/>
-      <c r="B69" s="914"/>
+      <c r="A69" s="931"/>
+      <c r="B69" s="934"/>
       <c r="C69" s="719" t="s">
         <v>389</v>
       </c>
@@ -23557,7 +23560,7 @@
         <v>390</v>
       </c>
       <c r="S69" s="609"/>
-      <c r="T69" s="929"/>
+      <c r="T69" s="923"/>
       <c r="V69" s="820"/>
       <c r="X69" s="612" t="s">
         <v>610</v>
@@ -23570,8 +23573,8 @@
       <c r="AF69" s="665"/>
     </row>
     <row r="70" spans="1:32" s="601" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A70" s="911"/>
-      <c r="B70" s="914"/>
+      <c r="A70" s="931"/>
+      <c r="B70" s="934"/>
       <c r="C70" s="719" t="s">
         <v>391</v>
       </c>
@@ -23592,7 +23595,7 @@
         <v>391</v>
       </c>
       <c r="S70" s="609"/>
-      <c r="T70" s="929"/>
+      <c r="T70" s="923"/>
       <c r="V70" s="820"/>
       <c r="X70" s="612" t="s">
         <v>610</v>
@@ -23605,8 +23608,8 @@
       <c r="AF70" s="665"/>
     </row>
     <row r="71" spans="1:32" s="601" customFormat="1">
-      <c r="A71" s="911"/>
-      <c r="B71" s="914"/>
+      <c r="A71" s="931"/>
+      <c r="B71" s="934"/>
       <c r="C71" s="719" t="s">
         <v>576</v>
       </c>
@@ -23627,7 +23630,7 @@
         <v>576</v>
       </c>
       <c r="S71" s="609"/>
-      <c r="T71" s="929"/>
+      <c r="T71" s="923"/>
       <c r="V71" s="709"/>
       <c r="X71" s="612" t="s">
         <v>610</v>
@@ -23640,8 +23643,8 @@
       <c r="AF71" s="665"/>
     </row>
     <row r="72" spans="1:32" s="601" customFormat="1">
-      <c r="A72" s="911"/>
-      <c r="B72" s="914"/>
+      <c r="A72" s="931"/>
+      <c r="B72" s="934"/>
       <c r="C72" s="719" t="s">
         <v>577</v>
       </c>
@@ -23662,7 +23665,7 @@
         <v>577</v>
       </c>
       <c r="S72" s="609"/>
-      <c r="T72" s="929"/>
+      <c r="T72" s="923"/>
       <c r="V72" s="709"/>
       <c r="X72" s="612" t="s">
         <v>610</v>
@@ -23675,8 +23678,8 @@
       <c r="AF72" s="665"/>
     </row>
     <row r="73" spans="1:32" s="601" customFormat="1">
-      <c r="A73" s="911"/>
-      <c r="B73" s="914"/>
+      <c r="A73" s="931"/>
+      <c r="B73" s="934"/>
       <c r="C73" s="719" t="s">
         <v>392</v>
       </c>
@@ -23697,7 +23700,7 @@
         <v>392</v>
       </c>
       <c r="S73" s="609"/>
-      <c r="T73" s="929"/>
+      <c r="T73" s="923"/>
       <c r="V73" s="709"/>
       <c r="X73" s="612" t="s">
         <v>610</v>
@@ -23710,8 +23713,8 @@
       <c r="AF73" s="665"/>
     </row>
     <row r="74" spans="1:32" s="601" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A74" s="911"/>
-      <c r="B74" s="914"/>
+      <c r="A74" s="931"/>
+      <c r="B74" s="934"/>
       <c r="C74" s="719" t="s">
         <v>545</v>
       </c>
@@ -23732,7 +23735,7 @@
         <v>545</v>
       </c>
       <c r="S74" s="609"/>
-      <c r="T74" s="929"/>
+      <c r="T74" s="923"/>
       <c r="V74" s="709"/>
       <c r="X74" s="612" t="s">
         <v>610</v>
@@ -23746,8 +23749,8 @@
       <c r="AF74" s="665"/>
     </row>
     <row r="75" spans="1:32" s="601" customFormat="1" ht="22.8">
-      <c r="A75" s="911"/>
-      <c r="B75" s="914"/>
+      <c r="A75" s="931"/>
+      <c r="B75" s="934"/>
       <c r="C75" s="719" t="s">
         <v>809</v>
       </c>
@@ -23780,7 +23783,7 @@
         <v>809</v>
       </c>
       <c r="S75" s="609"/>
-      <c r="T75" s="930"/>
+      <c r="T75" s="924"/>
       <c r="V75" s="709"/>
       <c r="X75" s="612" t="s">
         <v>610</v>
@@ -23793,8 +23796,8 @@
       <c r="AF75" s="665"/>
     </row>
     <row r="76" spans="1:32" s="601" customFormat="1" ht="61.5" customHeight="1">
-      <c r="A76" s="911"/>
-      <c r="B76" s="914"/>
+      <c r="A76" s="931"/>
+      <c r="B76" s="934"/>
       <c r="C76" s="719" t="s">
         <v>810</v>
       </c>
@@ -23842,8 +23845,8 @@
       <c r="AF76" s="665"/>
     </row>
     <row r="77" spans="1:32" s="601" customFormat="1" ht="150" customHeight="1">
-      <c r="A77" s="911"/>
-      <c r="B77" s="914"/>
+      <c r="A77" s="931"/>
+      <c r="B77" s="934"/>
       <c r="C77" s="719" t="s">
         <v>865</v>
       </c>
@@ -23893,8 +23896,8 @@
       <c r="AF77" s="665"/>
     </row>
     <row r="78" spans="1:32" s="601" customFormat="1" ht="121.5" customHeight="1">
-      <c r="A78" s="912"/>
-      <c r="B78" s="915"/>
+      <c r="A78" s="932"/>
+      <c r="B78" s="935"/>
       <c r="C78" s="719" t="s">
         <v>1013</v>
       </c>
@@ -23928,10 +23931,10 @@
       <c r="AF78" s="665"/>
     </row>
     <row r="79" spans="1:32" s="601" customFormat="1" ht="60" customHeight="1">
-      <c r="A79" s="907" t="s">
+      <c r="A79" s="927" t="s">
         <v>227</v>
       </c>
-      <c r="B79" s="909" t="s">
+      <c r="B79" s="929" t="s">
         <v>211</v>
       </c>
       <c r="C79" s="827" t="s">
@@ -23980,8 +23983,8 @@
       <c r="AF79" s="665"/>
     </row>
     <row r="80" spans="1:32" s="601" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A80" s="908"/>
-      <c r="B80" s="909"/>
+      <c r="A80" s="928"/>
+      <c r="B80" s="929"/>
       <c r="C80" s="827" t="s">
         <v>596</v>
       </c>
@@ -24028,8 +24031,8 @@
       <c r="AF80" s="665"/>
     </row>
     <row r="81" spans="1:32" s="601" customFormat="1" ht="126" customHeight="1">
-      <c r="A81" s="908"/>
-      <c r="B81" s="909"/>
+      <c r="A81" s="928"/>
+      <c r="B81" s="929"/>
       <c r="C81" s="827" t="s">
         <v>828</v>
       </c>
@@ -24075,8 +24078,8 @@
       <c r="AF81" s="665"/>
     </row>
     <row r="82" spans="1:32" s="601" customFormat="1" ht="69" customHeight="1">
-      <c r="A82" s="908"/>
-      <c r="B82" s="909"/>
+      <c r="A82" s="928"/>
+      <c r="B82" s="929"/>
       <c r="C82" s="827" t="s">
         <v>579</v>
       </c>
@@ -24122,8 +24125,8 @@
       <c r="AF82" s="665"/>
     </row>
     <row r="83" spans="1:32" s="601" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A83" s="908"/>
-      <c r="B83" s="909"/>
+      <c r="A83" s="928"/>
+      <c r="B83" s="929"/>
       <c r="C83" s="719" t="s">
         <v>393</v>
       </c>
@@ -24169,8 +24172,8 @@
       <c r="AF83" s="665"/>
     </row>
     <row r="84" spans="1:32" s="601" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A84" s="908"/>
-      <c r="B84" s="909"/>
+      <c r="A84" s="928"/>
+      <c r="B84" s="929"/>
       <c r="C84" s="719" t="s">
         <v>662</v>
       </c>
@@ -24218,8 +24221,8 @@
       <c r="AF84" s="665"/>
     </row>
     <row r="85" spans="1:32" s="601" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A85" s="908"/>
-      <c r="B85" s="909"/>
+      <c r="A85" s="928"/>
+      <c r="B85" s="929"/>
       <c r="C85" s="827" t="s">
         <v>395</v>
       </c>
@@ -25165,6 +25168,27 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="A79:A85"/>
+    <mergeCell ref="B79:B85"/>
+    <mergeCell ref="A59:A78"/>
+    <mergeCell ref="B59:B78"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="T24:T26"/>
+    <mergeCell ref="T61:T75"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="E27:E29"/>
     <mergeCell ref="AD1:AD2"/>
     <mergeCell ref="AF1:AF2"/>
     <mergeCell ref="A7:A8"/>
@@ -25181,27 +25205,6 @@
     <mergeCell ref="G1:L1"/>
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="N1:N2"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="T24:T26"/>
-    <mergeCell ref="T61:T75"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="A79:A85"/>
-    <mergeCell ref="B79:B85"/>
-    <mergeCell ref="A59:A78"/>
-    <mergeCell ref="B59:B78"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="X1:X2"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7 G89:M93 E86:E88 R83:R84 C33:M39 C12:D24 C40:C41 G31:M32 E24 R62:R78 E12:E20 F12:F24 R33:R38 G44:M49 E47 C83:C84 C59:F78 G79:M85 G27:M27 C7:F11 G59:M61 D40:M43 C31:F31 A59:A61" xr:uid="{00000000-0002-0000-0500-000000000000}">
@@ -25231,10 +25234,10 @@
   </sheetPr>
   <dimension ref="A1:AG60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="P1" sqref="P1:P1048576"/>
-      <selection pane="bottomLeft" activeCell="P6" sqref="P6"/>
+      <selection pane="bottomLeft" activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -28100,6 +28103,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="V1:V2"/>
     <mergeCell ref="AE1:AE2"/>
     <mergeCell ref="AG1:AG2"/>
     <mergeCell ref="A5:C5"/>
@@ -28107,13 +28117,6 @@
     <mergeCell ref="AB1:AB2"/>
     <mergeCell ref="Z1:Z2"/>
     <mergeCell ref="G1:L1"/>
-    <mergeCell ref="E40:E43"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="V1:V2"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G15:M15 G40:M44 G30:M37 E38:E39 G56:K60" xr:uid="{00000000-0002-0000-0600-000000000000}">
@@ -29121,10 +29124,10 @@
   </sheetPr>
   <dimension ref="A1:AF61"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z14" sqref="Z14"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="X15" sqref="X15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -29716,7 +29719,7 @@
       <c r="Y13" s="260"/>
       <c r="Z13" s="383">
         <f>IF(OR(X13="A",X14="A"),"",IF(OR(X13="N",X14="N"),0,1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA13" s="476"/>
       <c r="AB13" s="485" t="s">
@@ -29753,7 +29756,7 @@
       </c>
       <c r="V14" s="346"/>
       <c r="X14" s="378" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="Y14" s="260"/>
       <c r="Z14" s="384"/>

</xml_diff>